<commit_message>
update homePage objects  and connection class
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2689" uniqueCount="409">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1212,49 +1212,40 @@
     <t xml:space="preserve">Android_002</t>
   </si>
   <si>
-    <t xml:space="preserve">10.0.0</t>
+    <t xml:space="preserve">Android_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_0003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ios_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneXSMax_iOS_13.3.0_9049f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/bitbar/test-samples/raw/master/apps/ios/bitbar-ios-sample.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.bitbar.testdroid.BitbarIOSSample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_0003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ios_01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.3.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneXSMax_iOS_13.3.0_9049f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/bitbar/test-samples/raw/master/apps/ios/bitbar-ios-sample.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.bitbar.testdroid.BitbarIOSSample</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.iexceed.assistedonboardingapp.automation</t>
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
@@ -1458,7 +1449,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1599,10 +1590,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1689,7 +1676,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="A1" activeCellId="1" sqref="H6:I6 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20513,11 +20500,11 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H6" activeCellId="0" sqref="H6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20755,10 +20742,10 @@
         <v>377</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>392</v>
@@ -20786,7 +20773,7 @@
     </row>
     <row r="6" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>44</v>
@@ -20807,10 +20794,10 @@
         <v>377</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>399</v>
+        <v>390</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>391</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>392</v>
@@ -20838,7 +20825,7 @@
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>44</v>
@@ -20862,7 +20849,7 @@
         <v>390</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>392</v>
@@ -20890,7 +20877,7 @@
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>44</v>
@@ -20899,7 +20886,7 @@
         <v>386</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>388</v>
@@ -20911,21 +20898,21 @@
         <v>377</v>
       </c>
       <c r="H8" s="33" t="s">
+        <v>401</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="J8" s="30" t="s">
+        <v>403</v>
+      </c>
+      <c r="K8" s="30" t="s">
         <v>404</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="J8" s="30" t="s">
-        <v>406</v>
-      </c>
-      <c r="K8" s="30" t="s">
-        <v>407</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="8"/>
       <c r="N8" s="34" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="O8" s="1" t="n">
         <v>500</v>
@@ -20938,33 +20925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="32"/>
-    </row>
-    <row r="10" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L10" s="35" t="s">
-        <v>409</v>
-      </c>
-      <c r="M10" s="35" t="s">
-        <v>410</v>
-      </c>
-    </row>
+    <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -21002,7 +20963,7 @@
   <dimension ref="B4:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="1" sqref="H6:I6 E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21012,37 +20973,37 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="36" t="s">
-        <v>401</v>
+      <c r="B5" s="35" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="36" t="s">
-        <v>397</v>
+      <c r="B6" s="35" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="36" t="s">
-        <v>401</v>
+      <c r="B7" s="35" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="36" t="s">
-        <v>411</v>
+      <c r="B8" s="35" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="35" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="36" t="s">
-        <v>411</v>
+      <c r="B11" s="35" t="s">
+        <v>408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made changes in legalUserDetail feature file
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2689" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2689" uniqueCount="411">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1213,6 +1213,12 @@
   </si>
   <si>
     <t xml:space="preserve">Android_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
   </si>
   <si>
     <t xml:space="preserve">Android_0003</t>
@@ -1676,7 +1682,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A1" activeCellId="1" sqref="H6:I6 A1"/>
+      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20504,7 +20510,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H6" activeCellId="0" sqref="H6:I6"/>
+      <selection pane="bottomRight" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20771,7 +20777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
         <v>396</v>
       </c>
@@ -20794,10 +20800,10 @@
         <v>377</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="I6" s="30" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>392</v>
@@ -20825,7 +20831,7 @@
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>44</v>
@@ -20849,7 +20855,7 @@
         <v>390</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>392</v>
@@ -20877,7 +20883,7 @@
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>44</v>
@@ -20886,7 +20892,7 @@
         <v>386</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>388</v>
@@ -20898,21 +20904,21 @@
         <v>377</v>
       </c>
       <c r="H8" s="33" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="K8" s="30" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="8"/>
       <c r="N8" s="34" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="O8" s="1" t="n">
         <v>500</v>
@@ -20963,7 +20969,7 @@
   <dimension ref="B4:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="1" sqref="H6:I6 E8"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20973,27 +20979,27 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="35" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="35" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="35" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="35" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21003,7 +21009,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="35" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the connection class and page objects
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2689" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2690" uniqueCount="411">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1224,31 +1224,31 @@
     <t xml:space="preserve">Android_0003</t>
   </si>
   <si>
+    <t xml:space="preserve">Ios_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneXSMax_iOS_13.3.0_9049f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/bitbar/test-samples/raw/master/apps/ios/bitbar-ios-sample.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.bitbar.testdroid.BitbarIOSSample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ios_01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.3.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneXSMax_iOS_13.3.0_9049f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/bitbar/test-samples/raw/master/apps/ios/bitbar-ios-sample.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.bitbar.testdroid.BitbarIOSSample</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
@@ -1268,7 +1268,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1367,6 +1367,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF808080"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
@@ -1455,7 +1461,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1588,15 +1594,23 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20510,7 +20524,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20852,10 +20866,10 @@
         <v>377</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="I7" s="30" t="s">
-        <v>400</v>
+        <v>397</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>398</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>392</v>
@@ -20883,7 +20897,7 @@
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>44</v>
@@ -20891,8 +20905,8 @@
       <c r="C8" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="D8" s="33" t="s">
-        <v>402</v>
+      <c r="D8" s="34" t="s">
+        <v>401</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>388</v>
@@ -20903,22 +20917,22 @@
       <c r="G8" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="H8" s="34" t="s">
+        <v>402</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="30" t="s">
         <v>404</v>
       </c>
-      <c r="J8" s="30" t="s">
+      <c r="K8" s="30" t="s">
         <v>405</v>
-      </c>
-      <c r="K8" s="30" t="s">
-        <v>406</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="8"/>
-      <c r="N8" s="34" t="s">
-        <v>407</v>
+      <c r="N8" s="35" t="s">
+        <v>406</v>
       </c>
       <c r="O8" s="1" t="n">
         <v>500</v>
@@ -20966,10 +20980,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4:B11"/>
+  <dimension ref="B4:B13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20979,37 +20993,42 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="36" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="35" t="s">
-        <v>400</v>
-      </c>
-    </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="36" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="35" t="s">
-        <v>400</v>
+      <c r="B7" s="36" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="36" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="36" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="36" t="s">
         <v>410</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="37" t="s">
+        <v>398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made changes in propert file and connection class updated parameters as 7
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2690" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2689" uniqueCount="410">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1203,7 +1203,7 @@
     <t xml:space="preserve">uiautomator2</t>
   </si>
   <si>
-    <t xml:space="preserve">app-debugOct11.apk</t>
+    <t xml:space="preserve">Automation-1-0-0-18-11-2021.apk</t>
   </si>
   <si>
     <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
@@ -1224,25 +1224,22 @@
     <t xml:space="preserve">Android_0003</t>
   </si>
   <si>
-    <t xml:space="preserve">Ios_01</t>
+    <t xml:space="preserve">IOS_001</t>
   </si>
   <si>
     <t xml:space="preserve">ios</t>
   </si>
   <si>
-    <t xml:space="preserve">13.3.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneXSMax_iOS_13.3.0_9049f</t>
+    <t xml:space="preserve">12.5.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPadMini2_iOS_12.5.1_a3ea4</t>
   </si>
   <si>
     <t xml:space="preserve">XCUITest</t>
   </si>
   <si>
-    <t xml:space="preserve">https://github.com/bitbar/test-samples/raw/master/apps/ios/bitbar-ios-sample.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.bitbar.testdroid.BitbarIOSSample</t>
+    <t xml:space="preserve">Automation-1-0-0-18-11-2021.ipa</t>
   </si>
   <si>
     <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
@@ -1366,10 +1363,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1461,7 +1458,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1594,11 +1591,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1607,10 +1604,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20524,7 +20517,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20687,7 +20680,7 @@
       </c>
       <c r="S3" s="28"/>
     </row>
-    <row r="4" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>385</v>
       </c>
@@ -20868,7 +20861,7 @@
       <c r="H7" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="I7" s="30" t="s">
         <v>398</v>
       </c>
       <c r="J7" s="8" t="s">
@@ -20905,7 +20898,7 @@
       <c r="C8" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="33" t="s">
         <v>401</v>
       </c>
       <c r="E8" s="29" t="s">
@@ -20931,9 +20924,7 @@
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="8"/>
-      <c r="N8" s="35" t="s">
-        <v>406</v>
-      </c>
+      <c r="N8" s="35"/>
       <c r="O8" s="1" t="n">
         <v>500</v>
       </c>
@@ -20962,8 +20953,7 @@
     <hyperlink ref="E7" r:id="rId9" display="sriganesh.d@i-exceed.com"/>
     <hyperlink ref="P7" r:id="rId10" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E8" r:id="rId11" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="K8" r:id="rId12" display="https://github.com/bitbar/test-samples/raw/master/apps/ios/bitbar-ios-sample.ipa"/>
-    <hyperlink ref="P8" r:id="rId13" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="P8" r:id="rId12" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -20993,27 +20983,27 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="36" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="36" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="36" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="36" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21023,11 +21013,11 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="36" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="36" t="s">
         <v>398</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating dynamic ios app launch using URL
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -1230,16 +1230,16 @@
     <t xml:space="preserve">ios</t>
   </si>
   <si>
-    <t xml:space="preserve">12.5.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPadMini2_iOS_12.5.1_a3ea4</t>
+    <t xml:space="preserve">13.5.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhone7plus_iOS_13.5.1_b1cc7</t>
   </si>
   <si>
     <t xml:space="preserve">XCUITest</t>
   </si>
   <si>
-    <t xml:space="preserve">Automation-1-0-0-18-11-2021.ipa</t>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37.ipa</t>
   </si>
   <si>
     <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
@@ -1265,7 +1265,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1363,12 +1363,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF808080"/>
       <name val="JetBrains Mono"/>
@@ -1458,7 +1452,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1596,10 +1590,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20517,7 +20507,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20910,21 +20900,21 @@
       <c r="G8" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="H8" s="34" t="s">
+      <c r="H8" s="33" t="s">
         <v>402</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="11" t="s">
         <v>403</v>
       </c>
       <c r="J8" s="30" t="s">
         <v>404</v>
       </c>
-      <c r="K8" s="30" t="s">
+      <c r="K8" s="11" t="s">
         <v>405</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="8"/>
-      <c r="N8" s="35"/>
+      <c r="N8" s="34"/>
       <c r="O8" s="1" t="n">
         <v>500</v>
       </c>
@@ -20987,37 +20977,37 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="35" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="35" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="35" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="35" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="35" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="35" t="s">
         <v>398</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating Android and ios url access connection class and methods
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2689" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2690" uniqueCount="411">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1194,64 +1194,67 @@
     <t xml:space="preserve">bkx8w6zydrxh6kj7xxw5t4kr</t>
   </si>
   <si>
+    <t xml:space="preserve">11.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uiautomator2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation-1-0-0-24-11-2021.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_002</t>
+  </si>
+  <si>
     <t xml:space="preserve">9.0.0</t>
   </si>
   <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_0003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.5.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhone7plus_iOS_13.5.1_b1cc7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uiautomator2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automation-1-0-0-18-11-2021.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.0.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_0003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.5.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhone7plus_iOS_13.5.1_b1cc7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1268,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1353,13 +1356,6 @@
       <color rgb="FF6A8759"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono:case"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1452,7 +1448,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1577,10 +1573,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1589,7 +1581,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20503,11 +20495,11 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20701,7 +20693,7 @@
       <c r="J4" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="K4" s="31" t="s">
+      <c r="K4" s="8" t="s">
         <v>393</v>
       </c>
       <c r="L4" s="24" t="s">
@@ -20712,12 +20704,12 @@
       </c>
       <c r="N4" s="8"/>
       <c r="O4" s="19" t="n">
-        <v>104</v>
+        <v>306</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="Q4" s="32" t="n">
+      <c r="Q4" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20745,15 +20737,15 @@
         <v>377</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="K5" s="31" t="s">
+      <c r="K5" s="8" t="s">
         <v>393</v>
       </c>
       <c r="L5" s="24" t="s">
@@ -20769,14 +20761,14 @@
       <c r="P5" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="Q5" s="32" t="n">
+      <c r="Q5" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>44</v>
@@ -20797,15 +20789,15 @@
         <v>377</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="I6" s="30" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="K6" s="31" t="s">
+      <c r="K6" s="8" t="s">
         <v>393</v>
       </c>
       <c r="L6" s="24" t="s">
@@ -20821,7 +20813,7 @@
       <c r="P6" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="Q6" s="32" t="n">
+      <c r="Q6" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20849,15 +20841,15 @@
         <v>377</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="K7" s="31" t="s">
+      <c r="K7" s="8" t="s">
         <v>393</v>
       </c>
       <c r="L7" s="24" t="s">
@@ -20873,7 +20865,7 @@
       <c r="P7" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="Q7" s="32" t="n">
+      <c r="Q7" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20888,7 +20880,7 @@
       <c r="C8" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="32" t="s">
         <v>401</v>
       </c>
       <c r="E8" s="29" t="s">
@@ -20900,7 +20892,7 @@
       <c r="G8" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="H8" s="32" t="s">
         <v>402</v>
       </c>
       <c r="I8" s="11" t="s">
@@ -20914,14 +20906,14 @@
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="8"/>
-      <c r="N8" s="34"/>
+      <c r="N8" s="33"/>
       <c r="O8" s="1" t="n">
         <v>500</v>
       </c>
       <c r="P8" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="Q8" s="32" t="n">
+      <c r="Q8" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20963,7 +20955,7 @@
   <dimension ref="B4:B13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20977,38 +20969,43 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="34" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="34" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="34" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="34" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="34" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="34" t="s">
         <v>391</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="35" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="35" t="s">
-        <v>398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made changes in test runner
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="416">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1194,79 +1194,82 @@
     <t xml:space="preserve">bkx8w6zydrxh6kj7xxw5t4kr</t>
   </si>
   <si>
+    <t xml:space="preserve">9.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uiautomator2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation-1-0-0-24-11-2021.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_003</t>
+  </si>
+  <si>
     <t xml:space="preserve">11.0.0</t>
   </si>
   <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_0003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneX_iOS_13.3.1_90703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
   </si>
   <si>
-    <t xml:space="preserve">uiautomator2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automation-1-0-0-24-11-2021.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.0.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_0003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ios</t>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhone7_iOS_13.1.3_316f0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
   </si>
   <si>
     <t xml:space="preserve">13.5.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhone7_iOS_13.1.3_316f0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneX_iOS_13.3.1_90703</t>
   </si>
 </sst>
 </file>
@@ -1280,7 +1283,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1369,6 +1372,12 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1466,7 +1475,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1587,7 +1596,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1595,15 +1604,19 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20521,11 +20534,11 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20763,10 +20776,10 @@
         <v>377</v>
       </c>
       <c r="H5" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="I5" s="32" t="s">
         <v>396</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>397</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>392</v>
@@ -20794,7 +20807,7 @@
     </row>
     <row r="6" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>44</v>
@@ -20815,9 +20828,9 @@
         <v>377</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="I6" s="30" t="s">
+        <v>398</v>
+      </c>
+      <c r="I6" s="32" t="s">
         <v>399</v>
       </c>
       <c r="J6" s="8" t="s">
@@ -20867,9 +20880,9 @@
         <v>377</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="I7" s="30" t="s">
+        <v>398</v>
+      </c>
+      <c r="I7" s="32" t="s">
         <v>399</v>
       </c>
       <c r="J7" s="8" t="s">
@@ -20906,7 +20919,7 @@
       <c r="C8" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="33" t="s">
         <v>402</v>
       </c>
       <c r="E8" s="29" t="s">
@@ -20918,13 +20931,13 @@
       <c r="G8" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="33" t="s">
         <v>403</v>
       </c>
-      <c r="I8" s="33" t="s">
+      <c r="I8" s="34" t="s">
         <v>404</v>
       </c>
-      <c r="J8" s="30" t="s">
+      <c r="J8" s="32" t="s">
         <v>405</v>
       </c>
       <c r="K8" s="11" t="s">
@@ -20932,7 +20945,7 @@
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="8"/>
-      <c r="N8" s="34"/>
+      <c r="N8" s="35"/>
       <c r="O8" s="1" t="n">
         <v>500</v>
       </c>
@@ -20981,7 +20994,7 @@
   <dimension ref="B4:F20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20995,42 +21008,42 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="36" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="36" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="36" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="36" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="36" t="s">
         <v>391</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="35" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="35" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="35" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="35" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="35" t="s">
-        <v>409</v>
+      <c r="B11" s="36" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="36" t="s">
         <v>399</v>
       </c>
     </row>
@@ -21048,16 +21061,16 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="36" t="s">
-        <v>404</v>
-      </c>
-      <c r="F19" s="36" t="s">
-        <v>403</v>
+      <c r="B19" s="37" t="s">
+        <v>414</v>
+      </c>
+      <c r="F19" s="37" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating gesture and search field feature in sanity and UserCOntact
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -1227,43 +1227,43 @@
     <t xml:space="preserve">Android_002</t>
   </si>
   <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.iexceed.assistedonboardingapp.qa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_0003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation-1-0-0-24-11-2021.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneX_iOS_13.3.1_90703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.iexceed.assistedonboardingapp.qa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automation-1-0-0-24-11-2021.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_0003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.3.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneX_iOS_13.3.1_90703</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
@@ -20610,11 +20610,11 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20881,7 +20881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
         <v>403</v>
       </c>
@@ -20906,20 +20906,20 @@
       <c r="H6" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="I6" s="34" t="s">
-        <v>404</v>
+      <c r="I6" s="30" t="s">
+        <v>395</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>396</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="L6" s="24" t="s">
-        <v>384</v>
+      <c r="K6" s="31" t="s">
+        <v>397</v>
+      </c>
+      <c r="L6" s="32" t="s">
+        <v>398</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>385</v>
+        <v>402</v>
       </c>
       <c r="N6" s="8"/>
       <c r="O6" s="19" t="n">
@@ -20935,7 +20935,7 @@
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>44</v>
@@ -20959,7 +20959,7 @@
         <v>394</v>
       </c>
       <c r="I7" s="34" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>396</v>
@@ -20987,7 +20987,7 @@
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>44</v>
@@ -20996,7 +20996,7 @@
         <v>390</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>392</v>
@@ -21008,16 +21008,16 @@
         <v>381</v>
       </c>
       <c r="H8" s="35" t="s">
+        <v>408</v>
+      </c>
+      <c r="I8" s="36" t="s">
         <v>409</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="J8" s="34" t="s">
         <v>410</v>
       </c>
-      <c r="J8" s="34" t="s">
+      <c r="K8" s="11" t="s">
         <v>411</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>412</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="8"/>
@@ -21070,7 +21070,7 @@
   <dimension ref="B4:F24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21080,12 +21080,12 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="38" t="s">
-        <v>401</v>
+        <v>413</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21095,7 +21095,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="38" t="s">
-        <v>401</v>
+        <v>413</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21120,7 +21120,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="38" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21158,7 +21158,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updating project according to Appurl upgrade jenkins project
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="425">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1209,7 +1209,7 @@
     <t xml:space="preserve">11.0.0</t>
   </si>
   <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM12_Android_11.0.0_df6a7</t>
+    <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
   </si>
   <si>
     <t xml:space="preserve">uiautomator2</t>
@@ -1236,6 +1236,9 @@
     <t xml:space="preserve">Android_003</t>
   </si>
   <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Android_0003</t>
   </si>
   <si>
@@ -1263,9 +1266,6 @@
     <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
   </si>
   <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
-  </si>
-  <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
   </si>
   <si>
@@ -1276,9 +1276,6 @@
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyM01_Android_11.0.0_7425f</t>
@@ -1404,10 +1401,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1416,10 +1413,10 @@
       <family val="3"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="12"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1648,16 +1645,16 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -20614,7 +20611,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20777,7 +20774,7 @@
       </c>
       <c r="S3" s="28"/>
     </row>
-    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>389</v>
       </c>
@@ -20854,7 +20851,7 @@
       <c r="H5" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="I5" s="30" t="s">
+      <c r="I5" s="34" t="s">
         <v>401</v>
       </c>
       <c r="J5" s="8" t="s">
@@ -20906,8 +20903,8 @@
       <c r="H6" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="I6" s="30" t="s">
-        <v>395</v>
+      <c r="I6" s="34" t="s">
+        <v>404</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>396</v>
@@ -20935,7 +20932,7 @@
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>44</v>
@@ -20958,14 +20955,14 @@
       <c r="H7" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="35" t="s">
         <v>401</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>396</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="L7" s="24" t="s">
         <v>384</v>
@@ -20987,7 +20984,7 @@
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>44</v>
@@ -20995,8 +20992,8 @@
       <c r="C8" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="D8" s="35" t="s">
-        <v>407</v>
+      <c r="D8" s="36" t="s">
+        <v>408</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>392</v>
@@ -21007,17 +21004,17 @@
       <c r="G8" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="H8" s="35" t="s">
-        <v>408</v>
-      </c>
-      <c r="I8" s="36" t="s">
+      <c r="H8" s="36" t="s">
         <v>409</v>
       </c>
-      <c r="J8" s="34" t="s">
+      <c r="I8" s="30" t="s">
         <v>410</v>
       </c>
+      <c r="J8" s="35" t="s">
+        <v>411</v>
+      </c>
       <c r="K8" s="11" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="8"/>
@@ -21070,7 +21067,7 @@
   <dimension ref="B4:F24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21080,12 +21077,12 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="38" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21095,7 +21092,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="38" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21125,45 +21122,45 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>418</v>
+        <v>395</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="F21" s="0" t="s">
         <v>421</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="39" t="s">
+        <v>422</v>
+      </c>
+      <c r="F22" s="39" t="s">
         <v>423</v>
-      </c>
-      <c r="F22" s="39" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made changes in pcloudy connetion class and home step definition
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2713" uniqueCount="427">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1137,6 +1137,9 @@
     <t xml:space="preserve">automationName</t>
   </si>
   <si>
+    <t xml:space="preserve">applicationURL</t>
+  </si>
+  <si>
     <t xml:space="preserve">applicationName</t>
   </si>
   <si>
@@ -1279,6 +1282,9 @@
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyM01_Android_11.0.0_7425f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM12_Android_11.0.0_df6a7</t>
   </si>
   <si>
     <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
@@ -1310,7 +1316,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1402,12 +1408,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF808080"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
@@ -1496,7 +1496,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1617,7 +1617,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1625,15 +1625,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20580,14 +20576,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="bottomRight" activeCell="K7" activeCellId="0" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20601,12 +20597,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="26.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="26.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="9.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20655,375 +20651,382 @@
       <c r="O1" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="P1" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="18" t="s">
         <v>377</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E2" s="21"/>
       <c r="F2" s="21"/>
       <c r="G2" s="20" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H2" s="20"/>
       <c r="I2" s="20" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>383</v>
-      </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="24" t="s">
         <v>384</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="K2" s="22"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="24" t="s">
         <v>385</v>
       </c>
-      <c r="N2" s="23"/>
-      <c r="O2" s="22" t="n">
+      <c r="N2" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="O2" s="23"/>
+      <c r="P2" s="22" t="n">
         <v>500</v>
       </c>
-      <c r="P2" s="25" t="s">
-        <v>386</v>
-      </c>
-      <c r="Q2" s="22" t="n">
+      <c r="Q2" s="25" t="s">
+        <v>387</v>
+      </c>
+      <c r="R2" s="22" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>44</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H3" s="26"/>
       <c r="I3" s="26" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K3" s="26"/>
-      <c r="L3" s="24" t="s">
-        <v>384</v>
-      </c>
-      <c r="M3" s="11" t="s">
+      <c r="L3" s="26"/>
+      <c r="M3" s="24" t="s">
         <v>385</v>
       </c>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19" t="n">
+      <c r="N3" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19" t="n">
         <v>103</v>
       </c>
-      <c r="P3" s="26" t="s">
-        <v>386</v>
-      </c>
-      <c r="Q3" s="27" t="n">
+      <c r="Q3" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="R3" s="27" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="S3" s="28"/>
-    </row>
-    <row r="4" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T3" s="28"/>
+    </row>
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="K4" s="11" t="s">
         <v>397</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="K4" s="8"/>
+      <c r="L4" s="11" t="s">
         <v>398</v>
       </c>
-      <c r="M4" s="11" t="s">
-        <v>385</v>
-      </c>
-      <c r="N4" s="8"/>
-      <c r="O4" s="19" t="n">
+      <c r="M4" s="24" t="s">
+        <v>399</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="O4" s="8"/>
+      <c r="P4" s="19" t="n">
         <v>306</v>
       </c>
-      <c r="P4" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="Q4" s="31" t="n">
+      <c r="Q4" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="R4" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>393</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>394</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>402</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="M5" s="24" t="s">
+        <v>399</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>403</v>
+      </c>
+      <c r="O5" s="8"/>
+      <c r="P5" s="19" t="n">
+        <v>105</v>
+      </c>
+      <c r="Q5" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>391</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>392</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>393</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="I5" s="32" t="s">
-        <v>401</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>397</v>
-      </c>
-      <c r="L5" s="24" t="s">
-        <v>398</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>402</v>
-      </c>
-      <c r="N5" s="8"/>
-      <c r="O5" s="19" t="n">
-        <v>105</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="Q5" s="31" t="n">
+      <c r="R5" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>393</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>394</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>396</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="M6" s="24" t="s">
+        <v>399</v>
+      </c>
+      <c r="N6" s="11" t="s">
         <v>403</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>391</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>392</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>393</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>395</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>397</v>
-      </c>
-      <c r="L6" s="24" t="s">
-        <v>398</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>402</v>
-      </c>
-      <c r="N6" s="8"/>
-      <c r="O6" s="19" t="n">
+      <c r="O6" s="8"/>
+      <c r="P6" s="19" t="n">
         <v>106</v>
       </c>
-      <c r="P6" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="Q6" s="31" t="n">
+      <c r="Q6" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="R6" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="I7" s="32" t="s">
-        <v>401</v>
+        <v>395</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>402</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="L7" s="24" t="s">
-        <v>384</v>
-      </c>
-      <c r="M7" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="M7" s="24" t="s">
         <v>385</v>
       </c>
-      <c r="N7" s="8"/>
-      <c r="O7" s="19" t="n">
+      <c r="N7" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="O7" s="8"/>
+      <c r="P7" s="19" t="n">
         <v>306</v>
       </c>
-      <c r="P7" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="Q7" s="31" t="n">
+      <c r="Q7" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="R7" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>407</v>
+        <v>391</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>408</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="H8" s="33" t="s">
-        <v>408</v>
+        <v>382</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>409</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>409</v>
-      </c>
-      <c r="J8" s="32" t="s">
         <v>410</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="J8" s="30" t="s">
         <v>411</v>
       </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="1" t="n">
+      <c r="K8" s="30"/>
+      <c r="L8" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="P8" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="Q8" s="31" t="n">
+      <c r="Q8" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="R8" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" display="http://127.0.0.1:4723/wd/hub"/>
-    <hyperlink ref="P3" r:id="rId2" display="http://127.0.0.1:4723/wd/hub"/>
+    <hyperlink ref="Q2" r:id="rId1" display="http://127.0.0.1:4723/wd/hub"/>
+    <hyperlink ref="Q3" r:id="rId2" display="http://127.0.0.1:4723/wd/hub"/>
     <hyperlink ref="E4" r:id="rId3" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="P4" r:id="rId4" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="Q4" r:id="rId4" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E5" r:id="rId5" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="P5" r:id="rId6" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="Q5" r:id="rId6" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E6" r:id="rId7" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="P6" r:id="rId8" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="Q6" r:id="rId8" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E7" r:id="rId9" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="P7" r:id="rId10" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="Q7" r:id="rId10" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E8" r:id="rId11" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="P8" r:id="rId12" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="Q8" r:id="rId12" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -21040,10 +21043,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4:F24"/>
+  <dimension ref="B4:F27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21053,90 +21056,97 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="35" t="s">
-        <v>395</v>
+      <c r="B5" s="34" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="35" t="s">
-        <v>413</v>
+      <c r="B6" s="34" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="35" t="s">
-        <v>395</v>
+      <c r="B7" s="34" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="35" t="s">
-        <v>414</v>
+      <c r="B8" s="34" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="35" t="s">
-        <v>415</v>
+      <c r="B9" s="34" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="35" t="s">
-        <v>414</v>
+      <c r="B11" s="34" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="35" t="s">
-        <v>401</v>
+      <c r="B13" s="34" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>420</v>
+      </c>
+    </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
-        <v>420</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="36" t="s">
-        <v>422</v>
-      </c>
-      <c r="F22" s="36" t="s">
-        <v>423</v>
-      </c>
-    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>409</v>
+        <v>421</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="35" t="s">
         <v>424</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="s">
+        <v>426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating testrunner and excel
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2713" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2715" uniqueCount="427">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1218,6 +1218,9 @@
     <t xml:space="preserve">uiautomator2</t>
   </si>
   <si>
+    <t xml:space="preserve">http://readuser:Re@d@1234@20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.5-06-12-2021-19:31.apk</t>
+  </si>
+  <si>
     <t xml:space="preserve">Automation-1-0-5-6-12-2021.apk</t>
   </si>
   <si>
@@ -1231,9 +1234,6 @@
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.iexceed.assistedonboardingapp.qa</t>
   </si>
   <si>
     <t xml:space="preserve">Android_003</t>
@@ -1316,7 +1316,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1408,6 +1408,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF808080"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
@@ -1496,7 +1502,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1625,11 +1631,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20579,11 +20589,11 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K7" activeCellId="0" sqref="K7"/>
+      <selection pane="bottomRight" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20751,7 +20761,7 @@
       </c>
       <c r="T3" s="28"/>
     </row>
-    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>390</v>
       </c>
@@ -20782,12 +20792,14 @@
       <c r="J4" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="K4" s="8"/>
+      <c r="K4" s="8" t="s">
+        <v>398</v>
+      </c>
       <c r="L4" s="11" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="M4" s="24" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="N4" s="11" t="s">
         <v>386</v>
@@ -20797,16 +20809,16 @@
         <v>306</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="R4" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>44</v>
@@ -20829,28 +20841,30 @@
       <c r="H5" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="I5" s="30" t="s">
-        <v>402</v>
+      <c r="I5" s="32" t="s">
+        <v>403</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="K5" s="8"/>
+      <c r="K5" s="8" t="s">
+        <v>398</v>
+      </c>
       <c r="L5" s="11" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="M5" s="24" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>403</v>
+        <v>386</v>
       </c>
       <c r="O5" s="8"/>
       <c r="P5" s="19" t="n">
-        <v>105</v>
+        <v>307</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="R5" s="31" t="n">
         <f aca="false">FALSE()</f>
@@ -20890,20 +20904,20 @@
       </c>
       <c r="K6" s="8"/>
       <c r="L6" s="11" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>403</v>
+        <v>386</v>
       </c>
       <c r="O6" s="8"/>
       <c r="P6" s="19" t="n">
         <v>106</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="R6" s="31" t="n">
         <f aca="false">FALSE()</f>
@@ -20936,7 +20950,7 @@
         <v>395</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>397</v>
@@ -20956,7 +20970,7 @@
         <v>306</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="R7" s="31" t="n">
         <f aca="false">FALSE()</f>
@@ -20973,7 +20987,7 @@
       <c r="C8" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="33" t="s">
         <v>408</v>
       </c>
       <c r="E8" s="29" t="s">
@@ -20985,7 +20999,7 @@
       <c r="G8" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="33" t="s">
         <v>409</v>
       </c>
       <c r="I8" s="8" t="s">
@@ -21000,12 +21014,12 @@
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="8"/>
-      <c r="O8" s="33"/>
+      <c r="O8" s="34"/>
       <c r="P8" s="1" t="n">
         <v>500</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="R8" s="31" t="n">
         <f aca="false">FALSE()</f>
@@ -21046,7 +21060,7 @@
   <dimension ref="B4:F27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21060,27 +21074,27 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="35" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="35" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="35" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="35" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="35" t="s">
         <v>416</v>
       </c>
     </row>
@@ -21090,13 +21104,13 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="35" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="34" t="s">
-        <v>402</v>
+      <c r="B13" s="35" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21132,10 +21146,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="36" t="s">
         <v>424</v>
       </c>
-      <c r="F25" s="35" t="s">
+      <c r="F25" s="36" t="s">
         <v>425</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating excel and pcloudy connection class
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2715" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2715" uniqueCount="428">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1233,13 +1233,16 @@
     <t xml:space="preserve">Android_002</t>
   </si>
   <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_0003</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_0003</t>
   </si>
   <si>
     <t xml:space="preserve">Automation-1-0-0-24-11-2021.apk</t>
@@ -1316,7 +1319,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1408,12 +1411,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF808080"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
@@ -1502,7 +1499,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1631,15 +1628,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1730,10 +1723,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ248"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B10" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="topRight" activeCell="A26" activeCellId="0" sqref="A26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20589,11 +20582,11 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20841,7 +20834,7 @@
       <c r="H5" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="I5" s="30" t="s">
         <v>403</v>
       </c>
       <c r="J5" s="8" t="s">
@@ -20950,14 +20943,14 @@
         <v>395</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>397</v>
       </c>
       <c r="K7" s="8"/>
       <c r="L7" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M7" s="24" t="s">
         <v>385</v>
@@ -20979,7 +20972,7 @@
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>44</v>
@@ -20987,8 +20980,8 @@
       <c r="C8" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="D8" s="33" t="s">
-        <v>408</v>
+      <c r="D8" s="32" t="s">
+        <v>409</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>393</v>
@@ -20999,22 +20992,22 @@
       <c r="G8" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="H8" s="33" t="s">
-        <v>409</v>
+      <c r="H8" s="32" t="s">
+        <v>410</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="K8" s="30"/>
       <c r="L8" s="11" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="8"/>
-      <c r="O8" s="34"/>
+      <c r="O8" s="33"/>
       <c r="P8" s="1" t="n">
         <v>500</v>
       </c>
@@ -21060,7 +21053,7 @@
   <dimension ref="B4:F27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21070,62 +21063,62 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="35" t="s">
-        <v>414</v>
+      <c r="B6" s="34" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="34" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="35" t="s">
-        <v>415</v>
+      <c r="B8" s="34" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="35" t="s">
-        <v>416</v>
+      <c r="B9" s="34" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="35" t="s">
-        <v>415</v>
+      <c r="B11" s="34" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="35" t="s">
-        <v>403</v>
+      <c r="B13" s="34" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -21134,33 +21127,33 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="36" t="s">
-        <v>424</v>
-      </c>
-      <c r="F25" s="36" t="s">
+      <c r="B25" s="35" t="s">
         <v>425</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating project with adding credentials to the trigger APPURL
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2715" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2715" uniqueCount="427">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1221,7 +1221,25 @@
     <t xml:space="preserve">http://readuser:Re@d@1234@20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.5-06-12-2021-19:31.apk</t>
   </si>
   <si>
-    <t xml:space="preserve">Automation-1-0-5-6-12-2021.apk</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF067D17"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">Automation-1-0-6-13-12-2021</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF067D17"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.apk</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
@@ -1245,67 +1263,64 @@
     <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
   </si>
   <si>
-    <t xml:space="preserve">Automation-1-0-0-24-11-2021.apk</t>
-  </si>
-  <si>
     <t xml:space="preserve">IOS_001</t>
   </si>
   <si>
     <t xml:space="preserve">ios</t>
   </si>
   <si>
-    <t xml:space="preserve">13.3.1</t>
+    <t xml:space="preserve">14.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneX_iOS_14.0.0_1b718</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM01_Android_11.0.0_7425f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM12_Android_11.0.0_df6a7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhone7_iOS_13.1.3_316f0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.5.1</t>
   </si>
   <si>
     <t xml:space="preserve">APPLE_iPhoneX_iOS_13.3.1_90703</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM01_Android_11.0.0_7425f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM12_Android_11.0.0_df6a7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhone7_iOS_13.1.3_316f0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.5.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneX_iOS_14.0.0_1b718</t>
   </si>
 </sst>
 </file>
@@ -1319,7 +1334,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1408,6 +1423,25 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF067D17"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF067D17"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1499,7 +1533,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1624,6 +1658,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1632,7 +1670,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20582,11 +20624,11 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20600,7 +20642,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="26.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="9.17"/>
@@ -20788,7 +20831,7 @@
       <c r="K4" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="31" t="s">
         <v>399</v>
       </c>
       <c r="M4" s="24" t="s">
@@ -20804,7 +20847,7 @@
       <c r="Q4" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="R4" s="31" t="n">
+      <c r="R4" s="32" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20843,7 +20886,7 @@
       <c r="K5" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="31" t="s">
         <v>399</v>
       </c>
       <c r="M5" s="24" t="s">
@@ -20859,7 +20902,7 @@
       <c r="Q5" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="R5" s="31" t="n">
+      <c r="R5" s="32" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20896,7 +20939,7 @@
         <v>397</v>
       </c>
       <c r="K6" s="8"/>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="31" t="s">
         <v>399</v>
       </c>
       <c r="M6" s="24" t="s">
@@ -20912,7 +20955,7 @@
       <c r="Q6" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="R6" s="31" t="n">
+      <c r="R6" s="32" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20949,8 +20992,8 @@
         <v>397</v>
       </c>
       <c r="K7" s="8"/>
-      <c r="L7" s="8" t="s">
-        <v>407</v>
+      <c r="L7" s="31" t="s">
+        <v>399</v>
       </c>
       <c r="M7" s="24" t="s">
         <v>385</v>
@@ -20965,14 +21008,14 @@
       <c r="Q7" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="R7" s="31" t="n">
+      <c r="R7" s="32" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>44</v>
@@ -20980,8 +21023,8 @@
       <c r="C8" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="D8" s="32" t="s">
-        <v>409</v>
+      <c r="D8" s="33" t="s">
+        <v>408</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>393</v>
@@ -20992,29 +21035,29 @@
       <c r="G8" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="33" t="s">
+        <v>409</v>
+      </c>
+      <c r="I8" s="34" t="s">
         <v>410</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="30" t="s">
         <v>411</v>
       </c>
-      <c r="J8" s="30" t="s">
+      <c r="K8" s="30" t="s">
         <v>412</v>
       </c>
-      <c r="K8" s="30"/>
-      <c r="L8" s="11" t="s">
-        <v>413</v>
-      </c>
+      <c r="L8" s="31"/>
       <c r="M8" s="1"/>
       <c r="N8" s="8"/>
-      <c r="O8" s="33"/>
+      <c r="O8" s="35"/>
       <c r="P8" s="1" t="n">
         <v>500</v>
       </c>
       <c r="Q8" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="R8" s="31" t="n">
+      <c r="R8" s="32" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21053,7 +21096,7 @@
   <dimension ref="B4:F27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21063,62 +21106,62 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="36" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="36" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="34" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="36" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="34" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="36" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="34" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="34" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="36" t="s">
         <v>416</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="34" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="34" t="s">
-        <v>416</v>
+      <c r="B11" s="36" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="36" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -21127,33 +21170,33 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>423</v>
       </c>
-      <c r="F24" s="0" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="37" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="35" t="s">
+      <c r="F25" s="37" t="s">
         <v>425</v>
-      </c>
-      <c r="F25" s="35" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>411</v>
+        <v>426</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>427</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating test runner 2 and excel
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2715" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2715" uniqueCount="426">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1212,7 +1212,7 @@
     <t xml:space="preserve">11.0.0</t>
   </si>
   <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
+    <t xml:space="preserve">SAMSUNG_GalaxyM12_Android_11.0.0_df6a7</t>
   </si>
   <si>
     <t xml:space="preserve">uiautomator2</t>
@@ -1257,6 +1257,9 @@
     <t xml:space="preserve">Android_003</t>
   </si>
   <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Android_0003</t>
   </si>
   <si>
@@ -1269,58 +1272,52 @@
     <t xml:space="preserve">ios</t>
   </si>
   <si>
-    <t xml:space="preserve">14.0.0</t>
+    <t xml:space="preserve">13.5.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM01_Android_11.0.0_7425f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhone7_iOS_13.1.3_316f0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneX_iOS_13.3.1_90703</t>
   </si>
   <si>
     <t xml:space="preserve">APPLE_iPhoneX_iOS_14.0.0_1b718</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM01_Android_11.0.0_7425f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM12_Android_11.0.0_df6a7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhone7_iOS_13.1.3_316f0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.5.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneX_iOS_13.3.1_90703</t>
   </si>
 </sst>
 </file>
@@ -1425,6 +1422,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF067D17"/>
       <name val="JetBrains Mono"/>
@@ -1436,12 +1439,6 @@
       <name val=""/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1654,11 +1651,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1666,12 +1663,12 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -20624,11 +20621,11 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20797,7 +20794,7 @@
       </c>
       <c r="T3" s="28"/>
     </row>
-    <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>390</v>
       </c>
@@ -20877,7 +20874,7 @@
       <c r="H5" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="I5" s="30" t="s">
+      <c r="I5" s="33" t="s">
         <v>403</v>
       </c>
       <c r="J5" s="8" t="s">
@@ -20932,8 +20929,8 @@
       <c r="H6" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="I6" s="30" t="s">
-        <v>396</v>
+      <c r="I6" s="33" t="s">
+        <v>405</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>397</v>
@@ -20962,7 +20959,7 @@
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>44</v>
@@ -20985,8 +20982,8 @@
       <c r="H7" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="I7" s="30" t="s">
-        <v>406</v>
+      <c r="I7" s="33" t="s">
+        <v>407</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>397</v>
@@ -21015,7 +21012,7 @@
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>44</v>
@@ -21023,8 +21020,8 @@
       <c r="C8" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="D8" s="33" t="s">
-        <v>408</v>
+      <c r="D8" s="34" t="s">
+        <v>409</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>393</v>
@@ -21035,17 +21032,17 @@
       <c r="G8" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="H8" s="33" t="s">
-        <v>409</v>
-      </c>
-      <c r="I8" s="34" t="s">
+      <c r="H8" s="34" t="s">
         <v>410</v>
       </c>
-      <c r="J8" s="30" t="s">
+      <c r="I8" s="30" t="s">
         <v>411</v>
       </c>
-      <c r="K8" s="30" t="s">
+      <c r="J8" s="33" t="s">
         <v>412</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>413</v>
       </c>
       <c r="L8" s="31"/>
       <c r="M8" s="1"/>
@@ -21096,7 +21093,7 @@
   <dimension ref="B4:F27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21106,62 +21103,62 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="36" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="36" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="36" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="36" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="36" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="36" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="36" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>420</v>
+        <v>396</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -21183,20 +21180,20 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="37" t="s">
-        <v>424</v>
+        <v>411</v>
       </c>
       <c r="F25" s="37" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>410</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating test runner class
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2728" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2728" uniqueCount="429">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1252,64 +1252,67 @@
     <t xml:space="preserve">Android_002</t>
   </si>
   <si>
+    <t xml:space="preserve">9.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_0003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.5.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneXS_iOS_14.1.0_21d51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM01_Android_11.0.0_7425f</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAMSUNG_GalaxyM12_Android_11.0.0_df6a7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_0003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.5.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.3.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneXS_iOS_14.1.0_21d51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM01_Android_11.0.0_7425f</t>
   </si>
   <si>
     <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
@@ -20626,11 +20629,11 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20799,7 +20802,7 @@
       </c>
       <c r="T3" s="29"/>
     </row>
-    <row r="4" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>390</v>
       </c>
@@ -20877,10 +20880,10 @@
         <v>382</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>395</v>
+        <v>403</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>397</v>
@@ -20911,7 +20914,7 @@
     </row>
     <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>44</v>
@@ -20935,7 +20938,7 @@
         <v>395</v>
       </c>
       <c r="I6" s="33" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>397</v>
@@ -20964,7 +20967,7 @@
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>44</v>
@@ -21017,7 +21020,7 @@
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>44</v>
@@ -21026,7 +21029,7 @@
         <v>391</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="E8" s="30" t="s">
         <v>393</v>
@@ -21038,16 +21041,16 @@
         <v>382</v>
       </c>
       <c r="H8" s="34" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="J8" s="33" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="K8" s="33" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="L8" s="11"/>
       <c r="M8" s="1"/>
@@ -21066,7 +21069,7 @@
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>44</v>
@@ -21075,7 +21078,7 @@
         <v>391</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="E9" s="30" t="s">
         <v>393</v>
@@ -21087,16 +21090,16 @@
         <v>382</v>
       </c>
       <c r="H9" s="34" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="I9" s="32" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="J9" s="33" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="K9" s="36" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="P9" s="1" t="n">
         <v>501</v>
@@ -21144,7 +21147,7 @@
   <dimension ref="B4:F28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21154,42 +21157,42 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="37" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="37" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="37" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="37" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="37" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="37" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21209,7 +21212,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>403</v>
+        <v>423</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -21218,38 +21221,38 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="38" t="s">
+        <v>411</v>
+      </c>
+      <c r="F25" s="38" t="s">
         <v>410</v>
-      </c>
-      <c r="F25" s="38" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating android and ios utility classes
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -1341,7 +1341,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1439,12 +1439,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF808080"/>
       <name val="JetBrains Mono"/>
@@ -1534,7 +1528,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1663,10 +1657,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1675,7 +1665,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20629,11 +20619,11 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20756,7 +20746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
         <v>388</v>
       </c>
@@ -20802,7 +20792,7 @@
       </c>
       <c r="T3" s="29"/>
     </row>
-    <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>390</v>
       </c>
@@ -20882,7 +20872,7 @@
       <c r="H5" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="I5" s="8" t="s">
         <v>404</v>
       </c>
       <c r="J5" s="8" t="s">
@@ -20937,7 +20927,7 @@
       <c r="H6" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="I6" s="33" t="s">
+      <c r="I6" s="32" t="s">
         <v>406</v>
       </c>
       <c r="J6" s="8" t="s">
@@ -20990,8 +20980,8 @@
       <c r="H7" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="I7" s="33" t="s">
-        <v>396</v>
+      <c r="I7" s="32" t="s">
+        <v>406</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>397</v>
@@ -21028,7 +21018,7 @@
       <c r="C8" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="33" t="s">
         <v>409</v>
       </c>
       <c r="E8" s="30" t="s">
@@ -21040,22 +21030,22 @@
       <c r="G8" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="H8" s="34" t="s">
+      <c r="H8" s="33" t="s">
         <v>410</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>411</v>
       </c>
-      <c r="J8" s="33" t="s">
+      <c r="J8" s="32" t="s">
         <v>412</v>
       </c>
-      <c r="K8" s="33" t="s">
+      <c r="K8" s="32" t="s">
         <v>413</v>
       </c>
       <c r="L8" s="11"/>
       <c r="M8" s="1"/>
       <c r="N8" s="8"/>
-      <c r="O8" s="35"/>
+      <c r="O8" s="34"/>
       <c r="P8" s="1" t="n">
         <v>500</v>
       </c>
@@ -21086,19 +21076,19 @@
       <c r="F9" s="30" t="s">
         <v>394</v>
       </c>
-      <c r="G9" s="34" t="s">
+      <c r="G9" s="33" t="s">
         <v>382</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="33" t="s">
         <v>415</v>
       </c>
-      <c r="I9" s="32" t="s">
+      <c r="I9" s="8" t="s">
         <v>416</v>
       </c>
-      <c r="J9" s="33" t="s">
+      <c r="J9" s="32" t="s">
         <v>412</v>
       </c>
-      <c r="K9" s="36" t="s">
+      <c r="K9" s="35" t="s">
         <v>413</v>
       </c>
       <c r="P9" s="1" t="n">
@@ -21147,7 +21137,7 @@
   <dimension ref="B4:F28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21161,27 +21151,27 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="36" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="36" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="36" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="36" t="s">
         <v>420</v>
       </c>
     </row>
@@ -21191,12 +21181,12 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="36" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="36" t="s">
         <v>396</v>
       </c>
     </row>
@@ -21233,10 +21223,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="38" t="s">
+      <c r="B25" s="37" t="s">
         <v>411</v>
       </c>
-      <c r="F25" s="38" t="s">
+      <c r="F25" s="37" t="s">
         <v>410</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating code which old url is updated dynamic in xl
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2728" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2736" uniqueCount="433">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1140,6 +1140,9 @@
     <t xml:space="preserve">applicationURL</t>
   </si>
   <si>
+    <t xml:space="preserve">oldAppURL</t>
+  </si>
+  <si>
     <t xml:space="preserve">applicationName</t>
   </si>
   <si>
@@ -1212,103 +1215,112 @@
     <t xml:space="preserve">11.0.0</t>
   </si>
   <si>
+    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uiautomator2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://readuser:Re@d@1234@20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.5-06-12-2021-19:31.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation-1-0-7-21-12-2021.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.6-13-12-2021-17:50.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_0003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhone7_iOS_13.1.3_316f0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneXS_iOS_14.1.0_21d51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM01_Android_11.0.0_7425f</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAMSUNG_GalaxyM12_Android_11.0.0_df6a7</t>
   </si>
   <si>
-    <t xml:space="preserve">uiautomator2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://readuser:Re@d@1234@20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.5-06-12-2021-19:31.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automation-1-0-7-21-12-2021.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.0.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_0003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ios</t>
+    <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
   </si>
   <si>
     <t xml:space="preserve">13.5.1</t>
   </si>
   <si>
-    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.3.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneXS_iOS_14.1.0_21d51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM01_Android_11.0.0_7425f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhone7_iOS_13.1.3_316f0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.1.3</t>
-  </si>
-  <si>
     <t xml:space="preserve">APPLE_iPhoneX_iOS_13.3.1_90703</t>
   </si>
   <si>
     <t xml:space="preserve">APPLE_iPhoneX_iOS_14.0.0_1b718</t>
+  </si>
+  <si>
+    <t>di</t>
+  </si>
+  <si>
+    <t>https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
   </si>
 </sst>
 </file>
@@ -1322,7 +1334,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1426,6 +1438,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF067D17"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF808080"/>
       <name val="JetBrains Mono"/>
@@ -1515,7 +1533,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1652,6 +1670,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1660,7 +1682,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1763,56 +1785,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="0" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="12.85" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
+    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
+    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
+    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
+    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
+    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
+    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
+    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
+    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
+    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
+    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
+    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
+    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
+    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
+    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="991" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20611,37 +20633,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="5.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="17" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="17" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="17" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="17" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="17" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="17" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="17" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="17" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="17" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="17" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="17" width="26.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="17" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="17" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="17" width="9.17"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="17" width="12.57" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="17" width="5.18" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="4" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="17" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="17" width="20.5" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="17" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="17" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="17" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="13" customWidth="true" hidden="false" style="17" width="14.87" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="17" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="17" width="26.35" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="17" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="17" width="29.45" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="1025" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -20690,429 +20712,448 @@
       <c r="P1" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="19" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S1" s="4" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>381</v>
-      </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+        <v>382</v>
+      </c>
+      <c r="E2"/>
+      <c r="F2"/>
       <c r="G2" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="H2" s="21"/>
+        <v>383</v>
+      </c>
+      <c r="H2"/>
       <c r="I2" s="21" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>384</v>
-      </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="25" t="s">
         <v>385</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2" s="25" t="s">
         <v>386</v>
       </c>
-      <c r="O2" s="24"/>
-      <c r="P2" s="23" t="n">
+      <c r="O2" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="P2"/>
+      <c r="Q2" s="23" t="n">
         <v>500</v>
       </c>
-      <c r="Q2" s="26" t="s">
-        <v>387</v>
-      </c>
-      <c r="R2" s="23" t="n">
+      <c r="R2" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="S2" s="23" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3" s="20" t="s">
+        <v>383</v>
+      </c>
+      <c r="H3"/>
+      <c r="I3" s="27" t="s">
+        <v>390</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>385</v>
+      </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3" s="25" t="s">
+        <v>386</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="P3"/>
+      <c r="Q3" s="20" t="n">
+        <v>103</v>
+      </c>
+      <c r="R3" s="27" t="s">
         <v>388</v>
       </c>
-      <c r="B3" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>380</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>381</v>
-      </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20" t="s">
-        <v>382</v>
-      </c>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27" t="s">
-        <v>389</v>
-      </c>
-      <c r="J3" s="27" t="s">
-        <v>384</v>
-      </c>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="25" t="s">
-        <v>385</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>386</v>
-      </c>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20" t="n">
-        <v>103</v>
-      </c>
-      <c r="Q3" s="27" t="s">
-        <v>387</v>
-      </c>
-      <c r="R3" s="28" t="n">
+      <c r="S3" s="28" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="T3" s="29"/>
-    </row>
-    <row r="4" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U3" s="29"/>
+    </row>
+    <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="I4" s="31" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>398</v>
-      </c>
-      <c r="L4" s="32" t="s">
         <v>399</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="L4" t="s">
+        <v>432</v>
+      </c>
+      <c r="M4" s="32" t="s">
         <v>400</v>
       </c>
-      <c r="N4" s="11" t="s">
-        <v>386</v>
-      </c>
-      <c r="O4" s="8"/>
-      <c r="P4" s="20" t="n">
+      <c r="N4" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="P4"/>
+      <c r="Q4" s="20" t="n">
         <v>306</v>
       </c>
-      <c r="Q4" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="R4" s="33" t="n">
+      <c r="R4" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="S4" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>394</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="L5"/>
+      <c r="M5" s="32" t="s">
+        <v>400</v>
+      </c>
+      <c r="N5" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="P5"/>
+      <c r="Q5" s="20" t="n">
+        <v>307</v>
+      </c>
+      <c r="R5" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>392</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>393</v>
-      </c>
-      <c r="F5" s="30" t="s">
-        <v>394</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>403</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>404</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>398</v>
-      </c>
-      <c r="L5" s="32" t="s">
-        <v>399</v>
-      </c>
-      <c r="M5" s="25" t="s">
-        <v>400</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>386</v>
-      </c>
-      <c r="O5" s="8"/>
-      <c r="P5" s="20" t="n">
-        <v>307</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="R5" s="33" t="n">
+      <c r="S5" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="I6" s="34" t="s">
-        <v>406</v>
+        <v>396</v>
+      </c>
+      <c r="I6" s="31" t="s">
+        <v>397</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="K6" s="8"/>
-      <c r="L6" s="32" t="s">
-        <v>399</v>
-      </c>
-      <c r="M6" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="K6"/>
+      <c r="L6" s="34" t="s">
+        <v>407</v>
+      </c>
+      <c r="M6" s="32" t="s">
         <v>400</v>
       </c>
-      <c r="N6" s="11" t="s">
-        <v>386</v>
-      </c>
-      <c r="O6" s="8"/>
-      <c r="P6" s="20" t="n">
+      <c r="N6" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="P6"/>
+      <c r="Q6" s="20" t="n">
         <v>106</v>
       </c>
-      <c r="Q6" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="R6" s="33" t="n">
+      <c r="R6" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="S6" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="I7" s="34" t="s">
-        <v>406</v>
+        <v>396</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>409</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="K7" s="8"/>
-      <c r="L7" s="32" t="s">
-        <v>399</v>
-      </c>
-      <c r="M7" s="25" t="s">
-        <v>385</v>
-      </c>
-      <c r="N7" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7" s="32" t="s">
+        <v>400</v>
+      </c>
+      <c r="N7" s="25" t="s">
         <v>386</v>
       </c>
-      <c r="O7" s="8"/>
-      <c r="P7" s="20" t="n">
+      <c r="O7" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="P7"/>
+      <c r="Q7" s="20" t="n">
         <v>306</v>
       </c>
-      <c r="Q7" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="R7" s="33" t="n">
+      <c r="R7" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="S7" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="D8" s="35" t="s">
-        <v>409</v>
+        <v>392</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>411</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="H8" s="35" t="s">
-        <v>410</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>411</v>
-      </c>
-      <c r="J8" s="34" t="s">
+        <v>383</v>
+      </c>
+      <c r="H8" s="36" t="s">
         <v>412</v>
       </c>
-      <c r="K8" s="34" t="s">
+      <c r="I8" s="31" t="s">
         <v>413</v>
       </c>
-      <c r="L8" s="11"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="1" t="n">
+      <c r="J8" s="35" t="s">
+        <v>414</v>
+      </c>
+      <c r="K8" s="35" t="s">
+        <v>415</v>
+      </c>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="Q8" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="R8" s="33" t="n">
+      <c r="R8" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="S8" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
+        <v>416</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>394</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>383</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>417</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="J9" s="35" t="s">
         <v>414</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>409</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>393</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>394</v>
-      </c>
-      <c r="G9" s="35" t="s">
-        <v>382</v>
-      </c>
-      <c r="H9" s="35" t="s">
+      <c r="K9" s="38" t="s">
         <v>415</v>
       </c>
-      <c r="I9" s="8" t="s">
-        <v>416</v>
-      </c>
-      <c r="J9" s="34" t="s">
-        <v>412</v>
-      </c>
-      <c r="K9" s="37" t="s">
-        <v>413</v>
-      </c>
-      <c r="P9" s="1" t="n">
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9" s="1" t="n">
         <v>501</v>
       </c>
-      <c r="Q9" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="R9" s="33" t="n">
+      <c r="R9" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="S9" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1" display="http://127.0.0.1:4723/wd/hub"/>
-    <hyperlink ref="Q3" r:id="rId2" display="http://127.0.0.1:4723/wd/hub"/>
+    <hyperlink ref="R2" r:id="rId1" display="http://127.0.0.1:4723/wd/hub"/>
+    <hyperlink ref="R3" r:id="rId2" display="http://127.0.0.1:4723/wd/hub"/>
     <hyperlink ref="E4" r:id="rId3" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="Q4" r:id="rId4" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="R4" r:id="rId4" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E5" r:id="rId5" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="Q5" r:id="rId6" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="R5" r:id="rId6" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E6" r:id="rId7" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="Q6" r:id="rId8" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="R6" r:id="rId8" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E7" r:id="rId9" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="Q7" r:id="rId10" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="R7" r:id="rId10" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E8" r:id="rId11" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="Q8" r:id="rId12" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="R8" r:id="rId12" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E9" r:id="rId13" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="Q9" r:id="rId14" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="R9" r:id="rId14" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -21132,72 +21173,72 @@
   <dimension ref="B4:F28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
+    <col min="1" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>417</v>
+        <v>397</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="38" t="s">
-        <v>406</v>
+      <c r="B5" s="39" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="38" t="s">
-        <v>418</v>
+      <c r="B6" s="39" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="38" t="s">
-        <v>406</v>
+      <c r="B7" s="39" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="38" t="s">
-        <v>419</v>
+      <c r="B8" s="39" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="38" t="s">
-        <v>420</v>
+      <c r="B9" s="39" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="38" t="s">
-        <v>419</v>
+      <c r="B11" s="39" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="38" t="s">
-        <v>421</v>
+      <c r="B13" s="39" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>396</v>
+        <v>425</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -21206,38 +21247,38 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="39" t="s">
-        <v>411</v>
-      </c>
-      <c r="F25" s="39" t="s">
-        <v>410</v>
+      <c r="B25" s="40" t="s">
+        <v>427</v>
+      </c>
+      <c r="F25" s="40" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating hooks class with android old url
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2736" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2732" uniqueCount="432">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1224,6 +1224,9 @@
     <t xml:space="preserve">http://readuser:Re@d@1234@20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.5-06-12-2021-19:31.apk</t>
   </si>
   <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
+  </si>
+  <si>
     <t xml:space="preserve">Automation-1-0-7-21-12-2021.apk</t>
   </si>
   <si>
@@ -1315,12 +1318,6 @@
   </si>
   <si>
     <t xml:space="preserve">APPLE_iPhoneX_iOS_14.0.0_1b718</t>
-  </si>
-  <si>
-    <t>di</t>
-  </si>
-  <si>
-    <t>https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
   </si>
 </sst>
 </file>
@@ -1334,7 +1331,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1397,13 +1394,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="13.5"/>
-      <color rgb="FF000000"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="JetBrains Mono"/>
@@ -1425,27 +1415,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF067D17"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF067D17"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF808080"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
@@ -1533,7 +1504,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1622,15 +1593,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1638,11 +1601,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1654,15 +1617,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1670,11 +1629,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1682,15 +1637,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1720,11 +1671,11 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF067D17"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF6A8759"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB4C7DC"/>
-      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF6A8759"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
@@ -1785,56 +1736,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="12.85" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
-    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
-    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
-    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
-    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
-    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
-    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
-    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
-    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
-    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
-    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
-    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
-    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
-    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
-    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
-    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="991" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20636,31 +20587,31 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="17" width="12.57" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="17" width="5.18" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="4" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="17" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="17" width="20.5" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="17" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="17" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="17" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="13" customWidth="true" hidden="false" style="17" width="14.87" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="17" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="17" width="26.35" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="17" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="17" width="29.45" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="1025" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="17" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="17" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="17" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="17" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="17" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="17" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="17" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="17" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="17" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="17" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="17" width="26.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="17" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="17" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="17" width="9.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20735,35 +20686,28 @@
       <c r="D2" s="21" t="s">
         <v>382</v>
       </c>
-      <c r="E2"/>
-      <c r="F2"/>
       <c r="G2" s="21" t="s">
         <v>383</v>
       </c>
-      <c r="H2"/>
       <c r="I2" s="21" t="s">
         <v>384</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="22" t="s">
         <v>385</v>
       </c>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="23" t="s">
         <v>386</v>
       </c>
       <c r="O2" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="P2"/>
-      <c r="Q2" s="23" t="n">
+      <c r="Q2" s="22" t="n">
         <v>500</v>
       </c>
-      <c r="R2" s="26" t="s">
+      <c r="R2" s="24" t="s">
         <v>388</v>
       </c>
-      <c r="S2" s="23" t="n">
+      <c r="S2" s="22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -20780,41 +20724,34 @@
       <c r="D3" s="20" t="s">
         <v>382</v>
       </c>
-      <c r="E3"/>
-      <c r="F3"/>
       <c r="G3" s="20" t="s">
         <v>383</v>
       </c>
-      <c r="H3"/>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="25" t="s">
         <v>390</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="25" t="s">
         <v>385</v>
       </c>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3" s="25" t="s">
+      <c r="N3" s="23" t="s">
         <v>386</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="P3"/>
       <c r="Q3" s="20" t="n">
         <v>103</v>
       </c>
-      <c r="R3" s="27" t="s">
+      <c r="R3" s="25" t="s">
         <v>388</v>
       </c>
-      <c r="S3" s="28" t="b">
+      <c r="S3" s="26" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="U3" s="29"/>
-    </row>
-    <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U3" s="27"/>
+    </row>
+    <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>391</v>
       </c>
@@ -20827,10 +20764,10 @@
       <c r="D4" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="28" t="s">
         <v>394</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="28" t="s">
         <v>395</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -20839,7 +20776,7 @@
       <c r="H4" s="8" t="s">
         <v>396</v>
       </c>
-      <c r="I4" s="31" t="s">
+      <c r="I4" s="8" t="s">
         <v>397</v>
       </c>
       <c r="J4" s="8" t="s">
@@ -20848,33 +20785,32 @@
       <c r="K4" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="L4" t="s">
-        <v>432</v>
-      </c>
-      <c r="M4" s="32" t="s">
+      <c r="L4" s="17" t="s">
         <v>400</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="M4" s="29" t="s">
         <v>401</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>402</v>
       </c>
       <c r="O4" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="P4"/>
       <c r="Q4" s="20" t="n">
         <v>306</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="S4" s="33" t="b">
+        <v>403</v>
+      </c>
+      <c r="S4" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>44</v>
@@ -20885,20 +20821,20 @@
       <c r="D5" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="28" t="s">
         <v>394</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="28" t="s">
         <v>395</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>383</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>398</v>
@@ -20906,31 +20842,32 @@
       <c r="K5" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="L5"/>
-      <c r="M5" s="32" t="s">
+      <c r="L5" s="17" t="s">
         <v>400</v>
       </c>
-      <c r="N5" s="25" t="s">
+      <c r="M5" s="29" t="s">
         <v>401</v>
+      </c>
+      <c r="N5" s="23" t="s">
+        <v>402</v>
       </c>
       <c r="O5" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="P5"/>
       <c r="Q5" s="20" t="n">
         <v>307</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="S5" s="33" t="b">
+        <v>403</v>
+      </c>
+      <c r="S5" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>44</v>
@@ -20941,10 +20878,10 @@
       <c r="D6" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="28" t="s">
         <v>394</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="28" t="s">
         <v>395</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -20953,40 +20890,38 @@
       <c r="H6" s="8" t="s">
         <v>396</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="8" t="s">
         <v>397</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="K6"/>
-      <c r="L6" s="34" t="s">
-        <v>407</v>
-      </c>
-      <c r="M6" s="32" t="s">
-        <v>400</v>
-      </c>
-      <c r="N6" s="25" t="s">
+      <c r="L6" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="M6" s="29" t="s">
         <v>401</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>402</v>
       </c>
       <c r="O6" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="P6"/>
       <c r="Q6" s="20" t="n">
         <v>106</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="S6" s="33" t="b">
+        <v>403</v>
+      </c>
+      <c r="S6" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>44</v>
@@ -20997,10 +20932,10 @@
       <c r="D7" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="28" t="s">
         <v>394</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="28" t="s">
         <v>395</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -21009,38 +20944,35 @@
       <c r="H7" s="8" t="s">
         <v>396</v>
       </c>
-      <c r="I7" s="35" t="s">
-        <v>409</v>
+      <c r="I7" s="31" t="s">
+        <v>410</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7" s="32" t="s">
-        <v>400</v>
-      </c>
-      <c r="N7" s="25" t="s">
+      <c r="M7" s="29" t="s">
+        <v>401</v>
+      </c>
+      <c r="N7" s="23" t="s">
         <v>386</v>
       </c>
       <c r="O7" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="P7"/>
       <c r="Q7" s="20" t="n">
         <v>306</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="S7" s="33" t="b">
+        <v>403</v>
+      </c>
+      <c r="S7" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>44</v>
@@ -21048,49 +20980,44 @@
       <c r="C8" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="D8" s="36" t="s">
-        <v>411</v>
-      </c>
-      <c r="E8" s="30" t="s">
+      <c r="D8" s="32" t="s">
+        <v>412</v>
+      </c>
+      <c r="E8" s="28" t="s">
         <v>394</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="28" t="s">
         <v>395</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="H8" s="36" t="s">
-        <v>412</v>
-      </c>
-      <c r="I8" s="31" t="s">
+      <c r="H8" s="32" t="s">
         <v>413</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="I8" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="K8" s="35" t="s">
+      <c r="J8" s="31" t="s">
         <v>415</v>
       </c>
-      <c r="L8"/>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
+      <c r="K8" s="31" t="s">
+        <v>416</v>
+      </c>
       <c r="Q8" s="1" t="n">
         <v>500</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="S8" s="33" t="b">
+        <v>403</v>
+      </c>
+      <c r="S8" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>44</v>
@@ -21099,41 +21026,36 @@
         <v>392</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>411</v>
-      </c>
-      <c r="E9" s="30" t="s">
+        <v>412</v>
+      </c>
+      <c r="E9" s="28" t="s">
         <v>394</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="28" t="s">
         <v>395</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="32" t="s">
         <v>383</v>
       </c>
-      <c r="H9" s="36" t="s">
-        <v>417</v>
+      <c r="H9" s="32" t="s">
+        <v>418</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>418</v>
-      </c>
-      <c r="J9" s="35" t="s">
-        <v>414</v>
-      </c>
-      <c r="K9" s="38" t="s">
+        <v>419</v>
+      </c>
+      <c r="J9" s="31" t="s">
         <v>415</v>
       </c>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
+      <c r="K9" s="33" t="s">
+        <v>416</v>
+      </c>
       <c r="Q9" s="1" t="n">
         <v>501</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="S9" s="33" t="b">
+        <v>403</v>
+      </c>
+      <c r="S9" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21178,7 +21100,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21187,58 +21109,58 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="39" t="s">
-        <v>409</v>
+      <c r="B5" s="34" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="39" t="s">
-        <v>419</v>
+      <c r="B6" s="34" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="39" t="s">
-        <v>409</v>
+      <c r="B7" s="34" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="39" t="s">
-        <v>420</v>
+      <c r="B8" s="34" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="39" t="s">
-        <v>421</v>
+      <c r="B9" s="34" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="39" t="s">
-        <v>420</v>
+      <c r="B11" s="34" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="39" t="s">
-        <v>422</v>
+      <c r="B13" s="34" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -21247,38 +21169,38 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>413</v>
       </c>
-      <c r="F24" s="0" t="s">
-        <v>412</v>
-      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="40" t="s">
-        <v>427</v>
-      </c>
-      <c r="F25" s="40" t="s">
+      <c r="B25" s="35" t="s">
         <v>428</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating old jacoco plugin in pom file
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2735" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2778" uniqueCount="434">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1224,27 +1224,30 @@
     <t xml:space="preserve">http://readuser:Re@d@1234@20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.5-06-12-2021-19:31.apk</t>
   </si>
   <si>
+    <t xml:space="preserve">http://amazon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation-1-0-7-21-12-2021.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
   </si>
   <si>
-    <t xml:space="preserve">Automation-1-0-7-21-12-2021.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.0.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
-  </si>
-  <si>
     <t xml:space="preserve">Android_003</t>
   </si>
   <si>
@@ -1320,7 +1323,7 @@
     <t xml:space="preserve">APPLE_iPhoneX_iOS_14.0.0_1b718</t>
   </si>
   <si>
-    <t>https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
+    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
   </si>
 </sst>
 </file>
@@ -20590,11 +20593,11 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="L7" activeCellId="0" sqref="L7"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L4" activeCellId="0" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20768,7 +20771,7 @@
       </c>
       <c r="U3" s="27"/>
     </row>
-    <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>391</v>
       </c>
@@ -20803,7 +20806,7 @@
         <v>399</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="M4" s="29" t="s">
         <v>401</v>
@@ -20861,7 +20864,7 @@
         <v>399</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="M5" s="29" t="s">
         <v>401</v>
@@ -20886,7 +20889,7 @@
     </row>
     <row r="6" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>44</v>
@@ -20917,7 +20920,7 @@
       </c>
       <c r="K6"/>
       <c r="L6" s="11" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="M6" s="29" t="s">
         <v>401</v>
@@ -20942,7 +20945,7 @@
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>44</v>
@@ -20966,13 +20969,15 @@
         <v>396</v>
       </c>
       <c r="I7" s="31" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>398</v>
       </c>
       <c r="K7"/>
-      <c r="L7"/>
+      <c r="L7" t="s">
+        <v>433</v>
+      </c>
       <c r="M7" s="29" t="s">
         <v>401</v>
       </c>
@@ -20996,7 +21001,7 @@
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>44</v>
@@ -21005,7 +21010,7 @@
         <v>392</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E8" s="28" t="s">
         <v>394</v>
@@ -21017,16 +21022,16 @@
         <v>383</v>
       </c>
       <c r="H8" s="32" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="J8" s="31" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="K8" s="31" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="L8"/>
       <c r="M8"/>
@@ -21046,7 +21051,7 @@
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>44</v>
@@ -21055,7 +21060,7 @@
         <v>392</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E9" s="28" t="s">
         <v>394</v>
@@ -21067,16 +21072,16 @@
         <v>383</v>
       </c>
       <c r="H9" s="32" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="J9" s="31" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="K9" s="33" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="L9"/>
       <c r="M9"/>
@@ -21099,18 +21104,19 @@
     <hyperlink ref="R2" r:id="rId1" display="http://127.0.0.1:4723/wd/hub"/>
     <hyperlink ref="R3" r:id="rId2" display="http://127.0.0.1:4723/wd/hub"/>
     <hyperlink ref="E4" r:id="rId3" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="R4" r:id="rId4" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
-    <hyperlink ref="E5" r:id="rId5" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="R5" r:id="rId6" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
-    <hyperlink ref="E6" r:id="rId7" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="L6" r:id="rId8" display="http://di"/>
-    <hyperlink ref="R6" r:id="rId9" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
-    <hyperlink ref="E7" r:id="rId10" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="R7" r:id="rId11" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
-    <hyperlink ref="E8" r:id="rId12" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="R8" r:id="rId13" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
-    <hyperlink ref="E9" r:id="rId14" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="R9" r:id="rId15" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="L4" r:id="rId4" display="http://amazon"/>
+    <hyperlink ref="R4" r:id="rId5" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="E5" r:id="rId6" display="sriganesh.d@i-exceed.com"/>
+    <hyperlink ref="R5" r:id="rId7" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="E6" r:id="rId8" display="sriganesh.d@i-exceed.com"/>
+    <hyperlink ref="L6" r:id="rId9" display="http://di"/>
+    <hyperlink ref="R6" r:id="rId10" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="E7" r:id="rId11" display="sriganesh.d@i-exceed.com"/>
+    <hyperlink ref="R7" r:id="rId12" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="E8" r:id="rId13" display="sriganesh.d@i-exceed.com"/>
+    <hyperlink ref="R8" r:id="rId14" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="E9" r:id="rId15" display="sriganesh.d@i-exceed.com"/>
+    <hyperlink ref="R9" r:id="rId16" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -21145,27 +21151,27 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="34" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="34" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="34" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="34" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="34" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21175,27 +21181,27 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="34" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="34" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -21204,38 +21210,38 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>414</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="35" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="F25" s="35" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sonar fix for pcloudy connection class
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2778" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2779" uniqueCount="435">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1324,6 +1324,9 @@
   </si>
   <si>
     <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
+  </si>
+  <si>
+    <t>https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
   </si>
 </sst>
 </file>
@@ -20806,7 +20809,7 @@
         <v>399</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="M4" s="29" t="s">
         <v>401</v>

</xml_diff>

<commit_message>
made sonar fix changes in pcloudy connection class and homepageStepDef
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2779" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2732" uniqueCount="433">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1266,67 +1266,61 @@
     <t xml:space="preserve">ios</t>
   </si>
   <si>
+    <t xml:space="preserve">13.5.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneXS_iOS_14.1.0_21d51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM01_Android_11.0.0_7425f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM12_Android_11.0.0_df6a7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhone7_iOS_13.1.3_316f0</t>
+  </si>
+  <si>
     <t xml:space="preserve">13.1.3</t>
   </si>
   <si>
-    <t xml:space="preserve">APPLE_iPhone7_iOS_13.1.3_316f0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.3.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneXS_iOS_14.1.0_21d51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM01_Android_11.0.0_7425f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM12_Android_11.0.0_df6a7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.5.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">APPLE_iPhoneX_iOS_13.3.1_90703</t>
   </si>
   <si>
     <t xml:space="preserve">APPLE_iPhoneX_iOS_14.0.0_1b718</t>
-  </si>
-  <si>
-    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
-  </si>
-  <si>
-    <t>https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
   </si>
 </sst>
 </file>
@@ -1340,7 +1334,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1430,6 +1424,12 @@
       <family val="3"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1513,7 +1513,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1646,6 +1646,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1745,56 +1749,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="12.85" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
-    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
-    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
-    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
-    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
-    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
-    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
-    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
-    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
-    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
-    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
-    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
-    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
-    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
-    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
-    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="991" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20596,31 +20600,31 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L4" activeCellId="0" sqref="L4"/>
+      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="17" width="12.57" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="17" width="5.18" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="4" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="17" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="17" width="20.5" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="17" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="17" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="17" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="13" customWidth="true" hidden="false" style="17" width="14.87" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="17" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="17" width="26.35" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="17" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="17" width="29.45" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="1025" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="17" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="17" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="17" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="17" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="17" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="17" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="17" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="17" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="17" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="17" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="17" width="26.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="17" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="17" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="17" width="9.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20695,28 +20699,21 @@
       <c r="D2" s="21" t="s">
         <v>382</v>
       </c>
-      <c r="E2"/>
-      <c r="F2"/>
       <c r="G2" s="21" t="s">
         <v>383</v>
       </c>
-      <c r="H2"/>
       <c r="I2" s="21" t="s">
         <v>384</v>
       </c>
       <c r="J2" s="22" t="s">
         <v>385</v>
       </c>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
       <c r="N2" s="23" t="s">
         <v>386</v>
       </c>
       <c r="O2" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="P2"/>
       <c r="Q2" s="22" t="n">
         <v>500</v>
       </c>
@@ -20740,35 +20737,28 @@
       <c r="D3" s="20" t="s">
         <v>382</v>
       </c>
-      <c r="E3"/>
-      <c r="F3"/>
       <c r="G3" s="20" t="s">
         <v>383</v>
       </c>
-      <c r="H3"/>
       <c r="I3" s="25" t="s">
         <v>390</v>
       </c>
       <c r="J3" s="25" t="s">
         <v>385</v>
       </c>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
       <c r="N3" s="23" t="s">
         <v>386</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="P3"/>
       <c r="Q3" s="20" t="n">
         <v>103</v>
       </c>
       <c r="R3" s="25" t="s">
         <v>388</v>
       </c>
-      <c r="S3" s="26" t="b">
+      <c r="S3" s="26" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20809,7 +20799,7 @@
         <v>399</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>434</v>
+        <v>400</v>
       </c>
       <c r="M4" s="29" t="s">
         <v>401</v>
@@ -20820,14 +20810,13 @@
       <c r="O4" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="P4"/>
       <c r="Q4" s="20" t="n">
         <v>306</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S4" s="30" t="b">
+      <c r="S4" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20878,14 +20867,13 @@
       <c r="O5" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="P5"/>
       <c r="Q5" s="20" t="n">
         <v>307</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S5" s="30" t="b">
+      <c r="S5" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20921,7 +20909,6 @@
       <c r="J6" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="K6"/>
       <c r="L6" s="11" t="s">
         <v>409</v>
       </c>
@@ -20934,14 +20921,13 @@
       <c r="O6" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="P6"/>
       <c r="Q6" s="20" t="n">
         <v>106</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S6" s="30" t="b">
+      <c r="S6" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20977,10 +20963,6 @@
       <c r="J7" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="K7"/>
-      <c r="L7" t="s">
-        <v>433</v>
-      </c>
       <c r="M7" s="29" t="s">
         <v>401</v>
       </c>
@@ -20990,14 +20972,13 @@
       <c r="O7" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="P7"/>
       <c r="Q7" s="20" t="n">
         <v>306</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S7" s="30" t="b">
+      <c r="S7" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21027,7 +21008,7 @@
       <c r="H8" s="32" t="s">
         <v>414</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="33" t="s">
         <v>415</v>
       </c>
       <c r="J8" s="31" t="s">
@@ -21036,18 +21017,13 @@
       <c r="K8" s="31" t="s">
         <v>417</v>
       </c>
-      <c r="L8"/>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
       <c r="Q8" s="1" t="n">
         <v>500</v>
       </c>
       <c r="R8" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S8" s="30" t="b">
+      <c r="S8" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21083,21 +21059,16 @@
       <c r="J9" s="31" t="s">
         <v>416</v>
       </c>
-      <c r="K9" s="33" t="s">
+      <c r="K9" s="34" t="s">
         <v>417</v>
       </c>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
       <c r="Q9" s="1" t="n">
         <v>501</v>
       </c>
       <c r="R9" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S9" s="30" t="b">
+      <c r="S9" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21139,12 +21110,12 @@
   <dimension ref="B4:F28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21153,27 +21124,27 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="35" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="35" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="35" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="35" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="35" t="s">
         <v>423</v>
       </c>
     </row>
@@ -21183,12 +21154,12 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="35" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="35" t="s">
         <v>424</v>
       </c>
     </row>
@@ -21218,18 +21189,18 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="36" t="s">
         <v>415</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="F25" s="36" t="s">
         <v>414</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="35" t="s">
-        <v>429</v>
-      </c>
-      <c r="F25" s="35" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
made sonar fixes in connection class and pcloudy class
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2732" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2733" uniqueCount="434">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1321,6 +1321,9 @@
   </si>
   <si>
     <t xml:space="preserve">APPLE_iPhoneX_iOS_14.0.0_1b718</t>
+  </si>
+  <si>
+    <t>https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
   </si>
 </sst>
 </file>
@@ -1749,56 +1752,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="0" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="12.85" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
+    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
+    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
+    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
+    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
+    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
+    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
+    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
+    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
+    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
+    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
+    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
+    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
+    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
+    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="991" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20609,22 +20612,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="5.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="17" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="17" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="17" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="17" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="17" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="17" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="17" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="17" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="17" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="17" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="17" width="26.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="17" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="17" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="17" width="9.17"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="17" width="12.57" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="17" width="5.18" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="4" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="17" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="17" width="20.5" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="17" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="17" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="17" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="13" customWidth="true" hidden="false" style="17" width="14.87" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="17" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="17" width="26.35" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="17" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="17" width="29.45" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="1025" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20699,21 +20702,28 @@
       <c r="D2" s="21" t="s">
         <v>382</v>
       </c>
+      <c r="E2"/>
+      <c r="F2"/>
       <c r="G2" s="21" t="s">
         <v>383</v>
       </c>
+      <c r="H2"/>
       <c r="I2" s="21" t="s">
         <v>384</v>
       </c>
       <c r="J2" s="22" t="s">
         <v>385</v>
       </c>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
       <c r="N2" s="23" t="s">
         <v>386</v>
       </c>
       <c r="O2" s="11" t="s">
         <v>387</v>
       </c>
+      <c r="P2"/>
       <c r="Q2" s="22" t="n">
         <v>500</v>
       </c>
@@ -20737,28 +20747,35 @@
       <c r="D3" s="20" t="s">
         <v>382</v>
       </c>
+      <c r="E3"/>
+      <c r="F3"/>
       <c r="G3" s="20" t="s">
         <v>383</v>
       </c>
+      <c r="H3"/>
       <c r="I3" s="25" t="s">
         <v>390</v>
       </c>
       <c r="J3" s="25" t="s">
         <v>385</v>
       </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
       <c r="N3" s="23" t="s">
         <v>386</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>387</v>
       </c>
+      <c r="P3"/>
       <c r="Q3" s="20" t="n">
         <v>103</v>
       </c>
       <c r="R3" s="25" t="s">
         <v>388</v>
       </c>
-      <c r="S3" s="26" t="n">
+      <c r="S3" s="26" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20799,7 +20816,7 @@
         <v>399</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>400</v>
+        <v>433</v>
       </c>
       <c r="M4" s="29" t="s">
         <v>401</v>
@@ -20810,13 +20827,14 @@
       <c r="O4" s="11" t="s">
         <v>387</v>
       </c>
+      <c r="P4"/>
       <c r="Q4" s="20" t="n">
         <v>306</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S4" s="30" t="n">
+      <c r="S4" s="30" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20867,13 +20885,14 @@
       <c r="O5" s="11" t="s">
         <v>387</v>
       </c>
+      <c r="P5"/>
       <c r="Q5" s="20" t="n">
         <v>307</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S5" s="30" t="n">
+      <c r="S5" s="30" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20909,6 +20928,7 @@
       <c r="J6" s="8" t="s">
         <v>398</v>
       </c>
+      <c r="K6"/>
       <c r="L6" s="11" t="s">
         <v>409</v>
       </c>
@@ -20921,13 +20941,14 @@
       <c r="O6" s="11" t="s">
         <v>387</v>
       </c>
+      <c r="P6"/>
       <c r="Q6" s="20" t="n">
         <v>106</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S6" s="30" t="n">
+      <c r="S6" s="30" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20963,6 +20984,8 @@
       <c r="J7" s="8" t="s">
         <v>398</v>
       </c>
+      <c r="K7"/>
+      <c r="L7"/>
       <c r="M7" s="29" t="s">
         <v>401</v>
       </c>
@@ -20972,13 +20995,14 @@
       <c r="O7" s="11" t="s">
         <v>387</v>
       </c>
+      <c r="P7"/>
       <c r="Q7" s="20" t="n">
         <v>306</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S7" s="30" t="n">
+      <c r="S7" s="30" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21017,13 +21041,18 @@
       <c r="K8" s="31" t="s">
         <v>417</v>
       </c>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
       <c r="Q8" s="1" t="n">
         <v>500</v>
       </c>
       <c r="R8" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S8" s="30" t="n">
+      <c r="S8" s="30" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21062,13 +21091,18 @@
       <c r="K9" s="34" t="s">
         <v>417</v>
       </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
       <c r="Q9" s="1" t="n">
         <v>501</v>
       </c>
       <c r="R9" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S9" s="30" t="n">
+      <c r="S9" s="30" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21115,7 +21149,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
+    <col min="1" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updaing pcloudy connection class
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2733" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2737" uniqueCount="436">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1215,112 +1215,136 @@
     <t xml:space="preserve">11.0.0</t>
   </si>
   <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uiautomator2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://readuser:Re@d@1234@20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.5-06-12-2021-19:31.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://amazon</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF067D17"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">Automation-1-0-8-03-01-2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF067D17"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.apk</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_003</t>
+  </si>
+  <si>
     <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
   </si>
   <si>
-    <t xml:space="preserve">uiautomator2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://readuser:Re@d@1234@20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.5-06-12-2021-19:31.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://amazon</t>
+    <t xml:space="preserve">http://di</t>
   </si>
   <si>
     <t xml:space="preserve">Automation-1-0-7-21-12-2021.apk</t>
   </si>
   <si>
-    <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.0.0</t>
+    <t xml:space="preserve">Android_0003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneXS_iOS_14.1.0_21d51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
   </si>
   <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://di</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_0003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ios</t>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM01_Android_11.0.0_7425f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM12_Android_11.0.0_df6a7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhone7_iOS_13.1.3_316f0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.1.3</t>
   </si>
   <si>
     <t xml:space="preserve">13.5.1</t>
   </si>
   <si>
-    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.3.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneXS_iOS_14.1.0_21d51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM01_Android_11.0.0_7425f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM12_Android_11.0.0_df6a7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhone7_iOS_13.1.3_316f0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.1.3</t>
-  </si>
-  <si>
     <t xml:space="preserve">APPLE_iPhoneX_iOS_13.3.1_90703</t>
   </si>
   <si>
     <t xml:space="preserve">APPLE_iPhoneX_iOS_14.0.0_1b718</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhone7plus_iOS_13.3.1_ce483</t>
   </si>
   <si>
     <t>https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
@@ -1337,7 +1361,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1418,6 +1442,25 @@
       <color rgb="FF6A8759"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF067D17"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF067D17"/>
+      <name val=""/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1516,7 +1559,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1637,11 +1680,19 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1649,7 +1700,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20603,11 +20654,11 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20806,7 +20857,7 @@
       <c r="H4" s="8" t="s">
         <v>396</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="29" t="s">
         <v>397</v>
       </c>
       <c r="J4" s="8" t="s">
@@ -20816,9 +20867,9 @@
         <v>399</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>433</v>
-      </c>
-      <c r="M4" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="M4" s="30" t="s">
         <v>401</v>
       </c>
       <c r="N4" s="23" t="s">
@@ -20834,12 +20885,12 @@
       <c r="R4" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S4" s="30" t="b">
+      <c r="S4" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>404</v>
       </c>
@@ -20862,10 +20913,10 @@
         <v>383</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>406</v>
+        <v>396</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>397</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>398</v>
@@ -20874,9 +20925,9 @@
         <v>399</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>407</v>
-      </c>
-      <c r="M5" s="29" t="s">
+        <v>405</v>
+      </c>
+      <c r="M5" s="30" t="s">
         <v>401</v>
       </c>
       <c r="N5" s="23" t="s">
@@ -20892,14 +20943,14 @@
       <c r="R5" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S5" s="30" t="b">
+      <c r="S5" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>44</v>
@@ -20923,17 +20974,19 @@
         <v>396</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="K6"/>
+      <c r="K6" s="8" t="s">
+        <v>399</v>
+      </c>
       <c r="L6" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="M6" s="32" t="s">
         <v>409</v>
-      </c>
-      <c r="M6" s="29" t="s">
-        <v>401</v>
       </c>
       <c r="N6" s="23" t="s">
         <v>402</v>
@@ -20948,7 +21001,7 @@
       <c r="R6" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S6" s="30" t="b">
+      <c r="S6" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20976,18 +21029,20 @@
         <v>383</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="I7" s="31" t="s">
         <v>411</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>407</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="K7"/>
+      <c r="K7" s="8" t="s">
+        <v>399</v>
+      </c>
       <c r="L7"/>
-      <c r="M7" s="29" t="s">
-        <v>401</v>
+      <c r="M7" s="32" t="s">
+        <v>409</v>
       </c>
       <c r="N7" s="23" t="s">
         <v>386</v>
@@ -21002,7 +21057,7 @@
       <c r="R7" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S7" s="30" t="b">
+      <c r="S7" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21017,7 +21072,7 @@
       <c r="C8" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="34" t="s">
         <v>413</v>
       </c>
       <c r="E8" s="28" t="s">
@@ -21029,16 +21084,16 @@
       <c r="G8" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="34" t="s">
         <v>414</v>
       </c>
       <c r="I8" s="33" t="s">
         <v>415</v>
       </c>
-      <c r="J8" s="31" t="s">
+      <c r="J8" s="35" t="s">
         <v>416</v>
       </c>
-      <c r="K8" s="31" t="s">
+      <c r="K8" s="35" t="s">
         <v>417</v>
       </c>
       <c r="L8"/>
@@ -21052,7 +21107,7 @@
       <c r="R8" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S8" s="30" t="b">
+      <c r="S8" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21076,19 +21131,19 @@
       <c r="F9" s="28" t="s">
         <v>395</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="G9" s="34" t="s">
         <v>383</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="34" t="s">
+        <v>414</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="I9" s="8" t="s">
-        <v>420</v>
-      </c>
-      <c r="J9" s="31" t="s">
+      <c r="J9" s="35" t="s">
         <v>416</v>
       </c>
-      <c r="K9" s="34" t="s">
+      <c r="K9" s="36" t="s">
         <v>417</v>
       </c>
       <c r="L9"/>
@@ -21102,7 +21157,7 @@
       <c r="R9" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S9" s="30" t="b">
+      <c r="S9" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21141,10 +21196,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4:F28"/>
+  <dimension ref="B4:F29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21154,46 +21209,46 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="37" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="35" t="s">
-        <v>411</v>
-      </c>
-    </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="37" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="37" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="37" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="35" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="35" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="37" t="s">
         <v>422</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="35" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>406</v>
+        <v>423</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="35" t="s">
-        <v>422</v>
+      <c r="B11" s="37" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="37" t="s">
         <v>424</v>
       </c>
     </row>
@@ -21230,26 +21285,31 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="38" t="s">
         <v>415</v>
       </c>
-      <c r="F25" s="36" t="s">
-        <v>414</v>
+      <c r="F25" s="38" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>420</v>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating connection utilitis for for both android and ios
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2737" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2736" uniqueCount="436">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1224,7 +1224,7 @@
     <t xml:space="preserve">http://readuser:Re@d@1234@20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.5-06-12-2021-19:31.apk</t>
   </si>
   <si>
-    <t xml:space="preserve">http://amazon</t>
+    <t xml:space="preserve">http://20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.8-31-12-2021-14:16.apk</t>
   </si>
   <si>
     <r>
@@ -1233,6 +1233,7 @@
         <color rgb="FF067D17"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Automation-1-0-8-03-01-2022</t>
     </r>
@@ -1240,8 +1241,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF067D17"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.apk</t>
@@ -1347,7 +1348,7 @@
     <t xml:space="preserve">APPLE_iPhone7plus_iOS_13.3.1_ce483</t>
   </si>
   <si>
-    <t>https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -1361,7 +1362,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1446,35 +1447,10 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF067D17"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF067D17"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF067D17"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1559,7 +1535,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1676,11 +1652,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1688,20 +1660,12 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -20654,11 +20618,11 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K5" activeCellId="0" sqref="K5"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20867,9 +20831,9 @@
         <v>399</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>435</v>
-      </c>
-      <c r="M4" s="30" t="s">
+        <v>400</v>
+      </c>
+      <c r="M4" s="11" t="s">
         <v>401</v>
       </c>
       <c r="N4" s="23" t="s">
@@ -20885,7 +20849,7 @@
       <c r="R4" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S4" s="31" t="b">
+      <c r="S4" s="30" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20927,7 +20891,7 @@
       <c r="L5" s="17" t="s">
         <v>405</v>
       </c>
-      <c r="M5" s="30" t="s">
+      <c r="M5" s="11" t="s">
         <v>401</v>
       </c>
       <c r="N5" s="23" t="s">
@@ -20943,7 +20907,7 @@
       <c r="R5" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S5" s="31" t="b">
+      <c r="S5" s="30" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20985,7 +20949,7 @@
       <c r="L6" s="11" t="s">
         <v>408</v>
       </c>
-      <c r="M6" s="32" t="s">
+      <c r="M6" s="31" t="s">
         <v>409</v>
       </c>
       <c r="N6" s="23" t="s">
@@ -21001,7 +20965,7 @@
       <c r="R6" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S6" s="31" t="b">
+      <c r="S6" s="30" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21031,7 +20995,7 @@
       <c r="H7" s="8" t="s">
         <v>411</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="I7" s="8" t="s">
         <v>407</v>
       </c>
       <c r="J7" s="8" t="s">
@@ -21041,7 +21005,7 @@
         <v>399</v>
       </c>
       <c r="L7"/>
-      <c r="M7" s="32" t="s">
+      <c r="M7" s="31" t="s">
         <v>409</v>
       </c>
       <c r="N7" s="23" t="s">
@@ -21057,7 +21021,7 @@
       <c r="R7" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S7" s="31" t="b">
+      <c r="S7" s="30" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21072,7 +21036,7 @@
       <c r="C8" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="32" t="s">
         <v>413</v>
       </c>
       <c r="E8" s="28" t="s">
@@ -21084,19 +21048,21 @@
       <c r="G8" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="H8" s="34" t="s">
+      <c r="H8" s="32" t="s">
         <v>414</v>
       </c>
-      <c r="I8" s="33" t="s">
+      <c r="I8" s="8" t="s">
         <v>415</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="J8" s="29" t="s">
         <v>416</v>
       </c>
-      <c r="K8" s="35" t="s">
+      <c r="K8" s="29" t="s">
         <v>417</v>
       </c>
-      <c r="L8"/>
+      <c r="L8" t="s">
+        <v>435</v>
+      </c>
       <c r="M8"/>
       <c r="N8"/>
       <c r="O8"/>
@@ -21107,7 +21073,7 @@
       <c r="R8" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S8" s="31" t="b">
+      <c r="S8" s="30" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21131,19 +21097,19 @@
       <c r="F9" s="28" t="s">
         <v>395</v>
       </c>
-      <c r="G9" s="34" t="s">
+      <c r="G9" s="32" t="s">
         <v>383</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="32" t="s">
         <v>414</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="J9" s="35" t="s">
+      <c r="J9" s="29" t="s">
         <v>416</v>
       </c>
-      <c r="K9" s="36" t="s">
+      <c r="K9" s="33" t="s">
         <v>417</v>
       </c>
       <c r="L9"/>
@@ -21157,7 +21123,7 @@
       <c r="R9" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S9" s="31" t="b">
+      <c r="S9" s="30" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21167,7 +21133,7 @@
     <hyperlink ref="R2" r:id="rId1" display="http://127.0.0.1:4723/wd/hub"/>
     <hyperlink ref="R3" r:id="rId2" display="http://127.0.0.1:4723/wd/hub"/>
     <hyperlink ref="E4" r:id="rId3" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="L4" r:id="rId4" display="http://amazon"/>
+    <hyperlink ref="L4" r:id="rId4" display="http://20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.8-31-12-2021-14:16.apk"/>
     <hyperlink ref="R4" r:id="rId5" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E5" r:id="rId6" display="sriganesh.d@i-exceed.com"/>
     <hyperlink ref="R5" r:id="rId7" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
@@ -21199,7 +21165,7 @@
   <dimension ref="B4:F29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21213,27 +21179,27 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="34" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="34" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="34" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="34" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="34" t="s">
         <v>422</v>
       </c>
     </row>
@@ -21243,12 +21209,12 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="34" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="34" t="s">
         <v>424</v>
       </c>
     </row>
@@ -21285,10 +21251,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="38" t="s">
+      <c r="B25" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="F25" s="38" t="s">
+      <c r="F25" s="35" t="s">
         <v>431</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made changes in sonar fix
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2736" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2735" uniqueCount="433">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1224,29 +1224,10 @@
     <t xml:space="preserve">http://readuser:Re@d@1234@20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.5-06-12-2021-19:31.apk</t>
   </si>
   <si>
-    <t xml:space="preserve">http://20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.8-31-12-2021-14:16.apk</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF067D17"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Automation-1-0-8-03-01-2022</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF067D17"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.apk</t>
-    </r>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation-1-0-7-21-12-2021.apk</t>
   </si>
   <si>
     <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
@@ -1258,7 +1239,10 @@
     <t xml:space="preserve">Android_002</t>
   </si>
   <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
+    <t xml:space="preserve">9.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
   </si>
   <si>
     <t xml:space="preserve">Android_003</t>
@@ -1270,36 +1254,33 @@
     <t xml:space="preserve">http://di</t>
   </si>
   <si>
-    <t xml:space="preserve">Automation-1-0-7-21-12-2021.apk</t>
-  </si>
-  <si>
     <t xml:space="preserve">Android_0003</t>
   </si>
   <si>
-    <t xml:space="preserve">10.0.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">IOS_001</t>
   </si>
   <si>
     <t xml:space="preserve">ios</t>
   </si>
   <si>
+    <t xml:space="preserve">13.5.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_02</t>
+  </si>
+  <si>
     <t xml:space="preserve">13.3.1</t>
   </si>
   <si>
-    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS_02</t>
-  </si>
-  <si>
     <t xml:space="preserve">APPLE_iPhoneXS_iOS_14.1.0_21d51</t>
   </si>
   <si>
@@ -1312,9 +1293,6 @@
     <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
   </si>
   <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
-  </si>
-  <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
   </si>
   <si>
@@ -1336,19 +1314,13 @@
     <t xml:space="preserve">13.1.3</t>
   </si>
   <si>
-    <t xml:space="preserve">13.5.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">APPLE_iPhoneX_iOS_13.3.1_90703</t>
   </si>
   <si>
     <t xml:space="preserve">APPLE_iPhoneX_iOS_14.0.0_1b718</t>
   </si>
   <si>
-    <t xml:space="preserve">APPLE_iPhone7plus_iOS_13.3.1_ce483</t>
-  </si>
-  <si>
-    <t>null</t>
+    <t>https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
   </si>
 </sst>
 </file>
@@ -1362,7 +1334,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1444,6 +1416,12 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1535,7 +1513,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1652,7 +1630,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1660,7 +1642,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20618,11 +20600,11 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20831,9 +20813,9 @@
         <v>399</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="M4" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="M4" s="30" t="s">
         <v>401</v>
       </c>
       <c r="N4" s="23" t="s">
@@ -20849,12 +20831,12 @@
       <c r="R4" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S4" s="30" t="b">
+      <c r="S4" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>404</v>
       </c>
@@ -20877,10 +20859,10 @@
         <v>383</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="I5" s="29" t="s">
-        <v>397</v>
+        <v>405</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>406</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>398</v>
@@ -20889,9 +20871,9 @@
         <v>399</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>405</v>
-      </c>
-      <c r="M5" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="M5" s="30" t="s">
         <v>401</v>
       </c>
       <c r="N5" s="23" t="s">
@@ -20907,14 +20889,14 @@
       <c r="R5" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S5" s="30" t="b">
+      <c r="S5" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>44</v>
@@ -20938,19 +20920,17 @@
         <v>396</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>399</v>
-      </c>
+      <c r="K6"/>
       <c r="L6" s="11" t="s">
-        <v>408</v>
-      </c>
-      <c r="M6" s="31" t="s">
         <v>409</v>
+      </c>
+      <c r="M6" s="30" t="s">
+        <v>401</v>
       </c>
       <c r="N6" s="23" t="s">
         <v>402</v>
@@ -20965,7 +20945,7 @@
       <c r="R6" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S6" s="30" t="b">
+      <c r="S6" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20993,20 +20973,18 @@
         <v>383</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>411</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>407</v>
+        <v>396</v>
+      </c>
+      <c r="I7" s="32" t="s">
+        <v>397</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="K7" s="8" t="s">
-        <v>399</v>
-      </c>
+      <c r="K7"/>
       <c r="L7"/>
-      <c r="M7" s="31" t="s">
-        <v>409</v>
+      <c r="M7" s="30" t="s">
+        <v>401</v>
       </c>
       <c r="N7" s="23" t="s">
         <v>386</v>
@@ -21021,14 +20999,14 @@
       <c r="R7" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S7" s="30" t="b">
+      <c r="S7" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>44</v>
@@ -21036,8 +21014,8 @@
       <c r="C8" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="D8" s="32" t="s">
-        <v>413</v>
+      <c r="D8" s="33" t="s">
+        <v>412</v>
       </c>
       <c r="E8" s="28" t="s">
         <v>394</v>
@@ -21048,21 +21026,19 @@
       <c r="G8" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="33" t="s">
+        <v>413</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="32" t="s">
         <v>415</v>
       </c>
-      <c r="J8" s="29" t="s">
+      <c r="K8" s="32" t="s">
         <v>416</v>
       </c>
-      <c r="K8" s="29" t="s">
-        <v>417</v>
-      </c>
-      <c r="L8" t="s">
-        <v>435</v>
-      </c>
+      <c r="L8"/>
       <c r="M8"/>
       <c r="N8"/>
       <c r="O8"/>
@@ -21073,14 +21049,14 @@
       <c r="R8" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S8" s="30" t="b">
+      <c r="S8" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>44</v>
@@ -21089,7 +21065,7 @@
         <v>392</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E9" s="28" t="s">
         <v>394</v>
@@ -21097,20 +21073,20 @@
       <c r="F9" s="28" t="s">
         <v>395</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="G9" s="33" t="s">
         <v>383</v>
       </c>
-      <c r="H9" s="32" t="s">
-        <v>414</v>
+      <c r="H9" s="33" t="s">
+        <v>418</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="J9" s="29" t="s">
+      <c r="J9" s="32" t="s">
+        <v>415</v>
+      </c>
+      <c r="K9" s="34" t="s">
         <v>416</v>
-      </c>
-      <c r="K9" s="33" t="s">
-        <v>417</v>
       </c>
       <c r="L9"/>
       <c r="M9"/>
@@ -21123,7 +21099,7 @@
       <c r="R9" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S9" s="30" t="b">
+      <c r="S9" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21133,7 +21109,7 @@
     <hyperlink ref="R2" r:id="rId1" display="http://127.0.0.1:4723/wd/hub"/>
     <hyperlink ref="R3" r:id="rId2" display="http://127.0.0.1:4723/wd/hub"/>
     <hyperlink ref="E4" r:id="rId3" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="L4" r:id="rId4" display="http://20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.8-31-12-2021-14:16.apk"/>
+    <hyperlink ref="L4" r:id="rId4" display="https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk"/>
     <hyperlink ref="R4" r:id="rId5" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E5" r:id="rId6" display="sriganesh.d@i-exceed.com"/>
     <hyperlink ref="R5" r:id="rId7" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
@@ -21162,10 +21138,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4:F29"/>
+  <dimension ref="B4:F28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21175,62 +21151,62 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="35" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="35" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="35" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="35" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="35" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="35" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="35" t="s">
         <v>423</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="34" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="34" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -21239,43 +21215,38 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>429</v>
       </c>
-      <c r="F24" s="0" t="s">
-        <v>430</v>
-      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="35" t="s">
-        <v>415</v>
-      </c>
-      <c r="F25" s="35" t="s">
-        <v>431</v>
+      <c r="B25" s="36" t="s">
+        <v>414</v>
+      </c>
+      <c r="F25" s="36" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
         <v>419</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
-        <v>434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating legal entity tyne and name feature file and class
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2750" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2779" uniqueCount="435">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -21004,7 +21004,7 @@
         <v>401</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>402</v>
+        <v>434</v>
       </c>
       <c r="M4" s="11" t="s">
         <v>403</v>

</xml_diff>

<commit_message>
updating Gson load error
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3415" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3418" uniqueCount="559">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -2042,6 +2042,9 @@
   </si>
   <si>
     <t xml:space="preserve">APPLE_iPhoneX_iOS_14.0.0_1b718</t>
+  </si>
+  <si>
+    <t>https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
   </si>
 </sst>
 </file>
@@ -2460,56 +2463,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="0" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="12.85" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
+    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
+    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
+    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
+    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
+    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
+    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
+    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
+    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
+    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
+    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
+    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
+    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
+    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
+    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="991" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23661,22 +23664,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="5.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="18" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="18" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="18" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="18" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="18" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="18" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="18" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="18" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="18" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="18" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="18" width="26.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="18" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="18" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="18" width="9.17"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="18" width="12.57" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="18" width="5.18" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="4" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="18" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="18" width="20.5" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="18" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="18" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="18" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="13" customWidth="true" hidden="false" style="18" width="14.87" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="18" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="18" width="26.35" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="17" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="18" width="29.45" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="1025" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23751,21 +23754,28 @@
       <c r="D2" s="22" t="s">
         <v>508</v>
       </c>
+      <c r="E2"/>
+      <c r="F2"/>
       <c r="G2" s="22" t="s">
         <v>509</v>
       </c>
+      <c r="H2"/>
       <c r="I2" s="22" t="s">
         <v>510</v>
       </c>
       <c r="J2" s="23" t="s">
         <v>511</v>
       </c>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
       <c r="N2" s="24" t="s">
         <v>512</v>
       </c>
       <c r="O2" s="11" t="s">
         <v>513</v>
       </c>
+      <c r="P2"/>
       <c r="Q2" s="23" t="n">
         <v>500</v>
       </c>
@@ -23789,28 +23799,35 @@
       <c r="D3" s="21" t="s">
         <v>508</v>
       </c>
+      <c r="E3"/>
+      <c r="F3"/>
       <c r="G3" s="21" t="s">
         <v>509</v>
       </c>
+      <c r="H3"/>
       <c r="I3" s="26" t="s">
         <v>516</v>
       </c>
       <c r="J3" s="26" t="s">
         <v>511</v>
       </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
       <c r="N3" s="24" t="s">
         <v>512</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>513</v>
       </c>
+      <c r="P3"/>
       <c r="Q3" s="21" t="n">
         <v>103</v>
       </c>
       <c r="R3" s="26" t="s">
         <v>514</v>
       </c>
-      <c r="S3" s="27" t="n">
+      <c r="S3" s="27" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23851,7 +23868,7 @@
         <v>525</v>
       </c>
       <c r="L4" s="18" t="s">
-        <v>526</v>
+        <v>558</v>
       </c>
       <c r="M4" s="11" t="s">
         <v>527</v>
@@ -23862,13 +23879,14 @@
       <c r="O4" s="11" t="s">
         <v>513</v>
       </c>
+      <c r="P4"/>
       <c r="Q4" s="21" t="n">
         <v>306</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>529</v>
       </c>
-      <c r="S4" s="31" t="n">
+      <c r="S4" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23919,13 +23937,14 @@
       <c r="O5" s="11" t="s">
         <v>513</v>
       </c>
+      <c r="P5"/>
       <c r="Q5" s="21" t="n">
         <v>307</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>529</v>
       </c>
-      <c r="S5" s="31" t="n">
+      <c r="S5" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23961,6 +23980,7 @@
       <c r="J6" s="8" t="s">
         <v>524</v>
       </c>
+      <c r="K6"/>
       <c r="L6" s="11" t="s">
         <v>535</v>
       </c>
@@ -23973,13 +23993,14 @@
       <c r="O6" s="11" t="s">
         <v>513</v>
       </c>
+      <c r="P6"/>
       <c r="Q6" s="21" t="n">
         <v>106</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>529</v>
       </c>
-      <c r="S6" s="31" t="n">
+      <c r="S6" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24015,6 +24036,8 @@
       <c r="J7" s="8" t="s">
         <v>524</v>
       </c>
+      <c r="K7"/>
+      <c r="L7"/>
       <c r="M7" s="11" t="s">
         <v>527</v>
       </c>
@@ -24024,13 +24047,14 @@
       <c r="O7" s="11" t="s">
         <v>513</v>
       </c>
+      <c r="P7"/>
       <c r="Q7" s="21" t="n">
         <v>306</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>529</v>
       </c>
-      <c r="S7" s="31" t="n">
+      <c r="S7" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24069,13 +24093,18 @@
       <c r="K8" s="30" t="s">
         <v>542</v>
       </c>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
       <c r="Q8" s="1" t="n">
         <v>500</v>
       </c>
       <c r="R8" s="8" t="s">
         <v>529</v>
       </c>
-      <c r="S8" s="31" t="n">
+      <c r="S8" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24114,13 +24143,18 @@
       <c r="K9" s="33" t="s">
         <v>542</v>
       </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
       <c r="Q9" s="1" t="n">
         <v>501</v>
       </c>
       <c r="R9" s="8" t="s">
         <v>529</v>
       </c>
-      <c r="S9" s="31" t="n">
+      <c r="S9" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24167,7 +24201,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
+    <col min="1" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updating feature file legal entity name and type
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4227" uniqueCount="703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4228" uniqueCount="704">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -2045,22 +2045,25 @@
     <t xml:space="preserve">14.6.0</t>
   </si>
   <si>
+    <t xml:space="preserve">APPLE_iPad7_iOS_14.0.1_7de055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://us.pcloudy.com/appiumcloud/wd/hub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.7.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">APPLE_iPad_iOS_13.7.0_c08f6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://us.pcloudy.com/appiumcloud/wd/hub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.7.0</t>
   </si>
   <si>
     <t xml:space="preserve">14.4.2</t>
@@ -2165,6 +2168,7 @@
         <color rgb="FF000000"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">listIOS</t>
     </r>
@@ -2174,6 +2178,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.add(</t>
     </r>
@@ -2183,6 +2188,7 @@
         <color rgb="FF067D17"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"APPLE_iPad9.7_iOS_14.4.0_a1d17"</t>
     </r>
@@ -2192,6 +2198,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">);</t>
     </r>
@@ -2206,6 +2213,7 @@
         <color rgb="FF000000"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">listIOS</t>
     </r>
@@ -2215,6 +2223,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.add(</t>
     </r>
@@ -2224,6 +2233,7 @@
         <color rgb="FF067D17"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"APPLE_iPad9.7_iOS_14.3.0_a13e3"</t>
     </r>
@@ -2233,6 +2243,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">);
 </t>
@@ -2243,6 +2254,7 @@
         <color rgb="FF000000"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">listIOS</t>
     </r>
@@ -2252,6 +2264,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.add(</t>
     </r>
@@ -2261,6 +2274,7 @@
         <color rgb="FF067D17"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"APPLE_iPad8thGen_iOS_14.4.2_d5dd0"</t>
     </r>
@@ -2270,6 +2284,7 @@
         <color rgb="FF080808"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">);</t>
     </r>
@@ -2290,7 +2305,7 @@
     <numFmt numFmtId="168" formatCode="&quot;+91&quot;"/>
     <numFmt numFmtId="169" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2381,28 +2396,24 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="10"/>
+      <color rgb="FF067D17"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF080808"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF067D17"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2487,7 +2498,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2616,16 +2627,12 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2727,7 +2734,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -25999,10 +26006,10 @@
   </sheetPr>
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
       <selection pane="bottomRight" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
@@ -26423,13 +26430,13 @@
       <c r="F8" s="28" t="s">
         <v>641</v>
       </c>
-      <c r="G8" s="32" t="s">
+      <c r="G8" s="8" t="s">
         <v>659</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="H8" s="32" t="s">
         <v>660</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="33" t="s">
         <v>661</v>
       </c>
       <c r="J8" s="29" t="s">
@@ -26439,7 +26446,7 @@
         <v>663</v>
       </c>
       <c r="L8" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="M8"/>
       <c r="N8"/>
@@ -26475,19 +26482,19 @@
       <c r="F9" s="28" t="s">
         <v>641</v>
       </c>
-      <c r="G9" s="34" t="s">
+      <c r="G9" s="31" t="s">
         <v>659</v>
       </c>
-      <c r="H9" s="33" t="s">
+      <c r="H9" s="32" t="s">
         <v>666</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>661</v>
+        <v>667</v>
       </c>
       <c r="J9" s="29" t="s">
         <v>662</v>
       </c>
-      <c r="K9" s="35" t="s">
+      <c r="K9" s="34" t="s">
         <v>663</v>
       </c>
       <c r="L9"/>
@@ -26514,11 +26521,11 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10"/>
-      <c r="H10" s="33" t="s">
-        <v>667</v>
+      <c r="H10" s="32" t="s">
+        <v>668</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="J10" s="29" t="s">
         <v>662</v>
@@ -26632,8 +26639,8 @@
   </sheetPr>
   <dimension ref="B4:G46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F46" activeCellId="0" sqref="F46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26645,32 +26652,32 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>643</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="36" t="s">
-        <v>670</v>
+      <c r="B6" s="35" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="35" t="s">
         <v>643</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="36" t="s">
-        <v>671</v>
+      <c r="B8" s="35" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="36" t="s">
-        <v>672</v>
+      <c r="B9" s="35" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26679,28 +26686,28 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="36" t="s">
-        <v>671</v>
+      <c r="B11" s="35" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="36" t="s">
-        <v>673</v>
+      <c r="B13" s="35" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -26709,139 +26716,139 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="37" t="s">
-        <v>680</v>
-      </c>
-      <c r="F25" s="37" t="s">
+      <c r="B25" s="36" t="s">
         <v>681</v>
+      </c>
+      <c r="F25" s="36" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="9" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="37" t="s">
-        <v>688</v>
+      <c r="B32" s="36" t="s">
+        <v>689</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>690</v>
       </c>
-      <c r="E33" s="0" t="s">
-        <v>689</v>
-      </c>
       <c r="F33" s="0" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
+        <v>693</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F34" s="0" t="s">
         <v>692</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>689</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="37" t="s">
-        <v>697</v>
+      <c r="B44" s="36" t="s">
+        <v>698</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="38" t="s">
-        <v>699</v>
+      <c r="B45" s="37" t="s">
+        <v>700</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="39" t="s">
-        <v>701</v>
+      <c r="B46" s="38" t="s">
+        <v>702</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified entity type class methods
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4228" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4238" uniqueCount="704">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -2045,7 +2045,7 @@
     <t xml:space="preserve">14.6.0</t>
   </si>
   <si>
-    <t xml:space="preserve">APPLE_iPad7_iOS_14.0.1_7de055</t>
+    <t xml:space="preserve">APPLE_iPadPro3_iOS_14.7.1_c7375</t>
   </si>
   <si>
     <t xml:space="preserve">XCUITest</t>
@@ -2133,9 +2133,6 @@
   </si>
   <si>
     <t xml:space="preserve">us</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPadPro3_iOS_14.7.1_c7375</t>
   </si>
   <si>
     <t xml:space="preserve">add</t>
@@ -2291,6 +2288,9 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.11-13-01-2022-15:16.apk</t>
   </si>
 </sst>
 </file>
@@ -26220,7 +26220,7 @@
         <v>645</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>646</v>
+        <v>703</v>
       </c>
       <c r="M4" s="11" t="s">
         <v>647</v>
@@ -26446,7 +26446,7 @@
         <v>663</v>
       </c>
       <c r="L8" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="M8"/>
       <c r="N8"/>
@@ -26773,43 +26773,43 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>691</v>
+        <v>661</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>690</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>690</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>690</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>690</v>
@@ -26823,32 +26823,32 @@
         <v>690</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="36" t="s">
+        <v>697</v>
+      </c>
+      <c r="E44" s="0" t="s">
         <v>698</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="37" t="s">
+        <v>699</v>
+      </c>
+      <c r="F45" s="0" t="s">
         <v>700</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="38" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
business loction page object creation
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4238" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4229" uniqueCount="703">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -2285,9 +2285,6 @@
       </rPr>
       <t xml:space="preserve">);</t>
     </r>
-  </si>
-  <si>
-    <t>null</t>
   </si>
   <si>
     <t>https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.11-13-01-2022-15:16.apk</t>
@@ -2734,10 +2731,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topRight" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26006,12 +26003,12 @@
   </sheetPr>
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="M6" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="bottomRight" activeCell="R8" activeCellId="0" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26220,7 +26217,7 @@
         <v>645</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="M4" s="11" t="s">
         <v>647</v>
@@ -26445,9 +26442,7 @@
       <c r="K8" s="29" t="s">
         <v>663</v>
       </c>
-      <c r="L8" t="s">
-        <v>702</v>
-      </c>
+      <c r="L8"/>
       <c r="M8"/>
       <c r="N8"/>
       <c r="O8"/>

</xml_diff>

<commit_message>
updating entity name and type objects,features
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2281" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2274" uniqueCount="501">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1236,6 +1236,18 @@
     <t xml:space="preserve">TestCase_166</t>
   </si>
   <si>
+    <t xml:space="preserve">TestCase_167</t>
+  </si>
+  <si>
+    <t xml:space="preserve">english</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arabic</t>
+  </si>
+  <si>
     <t xml:space="preserve">mode</t>
   </si>
   <si>
@@ -1347,7 +1359,7 @@
     <t xml:space="preserve">http://readuser:Re@d@1234@20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.5-06-12-2021-19:31.apk</t>
   </si>
   <si>
-    <t xml:space="preserve">https://artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.15-21-01-2022-14:05.apk</t>
+    <t xml:space="preserve">https://artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.16-27-01-2022-10:18.apk</t>
   </si>
   <si>
     <t xml:space="preserve">Automation-1-0-16-27-01-2022.apk</t>
@@ -1633,9 +1645,6 @@
       <t xml:space="preserve">);</t>
     </r>
   </si>
-  <si>
-    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.16-27-01-2022-10:18.apk</t>
-  </si>
 </sst>
 </file>
 
@@ -1649,7 +1658,7 @@
     <numFmt numFmtId="168" formatCode="&quot;+91&quot;"/>
     <numFmt numFmtId="169" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1694,12 +1703,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1835,7 +1838,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1904,19 +1907,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1936,11 +1935,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1952,11 +1951,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1972,11 +1971,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1984,11 +1983,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2071,64 +2070,64 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A165" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B165" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A165" activeCellId="0" sqref="A165"/>
-      <selection pane="topRight" activeCell="G166" activeCellId="0" sqref="G166"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A121" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B121" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A121" activeCellId="0" sqref="A121"/>
+      <selection pane="topRight" activeCell="A124" activeCellId="0" sqref="A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="12.85" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
-    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
-    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
-    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
-    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
-    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
-    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
-    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
-    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
-    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
-    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
-    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
-    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
-    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
-    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
-    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="991" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13565,7 +13564,7 @@
         <v>40</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="G124" s="1" t="n">
         <v>100</v>
@@ -16416,7 +16415,7 @@
       <c r="C167" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E167" s="17" t="s">
+      <c r="E167" s="8" t="s">
         <v>32</v>
       </c>
       <c r="F167" s="1" t="s">
@@ -16425,7 +16424,7 @@
       <c r="G167" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="H167" s="17" t="s">
+      <c r="H167" s="8" t="s">
         <v>398</v>
       </c>
       <c r="I167" s="8" t="s">
@@ -16496,7 +16495,7 @@
       <c r="G168" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="H168" s="17" t="s">
+      <c r="H168" s="8" t="s">
         <v>398</v>
       </c>
       <c r="I168" s="8" t="s">
@@ -16558,7 +16557,7 @@
       <c r="C169" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E169" s="17" t="s">
+      <c r="E169" s="8" t="s">
         <v>32</v>
       </c>
       <c r="F169" s="1" t="s">
@@ -16567,7 +16566,7 @@
       <c r="G169" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="H169" s="17" t="s">
+      <c r="H169" s="8" t="s">
         <v>398</v>
       </c>
       <c r="I169" s="8" t="s">
@@ -16619,7 +16618,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
         <v>402</v>
       </c>
@@ -16638,7 +16637,7 @@
       <c r="G170" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="H170" s="17" t="s">
+      <c r="H170" s="8" t="s">
         <v>398</v>
       </c>
       <c r="I170" s="8" t="s">
@@ -16689,6 +16688,88 @@
       <c r="AB170" s="16" t="n">
         <v>12</v>
       </c>
+    </row>
+    <row r="171" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B171" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="C171" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E171" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G171" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H171" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I171" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J171" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="K171" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="M171" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N171" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="U171" s="1"/>
+      <c r="V171" s="1"/>
+      <c r="AN171" s="1"/>
+      <c r="AO171" s="1"/>
+    </row>
+    <row r="172" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="B172" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="C172" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E172" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G172" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H172" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I172" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J172" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="K172" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="M172" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N172" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="R172" s="8"/>
+      <c r="T172" s="8"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -16747,6 +16828,8 @@
     <hyperlink ref="I168" r:id="rId52" display="parkjimin@gmail.com"/>
     <hyperlink ref="I169" r:id="rId53" display="parkjimin@gmail.com"/>
     <hyperlink ref="I170" r:id="rId54" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I171" r:id="rId55" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I172" r:id="rId56" display="parkjimin@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -16775,22 +16858,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="18" width="12.57" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="18" width="5.18" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="4" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="18" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="18" width="20.5" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="18" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="18" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="18" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="13" customWidth="true" hidden="false" style="18" width="14.87" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="18" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="18" width="26.35" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="17" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="18" width="29.45" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="1025" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="17" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="17" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="17" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="17" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="17" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="17" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="17" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="17" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="17" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="17" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="17" width="26.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="17" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="17" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="17" width="9.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16801,508 +16884,461 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>405</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>406</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>407</v>
+        <v>409</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>411</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>418</v>
-      </c>
-      <c r="R1" s="20" t="s">
-        <v>419</v>
+        <v>422</v>
+      </c>
+      <c r="R1" s="19" t="s">
+        <v>423</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="s">
-        <v>421</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>422</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>423</v>
-      </c>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2" s="22" t="s">
-        <v>424</v>
-      </c>
-      <c r="H2"/>
-      <c r="I2" s="22" t="s">
+      <c r="A2" s="20" t="s">
         <v>425</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="B2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>426</v>
       </c>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2" s="24" t="s">
+      <c r="D2" s="21" t="s">
         <v>427</v>
       </c>
+      <c r="G2" s="21" t="s">
+        <v>428</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>430</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>431</v>
+      </c>
       <c r="O2" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="Q2" s="22" t="n">
+        <v>500</v>
+      </c>
+      <c r="R2" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="S2" s="22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="20" t="s">
+        <v>434</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>426</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>428</v>
       </c>
-      <c r="P2"/>
-      <c r="Q2" s="23" t="n">
-        <v>500</v>
-      </c>
-      <c r="R2" s="25" t="s">
-        <v>429</v>
-      </c>
-      <c r="S2" s="23" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21" t="s">
+      <c r="I3" s="25" t="s">
+        <v>435</v>
+      </c>
+      <c r="J3" s="25" t="s">
         <v>430</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>422</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>423</v>
-      </c>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3" s="21" t="s">
-        <v>424</v>
-      </c>
-      <c r="H3"/>
-      <c r="I3" s="26" t="s">
+      <c r="N3" s="23" t="s">
         <v>431</v>
       </c>
-      <c r="J3" s="26" t="s">
-        <v>426</v>
-      </c>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3" s="24" t="s">
-        <v>427</v>
-      </c>
       <c r="O3" s="11" t="s">
-        <v>428</v>
-      </c>
-      <c r="P3"/>
-      <c r="Q3" s="23" t="n">
+        <v>432</v>
+      </c>
+      <c r="Q3" s="22" t="n">
         <v>501</v>
       </c>
-      <c r="R3" s="26" t="s">
-        <v>429</v>
-      </c>
-      <c r="S3" s="27" t="b">
+      <c r="R3" s="25" t="s">
+        <v>433</v>
+      </c>
+      <c r="S3" s="26" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="U3" s="28"/>
+      <c r="U3" s="27"/>
     </row>
     <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>439</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>440</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>442</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>445</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>447</v>
+      </c>
+      <c r="O4" s="11" t="s">
         <v>432</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>434</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>435</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>436</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>437</v>
-      </c>
-      <c r="I4" s="30" t="s">
-        <v>438</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>439</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="L4" s="18" t="s">
-        <v>497</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>442</v>
-      </c>
-      <c r="N4" s="24" t="s">
-        <v>443</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>428</v>
-      </c>
-      <c r="P4"/>
-      <c r="Q4" s="23" t="n">
+      <c r="Q4" s="22" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="S4" s="31" t="b">
+        <v>448</v>
+      </c>
+      <c r="S4" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>434</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>435</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>436</v>
+        <v>438</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>439</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>440</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="H5" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>452</v>
+      </c>
+      <c r="M5" s="11" t="s">
         <v>446</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="N5" s="23" t="s">
         <v>447</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>439</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="L5" s="18" t="s">
+      <c r="O5" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="Q5" s="22" t="n">
+        <v>503</v>
+      </c>
+      <c r="R5" s="8" t="s">
         <v>448</v>
       </c>
-      <c r="M5" s="11" t="s">
-        <v>442</v>
-      </c>
-      <c r="N5" s="24" t="s">
-        <v>443</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>428</v>
-      </c>
-      <c r="P5"/>
-      <c r="Q5" s="23" t="n">
-        <v>503</v>
-      </c>
-      <c r="R5" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="S5" s="31" t="b">
+      <c r="S5" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>434</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>435</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>436</v>
+        <v>438</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>439</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>440</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>437</v>
-      </c>
-      <c r="I6" s="30" t="s">
-        <v>438</v>
+        <v>441</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>442</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>439</v>
-      </c>
-      <c r="K6"/>
+        <v>443</v>
+      </c>
       <c r="L6" s="11" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>442</v>
-      </c>
-      <c r="N6" s="24" t="s">
-        <v>443</v>
+        <v>446</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>447</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>428</v>
-      </c>
-      <c r="P6"/>
-      <c r="Q6" s="23" t="n">
+        <v>432</v>
+      </c>
+      <c r="Q6" s="22" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="S6" s="31" t="b">
+        <v>448</v>
+      </c>
+      <c r="S6" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>434</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>435</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>436</v>
+        <v>438</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>439</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>440</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>437</v>
-      </c>
-      <c r="I7" s="30" t="s">
-        <v>438</v>
+        <v>441</v>
+      </c>
+      <c r="I7" s="29" t="s">
+        <v>442</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>439</v>
-      </c>
-      <c r="K7"/>
-      <c r="L7"/>
+        <v>443</v>
+      </c>
       <c r="M7" s="11" t="s">
-        <v>442</v>
-      </c>
-      <c r="N7" s="24" t="s">
-        <v>427</v>
+        <v>446</v>
+      </c>
+      <c r="N7" s="23" t="s">
+        <v>431</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>428</v>
-      </c>
-      <c r="P7"/>
-      <c r="Q7" s="23" t="n">
+        <v>432</v>
+      </c>
+      <c r="Q7" s="22" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="S7" s="31" t="b">
+        <v>448</v>
+      </c>
+      <c r="S7" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>453</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>435</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>436</v>
+        <v>437</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>457</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>439</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>440</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>454</v>
-      </c>
-      <c r="H8" s="33" t="s">
-        <v>455</v>
+        <v>458</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>459</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>456</v>
-      </c>
-      <c r="J8" s="30" t="s">
-        <v>457</v>
-      </c>
-      <c r="K8" s="30" t="s">
-        <v>458</v>
-      </c>
-      <c r="L8"/>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
-      <c r="Q8" s="23" t="n">
+        <v>460</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>461</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>462</v>
+      </c>
+      <c r="Q8" s="22" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>459</v>
-      </c>
-      <c r="S8" s="31" t="b">
+        <v>463</v>
+      </c>
+      <c r="S8" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="s">
-        <v>460</v>
-      </c>
-      <c r="B9" s="18" t="s">
+      <c r="A9" s="17" t="s">
+        <v>464</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>453</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>435</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>436</v>
-      </c>
-      <c r="G9" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="H9" s="33" t="s">
+        <v>437</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>457</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>439</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>440</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>458</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>465</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="J9" s="29" t="s">
         <v>461</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="K9" s="33" t="s">
         <v>462</v>
       </c>
-      <c r="J9" s="30" t="s">
-        <v>457</v>
-      </c>
-      <c r="K9" s="34" t="s">
-        <v>458</v>
-      </c>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
-      <c r="Q9" s="23" t="n">
+      <c r="Q9" s="22" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>459</v>
-      </c>
-      <c r="S9" s="31" t="b">
+        <v>463</v>
+      </c>
+      <c r="S9" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10" s="33" t="s">
-        <v>463</v>
+      <c r="H10" s="32" t="s">
+        <v>467</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>464</v>
-      </c>
-      <c r="J10" s="30" t="s">
-        <v>457</v>
-      </c>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="N10"/>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
+        <v>468</v>
+      </c>
+      <c r="J10" s="29" t="s">
+        <v>461</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="R2" r:id="rId1" display="http://127.0.0.1:4723/wd/hub"/>
     <hyperlink ref="R3" r:id="rId2" display="http://127.0.0.1:4723/wd/hub"/>
     <hyperlink ref="E4" r:id="rId3" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="L4" r:id="rId4" display="https://artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.15-21-01-2022-14:05.apk"/>
+    <hyperlink ref="L4" r:id="rId4" display="https://artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.16-27-01-2022-10:18.apk"/>
     <hyperlink ref="R4" r:id="rId5" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E5" r:id="rId6" display="sriganesh.d@i-exceed.com"/>
     <hyperlink ref="R5" r:id="rId7" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
@@ -17339,69 +17375,69 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="35" t="s">
-        <v>438</v>
+      <c r="B5" s="34" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="35" t="s">
-        <v>466</v>
+      <c r="B6" s="34" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="35" t="s">
-        <v>438</v>
+      <c r="B7" s="34" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="35" t="s">
-        <v>467</v>
+      <c r="B8" s="34" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="35" t="s">
-        <v>468</v>
+      <c r="B9" s="34" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="35" t="s">
-        <v>467</v>
+      <c r="B11" s="34" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="35" t="s">
-        <v>469</v>
+      <c r="B13" s="34" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -17410,139 +17446,139 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="36" t="s">
-        <v>476</v>
-      </c>
-      <c r="F25" s="36" t="s">
-        <v>477</v>
+      <c r="B25" s="35" t="s">
+        <v>480</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="9" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="36" t="s">
-        <v>484</v>
+      <c r="B32" s="35" t="s">
+        <v>488</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="36" t="s">
-        <v>492</v>
+      <c r="B44" s="35" t="s">
+        <v>496</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="37" t="s">
-        <v>494</v>
+      <c r="B45" s="36" t="s">
+        <v>498</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="38" t="s">
-        <v>496</v>
+      <c r="B46" s="37" t="s">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updation ios loginpage feature
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2439" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2276" uniqueCount="502">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1647,9 +1647,6 @@
   </si>
   <si>
     <t>null</t>
-  </si>
-  <si>
-    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.16-27-01-2022-10:18.apk</t>
   </si>
 </sst>
 </file>
@@ -2076,16 +2073,16 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A121" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B121" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A121" activeCellId="0" sqref="A121"/>
-      <selection pane="topRight" activeCell="A124" activeCellId="0" sqref="A124"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="12.85" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="14.33" collapsed="true" outlineLevel="0"/>
     <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
     <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
     <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
@@ -16854,12 +16851,12 @@
   </sheetPr>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17068,7 +17065,7 @@
         <v>444</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>502</v>
+        <v>445</v>
       </c>
       <c r="M4" s="11" t="s">
         <v>446</v>

</xml_diff>

<commit_message>
updating apk url with utilities'
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2284" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2357" uniqueCount="502">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1362,7 +1362,25 @@
     <t xml:space="preserve">https://artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.16-27-01-2022-10:18.apk</t>
   </si>
   <si>
-    <t xml:space="preserve">Automation-1-0-16-27-01-2022.apk</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF067D17"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">Automation-1-0-18-02-02-2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF067D17"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.apk</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
@@ -1646,7 +1664,7 @@
     </r>
   </si>
   <si>
-    <t>null</t>
+    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.18-02-02-2022-14:23.apk</t>
   </si>
 </sst>
 </file>
@@ -1661,7 +1679,7 @@
     <numFmt numFmtId="168" formatCode="&quot;+91&quot;"/>
     <numFmt numFmtId="169" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1742,6 +1760,19 @@
       <color rgb="FF6A8759"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF067D17"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF067D17"/>
+      <name val=""/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1841,7 +1872,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1962,6 +1993,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1986,11 +2021,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2073,7 +2108,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E4" activeCellId="0" sqref="E4"/>
@@ -16851,12 +16886,12 @@
   </sheetPr>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="L5" activeCellId="0" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17030,7 +17065,7 @@
       </c>
       <c r="U3" s="27"/>
     </row>
-    <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>436</v>
       </c>
@@ -17065,9 +17100,9 @@
         <v>444</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>445</v>
-      </c>
-      <c r="M4" s="11" t="s">
+        <v>501</v>
+      </c>
+      <c r="M4" s="30" t="s">
         <v>446</v>
       </c>
       <c r="N4" s="23" t="s">
@@ -17083,12 +17118,12 @@
       <c r="R4" s="8" t="s">
         <v>448</v>
       </c>
-      <c r="S4" s="30" t="b">
+      <c r="S4" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>449</v>
       </c>
@@ -17125,7 +17160,7 @@
       <c r="L5" s="17" t="s">
         <v>452</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="M5" s="30" t="s">
         <v>446</v>
       </c>
       <c r="N5" s="23" t="s">
@@ -17141,7 +17176,7 @@
       <c r="R5" s="8" t="s">
         <v>448</v>
       </c>
-      <c r="S5" s="30" t="b">
+      <c r="S5" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17181,7 +17216,7 @@
       <c r="L6" s="11" t="s">
         <v>454</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="M6" s="30" t="s">
         <v>446</v>
       </c>
       <c r="N6" s="23" t="s">
@@ -17197,7 +17232,7 @@
       <c r="R6" s="8" t="s">
         <v>448</v>
       </c>
-      <c r="S6" s="30" t="b">
+      <c r="S6" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17235,7 +17270,7 @@
       </c>
       <c r="K7"/>
       <c r="L7"/>
-      <c r="M7" s="11" t="s">
+      <c r="M7" s="30" t="s">
         <v>446</v>
       </c>
       <c r="N7" s="23" t="s">
@@ -17251,7 +17286,7 @@
       <c r="R7" s="8" t="s">
         <v>448</v>
       </c>
-      <c r="S7" s="30" t="b">
+      <c r="S7" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17266,7 +17301,7 @@
       <c r="C8" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="32" t="s">
         <v>457</v>
       </c>
       <c r="E8" s="28" t="s">
@@ -17278,7 +17313,7 @@
       <c r="G8" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="33" t="s">
         <v>458</v>
       </c>
       <c r="I8" s="11" t="s">
@@ -17291,7 +17326,7 @@
         <v>461</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>501</v>
+        <v>462</v>
       </c>
       <c r="M8"/>
       <c r="N8"/>
@@ -17303,7 +17338,7 @@
       <c r="R8" s="8" t="s">
         <v>463</v>
       </c>
-      <c r="S8" s="30" t="b">
+      <c r="S8" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17330,7 +17365,7 @@
       <c r="G9" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="33" t="s">
         <v>465</v>
       </c>
       <c r="I9" s="8" t="s">
@@ -17339,7 +17374,7 @@
       <c r="J9" s="29" t="s">
         <v>460</v>
       </c>
-      <c r="K9" s="33" t="s">
+      <c r="K9" s="34" t="s">
         <v>461</v>
       </c>
       <c r="L9"/>
@@ -17353,7 +17388,7 @@
       <c r="R9" s="8" t="s">
         <v>463</v>
       </c>
-      <c r="S9" s="30" t="b">
+      <c r="S9" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17366,7 +17401,7 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10"/>
-      <c r="H10" s="32" t="s">
+      <c r="H10" s="33" t="s">
         <v>467</v>
       </c>
       <c r="I10" s="8" t="s">
@@ -17438,27 +17473,27 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="35" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="35" t="s">
         <v>470</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="35" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="35" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="35" t="s">
         <v>472</v>
       </c>
     </row>
@@ -17468,12 +17503,12 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="35" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="35" t="s">
         <v>473</v>
       </c>
     </row>
@@ -17510,10 +17545,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="36" t="s">
         <v>480</v>
       </c>
-      <c r="F25" s="35" t="s">
+      <c r="F25" s="36" t="s">
         <v>481</v>
       </c>
     </row>
@@ -17546,7 +17581,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="36" t="s">
         <v>488</v>
       </c>
       <c r="E32" s="0" t="s">
@@ -17613,7 +17648,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="36" t="s">
         <v>496</v>
       </c>
       <c r="E44" s="0" t="s">
@@ -17621,7 +17656,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="36" t="s">
+      <c r="B45" s="37" t="s">
         <v>498</v>
       </c>
       <c r="F45" s="0" t="s">
@@ -17629,7 +17664,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="37" t="s">
+      <c r="B46" s="38" t="s">
         <v>500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating entity contact feature
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -2147,10 +2147,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A80" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B80" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
-      <selection pane="topRight" activeCell="E84" activeCellId="0" sqref="E84"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B7" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topRight" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17309,10 +17309,10 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="L5" activeCellId="0" sqref="L5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
made changes in business object
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2386" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2440" uniqueCount="521">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1701,6 +1701,9 @@
       </rPr>
       <t xml:space="preserve">);</t>
     </r>
+  </si>
+  <si>
+    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.19-02-02-2022-21:16.apk</t>
   </si>
 </sst>
 </file>
@@ -2155,56 +2158,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="0" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="14.33" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
+    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
+    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
+    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
+    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
+    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
+    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
+    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
+    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
+    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
+    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
+    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
+    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
+    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
+    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="991" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17318,22 +17321,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="5.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="17" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="17" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="17" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="17" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="17" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="17" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="17" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="17" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="17" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="17" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="17" width="26.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="17" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="17" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="17" width="9.17"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="17" width="12.57" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="17" width="5.18" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="4" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="17" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="17" width="20.5" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="17" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="17" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="17" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="13" customWidth="true" hidden="false" style="17" width="14.87" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="17" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="17" width="26.35" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="17" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="17" width="29.45" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="1025" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17408,21 +17411,28 @@
       <c r="D2" s="21" t="s">
         <v>447</v>
       </c>
+      <c r="E2"/>
+      <c r="F2"/>
       <c r="G2" s="21" t="s">
         <v>448</v>
       </c>
+      <c r="H2"/>
       <c r="I2" s="21" t="s">
         <v>449</v>
       </c>
       <c r="J2" s="22" t="s">
         <v>450</v>
       </c>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
       <c r="N2" s="23" t="s">
         <v>451</v>
       </c>
       <c r="O2" s="11" t="s">
         <v>452</v>
       </c>
+      <c r="P2"/>
       <c r="Q2" s="22" t="n">
         <v>500</v>
       </c>
@@ -17446,28 +17456,35 @@
       <c r="D3" s="20" t="s">
         <v>447</v>
       </c>
+      <c r="E3"/>
+      <c r="F3"/>
       <c r="G3" s="20" t="s">
         <v>448</v>
       </c>
+      <c r="H3"/>
       <c r="I3" s="25" t="s">
         <v>455</v>
       </c>
       <c r="J3" s="25" t="s">
         <v>450</v>
       </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
       <c r="N3" s="23" t="s">
         <v>451</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>452</v>
       </c>
+      <c r="P3"/>
       <c r="Q3" s="22" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="25" t="s">
         <v>453</v>
       </c>
-      <c r="S3" s="26" t="n">
+      <c r="S3" s="26" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17508,7 +17525,7 @@
         <v>464</v>
       </c>
       <c r="L4" s="30" t="s">
-        <v>465</v>
+        <v>520</v>
       </c>
       <c r="M4" s="31" t="s">
         <v>466</v>
@@ -17519,13 +17536,14 @@
       <c r="O4" s="11" t="s">
         <v>452</v>
       </c>
+      <c r="P4"/>
       <c r="Q4" s="22" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>468</v>
       </c>
-      <c r="S4" s="32" t="n">
+      <c r="S4" s="32" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17576,13 +17594,14 @@
       <c r="O5" s="11" t="s">
         <v>452</v>
       </c>
+      <c r="P5"/>
       <c r="Q5" s="22" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>468</v>
       </c>
-      <c r="S5" s="32" t="n">
+      <c r="S5" s="32" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17618,6 +17637,7 @@
       <c r="J6" s="8" t="s">
         <v>463</v>
       </c>
+      <c r="K6"/>
       <c r="L6" s="11" t="s">
         <v>473</v>
       </c>
@@ -17630,13 +17650,14 @@
       <c r="O6" s="11" t="s">
         <v>452</v>
       </c>
+      <c r="P6"/>
       <c r="Q6" s="22" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>468</v>
       </c>
-      <c r="S6" s="32" t="n">
+      <c r="S6" s="32" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17672,6 +17693,8 @@
       <c r="J7" s="8" t="s">
         <v>463</v>
       </c>
+      <c r="K7"/>
+      <c r="L7"/>
       <c r="M7" s="31" t="s">
         <v>466</v>
       </c>
@@ -17681,13 +17704,14 @@
       <c r="O7" s="11" t="s">
         <v>452</v>
       </c>
+      <c r="P7"/>
       <c r="Q7" s="22" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>468</v>
       </c>
-      <c r="S7" s="32" t="n">
+      <c r="S7" s="32" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17729,13 +17753,17 @@
       <c r="L8" s="17" t="s">
         <v>481</v>
       </c>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
       <c r="Q8" s="22" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="8" t="s">
         <v>482</v>
       </c>
-      <c r="S8" s="32" t="n">
+      <c r="S8" s="32" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17774,18 +17802,30 @@
       <c r="K9" s="35" t="s">
         <v>480</v>
       </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
       <c r="Q9" s="22" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="8" t="s">
         <v>482</v>
       </c>
-      <c r="S9" s="32" t="n">
+      <c r="S9" s="32" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
       <c r="H10" s="34" t="s">
         <v>486</v>
       </c>
@@ -17795,6 +17835,15 @@
       <c r="J10" s="29" t="s">
         <v>479</v>
       </c>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -17839,9 +17888,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updating ios user details screen
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2467" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2389" uniqueCount="520">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1287,9 +1287,6 @@
     <t xml:space="preserve">TestCase_170</t>
   </si>
   <si>
-    <t xml:space="preserve">Primary</t>
-  </si>
-  <si>
     <t xml:space="preserve">Agriculture, forestry and fishing</t>
   </si>
   <si>
@@ -1422,7 +1419,25 @@
     <t xml:space="preserve">https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.19-02-02-2022-21:16.apk</t>
   </si>
   <si>
-    <t xml:space="preserve">Automation-1-0-19-02-02-2022.apk</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF067D17"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">Automation-1-0-20-02-02-2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF067D17"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.apk</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
@@ -1705,9 +1720,6 @@
   <si>
     <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.19-02-02-2022-21:16.apk</t>
   </si>
-  <si>
-    <t>null</t>
-  </si>
 </sst>
 </file>
 
@@ -1721,7 +1733,7 @@
     <numFmt numFmtId="168" formatCode="&quot;+91&quot;"/>
     <numFmt numFmtId="169" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1809,12 +1821,20 @@
       <color rgb="FF067D17"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF067D17"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF067D17"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2066,11 +2086,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2153,10 +2173,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A172" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B172" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A172" activeCellId="0" sqref="A172"/>
-      <selection pane="topRight" activeCell="B175" activeCellId="0" sqref="B175"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A105" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="I105" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A105" activeCellId="0" sqref="A105"/>
+      <selection pane="topRight" activeCell="I107" activeCellId="0" sqref="I107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17046,19 +17066,19 @@
         <v>12</v>
       </c>
       <c r="AC174" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="AD174" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="AD174" s="1" t="s">
+      <c r="AE174" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="AE174" s="1" t="s">
+      <c r="AF174" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="AF174" s="1" t="s">
+      <c r="AG174" s="1" t="s">
         <v>424</v>
-      </c>
-      <c r="AG174" s="1" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17066,7 +17086,7 @@
         <v>413</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C175" s="8" t="s">
         <v>35</v>
@@ -17152,7 +17172,7 @@
         <v>413</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C176" s="8" t="s">
         <v>35</v>
@@ -17218,19 +17238,19 @@
         <v>12</v>
       </c>
       <c r="AC176" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="AD176" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="AD176" s="1" t="s">
+      <c r="AE176" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="AE176" s="1" t="s">
+      <c r="AF176" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="AF176" s="1" t="s">
+      <c r="AG176" s="1" t="s">
         <v>424</v>
-      </c>
-      <c r="AG176" s="1" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -17314,11 +17334,11 @@
   </sheetPr>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
       <selection pane="bottomRight" activeCell="L5" activeCellId="0" sqref="L5"/>
     </sheetView>
   </sheetViews>
@@ -17350,97 +17370,97 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="18" t="s">
         <v>429</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>430</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="19" t="s">
         <v>442</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="S1" s="4" t="s">
         <v>443</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
+        <v>444</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>445</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="21" t="s">
+      <c r="D2" s="21" t="s">
         <v>446</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>447</v>
       </c>
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2" s="21" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="H2"/>
       <c r="I2" s="21" t="s">
+        <v>448</v>
+      </c>
+      <c r="J2" s="22" t="s">
         <v>449</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>450</v>
       </c>
       <c r="K2"/>
       <c r="L2"/>
       <c r="M2"/>
       <c r="N2" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="O2" s="11" t="s">
         <v>451</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>452</v>
       </c>
       <c r="P2"/>
       <c r="Q2" s="22" t="n">
         <v>500</v>
       </c>
       <c r="R2" s="24" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="S2" s="22" t="n">
         <v>0</v>
@@ -17448,44 +17468,44 @@
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B3" s="20" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="20" t="s">
+        <v>445</v>
+      </c>
+      <c r="D3" s="20" t="s">
         <v>446</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>447</v>
       </c>
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" s="20" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="H3"/>
       <c r="I3" s="25" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J3" s="25" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="K3"/>
       <c r="L3"/>
       <c r="M3"/>
       <c r="N3" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="O3" s="11" t="s">
         <v>451</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>452</v>
       </c>
       <c r="P3"/>
       <c r="Q3" s="22" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="25" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="S3" s="26" t="b">
         <f aca="false">FALSE()</f>
@@ -17495,56 +17515,56 @@
     </row>
     <row r="4" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="8" t="s">
         <v>457</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="28" t="s">
         <v>458</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="F4" s="28" t="s">
         <v>459</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="G4" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>460</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="29" t="s">
         <v>461</v>
       </c>
-      <c r="I4" s="29" t="s">
+      <c r="J4" s="8" t="s">
         <v>462</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>463</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>464</v>
-      </c>
       <c r="L4" s="30" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="M4" s="31" t="s">
+        <v>465</v>
+      </c>
+      <c r="N4" s="23" t="s">
         <v>466</v>
       </c>
-      <c r="N4" s="23" t="s">
-        <v>467</v>
-      </c>
       <c r="O4" s="11" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="P4"/>
       <c r="Q4" s="22" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="S4" s="32" t="b">
         <f aca="false">FALSE()</f>
@@ -17553,56 +17573,56 @@
     </row>
     <row r="5" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>458</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>459</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>469</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>458</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>459</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>460</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="H5" s="8" t="s">
+      <c r="I5" s="8" t="s">
         <v>470</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>471</v>
-      </c>
       <c r="J5" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>463</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="L5" s="17" t="s">
         <v>464</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="M5" s="31" t="s">
         <v>465</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="N5" s="23" t="s">
         <v>466</v>
       </c>
-      <c r="N5" s="23" t="s">
-        <v>467</v>
-      </c>
       <c r="O5" s="11" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="P5"/>
       <c r="Q5" s="22" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="S5" s="32" t="b">
         <f aca="false">FALSE()</f>
@@ -17611,54 +17631,54 @@
     </row>
     <row r="6" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>457</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="28" t="s">
         <v>458</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="F6" s="28" t="s">
         <v>459</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="G6" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>460</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="H6" s="8" t="s">
+      <c r="I6" s="29" t="s">
         <v>461</v>
       </c>
-      <c r="I6" s="29" t="s">
+      <c r="J6" s="8" t="s">
         <v>462</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>463</v>
       </c>
       <c r="K6"/>
       <c r="L6" s="11" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="M6" s="31" t="s">
+        <v>465</v>
+      </c>
+      <c r="N6" s="23" t="s">
         <v>466</v>
       </c>
-      <c r="N6" s="23" t="s">
-        <v>467</v>
-      </c>
       <c r="O6" s="11" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="P6"/>
       <c r="Q6" s="22" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="S6" s="32" t="b">
         <f aca="false">FALSE()</f>
@@ -17667,52 +17687,52 @@
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>457</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="28" t="s">
         <v>458</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="F7" s="28" t="s">
         <v>459</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="G7" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>460</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="H7" s="8" t="s">
+      <c r="I7" s="29" t="s">
         <v>461</v>
       </c>
-      <c r="I7" s="29" t="s">
+      <c r="J7" s="8" t="s">
         <v>462</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>463</v>
       </c>
       <c r="K7"/>
       <c r="L7"/>
       <c r="M7" s="31" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="N7" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="O7" s="11" t="s">
         <v>451</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>452</v>
       </c>
       <c r="P7"/>
       <c r="Q7" s="22" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="S7" s="32" t="b">
         <f aca="false">FALSE()</f>
@@ -17721,40 +17741,40 @@
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D8" s="33" t="s">
         <v>475</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="D8" s="33" t="s">
+      <c r="E8" s="28" t="s">
+        <v>458</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>459</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="H8" s="34" t="s">
         <v>476</v>
       </c>
-      <c r="E8" s="28" t="s">
-        <v>459</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>460</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="H8" s="34" t="s">
+      <c r="I8" s="11" t="s">
         <v>477</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="J8" s="29" t="s">
         <v>478</v>
       </c>
-      <c r="J8" s="29" t="s">
+      <c r="K8" s="29" t="s">
         <v>479</v>
       </c>
-      <c r="K8" s="29" t="s">
+      <c r="L8" s="17" t="s">
         <v>480</v>
-      </c>
-      <c r="L8" s="17" t="s">
-        <v>521</v>
       </c>
       <c r="M8"/>
       <c r="N8"/>
@@ -17764,7 +17784,7 @@
         <v>506</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="S8" s="32" t="b">
         <f aca="false">FALSE()</f>
@@ -17773,37 +17793,37 @@
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
+        <v>482</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>475</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>458</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>459</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="H9" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>476</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>459</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>460</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="H9" s="34" t="s">
+      <c r="I9" s="8" t="s">
         <v>484</v>
       </c>
-      <c r="I9" s="8" t="s">
-        <v>485</v>
-      </c>
       <c r="J9" s="29" t="s">
+        <v>478</v>
+      </c>
+      <c r="K9" s="35" t="s">
         <v>479</v>
-      </c>
-      <c r="K9" s="35" t="s">
-        <v>480</v>
       </c>
       <c r="L9"/>
       <c r="M9"/>
@@ -17814,7 +17834,7 @@
         <v>507</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="S9" s="32" t="b">
         <f aca="false">FALSE()</f>
@@ -17830,13 +17850,13 @@
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10" s="34" t="s">
+        <v>485</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>486</v>
       </c>
-      <c r="I10" s="8" t="s">
-        <v>487</v>
-      </c>
       <c r="J10" s="29" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K10"/>
       <c r="L10"/>
@@ -17885,8 +17905,8 @@
   </sheetPr>
   <dimension ref="B4:G46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17898,62 +17918,62 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="36" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="36" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="36" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="36" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="36" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="36" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="36" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -17962,139 +17982,139 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>497</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="37" t="s">
+        <v>498</v>
+      </c>
+      <c r="F25" s="37" t="s">
         <v>499</v>
-      </c>
-      <c r="F25" s="37" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>505</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="37" t="s">
+        <v>506</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>507</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E33" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="F33" s="0" t="s">
         <v>508</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E34" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="F34" s="0" t="s">
         <v>508</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="G35" s="0" t="s">
         <v>511</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>508</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>509</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E37" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="F37" s="0" t="s">
         <v>508</v>
       </c>
-      <c r="F37" s="0" t="s">
-        <v>509</v>
-      </c>
       <c r="G37" s="0" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="37" t="s">
+        <v>514</v>
+      </c>
+      <c r="E44" s="0" t="s">
         <v>515</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="38" t="s">
+        <v>516</v>
+      </c>
+      <c r="F45" s="0" t="s">
         <v>517</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating business Location page objects
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2389" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2458" uniqueCount="528">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1303,6 +1303,30 @@
   </si>
   <si>
     <t xml:space="preserve">TestCase_172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#$#%$%^%^%^&amp;^        %^&amp;^&amp;*&amp;^*&amp;*(*(*)*()(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business Logic screen-countrycode and type of operation,with invalid input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_174</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_178</t>
   </si>
   <si>
     <t xml:space="preserve">mode</t>
@@ -1718,7 +1742,7 @@
     </r>
   </si>
   <si>
-    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.19-02-02-2022-21:16.apk</t>
+    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.20-09-02-2022-19:04.apk</t>
   </si>
 </sst>
 </file>
@@ -2171,12 +2195,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ1048576"/>
+  <dimension ref="A1:AMJ182"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A105" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="I105" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A105" activeCellId="0" sqref="A105"/>
-      <selection pane="topRight" activeCell="I107" activeCellId="0" sqref="I107"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A180" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="Z180" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A180" activeCellId="0" sqref="A180"/>
+      <selection pane="topRight" activeCell="AB182" activeCellId="0" sqref="AB182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17253,7 +17277,344 @@
         <v>424</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="C177" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E177" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G177" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H177" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I177" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J177" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K177" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="M177" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N177" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="W177" s="8"/>
+      <c r="X177" s="8"/>
+      <c r="Y177" s="8"/>
+      <c r="Z177" s="8"/>
+      <c r="AA177" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="AB177" s="16" t="n">
+        <v>189</v>
+      </c>
+      <c r="AC177" s="8"/>
+      <c r="AD177" s="8"/>
+      <c r="AE177" s="8"/>
+      <c r="AF177" s="8"/>
+      <c r="AG177" s="8"/>
+      <c r="AH177" s="16"/>
+      <c r="AI177" s="8"/>
+      <c r="AJ177" s="8"/>
+    </row>
+    <row r="178" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="C178" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E178" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G178" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="H178" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I178" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J178" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="K178" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="M178" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N178" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="W178" s="8"/>
+      <c r="X178" s="8"/>
+      <c r="Y178" s="8"/>
+      <c r="Z178" s="8"/>
+      <c r="AA178" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="AB178" s="16" t="n">
+        <v>129</v>
+      </c>
+      <c r="AC178" s="8"/>
+      <c r="AD178" s="8"/>
+      <c r="AE178" s="8"/>
+      <c r="AF178" s="8"/>
+      <c r="AG178" s="8"/>
+      <c r="AH178" s="16"/>
+      <c r="AI178" s="8"/>
+      <c r="AJ178" s="8"/>
+    </row>
+    <row r="179" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="B179" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="C179" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E179" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F179" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G179" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="H179" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I179" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J179" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="K179" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="M179" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N179" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="W179" s="8"/>
+      <c r="X179" s="8"/>
+      <c r="Y179" s="8"/>
+      <c r="Z179" s="8"/>
+      <c r="AA179" s="8"/>
+      <c r="AB179" s="16" t="n">
+        <v>900</v>
+      </c>
+      <c r="AC179" s="8"/>
+      <c r="AD179" s="8"/>
+      <c r="AE179" s="8"/>
+      <c r="AF179" s="8"/>
+      <c r="AG179" s="8"/>
+      <c r="AH179" s="16"/>
+      <c r="AI179" s="8"/>
+      <c r="AJ179" s="8"/>
+    </row>
+    <row r="180" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B180" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="C180" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E180" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G180" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H180" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I180" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J180" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K180" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="M180" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N180" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="R180" s="8"/>
+      <c r="T180" s="8"/>
+      <c r="W180" s="8"/>
+      <c r="X180" s="8"/>
+      <c r="Y180" s="8"/>
+      <c r="Z180" s="8"/>
+      <c r="AA180" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="AB180" s="16" t="n">
+        <v>555</v>
+      </c>
+      <c r="AC180" s="8"/>
+      <c r="AD180" s="8"/>
+      <c r="AE180" s="8"/>
+      <c r="AF180" s="8"/>
+      <c r="AG180" s="8"/>
+      <c r="AH180" s="16"/>
+      <c r="AI180" s="8"/>
+      <c r="AJ180" s="8"/>
+    </row>
+    <row r="181" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="C181" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E181" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F181" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G181" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="H181" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I181" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J181" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="K181" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="M181" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N181" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="R181" s="8"/>
+      <c r="T181" s="8"/>
+      <c r="W181" s="8"/>
+      <c r="X181" s="8"/>
+      <c r="Y181" s="8"/>
+      <c r="Z181" s="8"/>
+      <c r="AA181" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="AB181" s="16" t="n">
+        <v>345</v>
+      </c>
+      <c r="AC181" s="8"/>
+      <c r="AD181" s="8"/>
+      <c r="AE181" s="8"/>
+      <c r="AF181" s="8"/>
+      <c r="AG181" s="8"/>
+      <c r="AH181" s="16"/>
+      <c r="AI181" s="8"/>
+      <c r="AJ181" s="8"/>
+    </row>
+    <row r="182" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="B182" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="C182" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E182" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F182" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G182" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="H182" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I182" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J182" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="K182" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="M182" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N182" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="R182" s="8"/>
+      <c r="T182" s="8"/>
+      <c r="W182" s="8"/>
+      <c r="X182" s="8"/>
+      <c r="Y182" s="8"/>
+      <c r="Z182" s="8"/>
+      <c r="AA182" s="8"/>
+      <c r="AB182" s="16" t="n">
+        <v>340</v>
+      </c>
+      <c r="AC182" s="8"/>
+      <c r="AD182" s="8"/>
+      <c r="AE182" s="8"/>
+      <c r="AF182" s="8"/>
+      <c r="AG182" s="8"/>
+      <c r="AH182" s="16"/>
+      <c r="AI182" s="8"/>
+      <c r="AJ182" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I10" r:id="rId1" display="kimtaehyung@gmail.com"/>
@@ -17316,6 +17677,12 @@
     <hyperlink ref="I174" r:id="rId58" display="parkjimin@gmail.com"/>
     <hyperlink ref="I175" r:id="rId59" display="parkjimin@gmail.com"/>
     <hyperlink ref="I176" r:id="rId60" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I177" r:id="rId61" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I178" r:id="rId62" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I179" r:id="rId63" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I180" r:id="rId64" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I181" r:id="rId65" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I182" r:id="rId66" display="parkjimin@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -17334,12 +17701,12 @@
   </sheetPr>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L5" activeCellId="0" sqref="L5"/>
+      <selection pane="bottomRight" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17370,97 +17737,97 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>427</v>
+        <v>435</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>428</v>
+        <v>436</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>429</v>
+        <v>437</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>430</v>
+        <v>438</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>431</v>
+        <v>439</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>437</v>
+        <v>445</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>438</v>
+        <v>446</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>440</v>
+        <v>448</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>441</v>
+        <v>449</v>
       </c>
       <c r="R1" s="19" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>443</v>
+        <v>451</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>444</v>
+        <v>452</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>445</v>
+        <v>453</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2" s="21" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="H2"/>
       <c r="I2" s="21" t="s">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>449</v>
+        <v>457</v>
       </c>
       <c r="K2"/>
       <c r="L2"/>
       <c r="M2"/>
       <c r="N2" s="23" t="s">
-        <v>450</v>
+        <v>458</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
       <c r="P2"/>
       <c r="Q2" s="22" t="n">
         <v>500</v>
       </c>
       <c r="R2" s="24" t="s">
-        <v>452</v>
+        <v>460</v>
       </c>
       <c r="S2" s="22" t="n">
         <v>0</v>
@@ -17468,44 +17835,44 @@
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
+        <v>461</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>453</v>
       </c>
-      <c r="B3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>445</v>
-      </c>
       <c r="D3" s="20" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" s="20" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="H3"/>
       <c r="I3" s="25" t="s">
-        <v>454</v>
+        <v>462</v>
       </c>
       <c r="J3" s="25" t="s">
-        <v>449</v>
+        <v>457</v>
       </c>
       <c r="K3"/>
       <c r="L3"/>
       <c r="M3"/>
       <c r="N3" s="23" t="s">
-        <v>450</v>
+        <v>458</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
       <c r="P3"/>
       <c r="Q3" s="22" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="25" t="s">
-        <v>452</v>
+        <v>460</v>
       </c>
       <c r="S3" s="26" t="b">
         <f aca="false">FALSE()</f>
@@ -17515,56 +17882,56 @@
     </row>
     <row r="4" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>466</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>467</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>457</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>458</v>
-      </c>
-      <c r="F4" s="28" t="s">
+      <c r="H4" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>469</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="L4" s="30" t="s">
+        <v>527</v>
+      </c>
+      <c r="M4" s="31" t="s">
+        <v>473</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>474</v>
+      </c>
+      <c r="O4" s="11" t="s">
         <v>459</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>460</v>
-      </c>
-      <c r="I4" s="29" t="s">
-        <v>461</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>462</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>463</v>
-      </c>
-      <c r="L4" s="30" t="s">
-        <v>519</v>
-      </c>
-      <c r="M4" s="31" t="s">
-        <v>465</v>
-      </c>
-      <c r="N4" s="23" t="s">
-        <v>466</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>451</v>
       </c>
       <c r="P4"/>
       <c r="Q4" s="22" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="S4" s="32" t="b">
         <f aca="false">FALSE()</f>
@@ -17573,56 +17940,56 @@
     </row>
     <row r="5" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>457</v>
+        <v>465</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="F5" s="28" t="s">
+        <v>467</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>472</v>
+      </c>
+      <c r="M5" s="31" t="s">
+        <v>473</v>
+      </c>
+      <c r="N5" s="23" t="s">
+        <v>474</v>
+      </c>
+      <c r="O5" s="11" t="s">
         <v>459</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>469</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>470</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>462</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>463</v>
-      </c>
-      <c r="L5" s="17" t="s">
-        <v>464</v>
-      </c>
-      <c r="M5" s="31" t="s">
-        <v>465</v>
-      </c>
-      <c r="N5" s="23" t="s">
-        <v>466</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>451</v>
       </c>
       <c r="P5"/>
       <c r="Q5" s="22" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="S5" s="32" t="b">
         <f aca="false">FALSE()</f>
@@ -17631,54 +17998,54 @@
     </row>
     <row r="6" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>471</v>
+        <v>479</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>457</v>
+        <v>465</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>459</v>
+        <v>467</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>460</v>
+        <v>468</v>
       </c>
       <c r="I6" s="29" t="s">
-        <v>461</v>
+        <v>469</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="K6"/>
       <c r="L6" s="11" t="s">
-        <v>472</v>
+        <v>480</v>
       </c>
       <c r="M6" s="31" t="s">
-        <v>465</v>
+        <v>473</v>
       </c>
       <c r="N6" s="23" t="s">
-        <v>466</v>
+        <v>474</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
       <c r="P6"/>
       <c r="Q6" s="22" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="S6" s="32" t="b">
         <f aca="false">FALSE()</f>
@@ -17687,52 +18054,52 @@
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>473</v>
+        <v>481</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>457</v>
+        <v>465</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>459</v>
+        <v>467</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>460</v>
+        <v>468</v>
       </c>
       <c r="I7" s="29" t="s">
-        <v>461</v>
+        <v>469</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="K7"/>
       <c r="L7"/>
       <c r="M7" s="31" t="s">
-        <v>465</v>
+        <v>473</v>
       </c>
       <c r="N7" s="23" t="s">
-        <v>450</v>
+        <v>458</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
       <c r="P7"/>
       <c r="Q7" s="22" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="S7" s="32" t="b">
         <f aca="false">FALSE()</f>
@@ -17741,40 +18108,40 @@
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>474</v>
+        <v>482</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>475</v>
+        <v>483</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>459</v>
+        <v>467</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="H8" s="34" t="s">
-        <v>476</v>
+        <v>484</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>477</v>
+        <v>485</v>
       </c>
       <c r="J8" s="29" t="s">
-        <v>478</v>
+        <v>486</v>
       </c>
       <c r="K8" s="29" t="s">
-        <v>479</v>
+        <v>487</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>480</v>
+        <v>488</v>
       </c>
       <c r="M8"/>
       <c r="N8"/>
@@ -17784,7 +18151,7 @@
         <v>506</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>481</v>
+        <v>489</v>
       </c>
       <c r="S8" s="32" t="b">
         <f aca="false">FALSE()</f>
@@ -17793,37 +18160,37 @@
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>475</v>
+        <v>483</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>459</v>
+        <v>467</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="H9" s="34" t="s">
-        <v>483</v>
+        <v>491</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
       <c r="J9" s="29" t="s">
-        <v>478</v>
+        <v>486</v>
       </c>
       <c r="K9" s="35" t="s">
-        <v>479</v>
+        <v>487</v>
       </c>
       <c r="L9"/>
       <c r="M9"/>
@@ -17834,7 +18201,7 @@
         <v>507</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>481</v>
+        <v>489</v>
       </c>
       <c r="S9" s="32" t="b">
         <f aca="false">FALSE()</f>
@@ -17850,13 +18217,13 @@
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10" s="34" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
       <c r="I10" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="J10" s="29" t="s">
         <v>486</v>
-      </c>
-      <c r="J10" s="29" t="s">
-        <v>478</v>
       </c>
       <c r="K10"/>
       <c r="L10"/>
@@ -17918,62 +18285,62 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>487</v>
+        <v>495</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="36" t="s">
-        <v>461</v>
+        <v>469</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="36" t="s">
-        <v>488</v>
+        <v>496</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="36" t="s">
-        <v>461</v>
+        <v>469</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="36" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="36" t="s">
-        <v>490</v>
+        <v>498</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>470</v>
+        <v>478</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="36" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="36" t="s">
-        <v>491</v>
+        <v>499</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>492</v>
+        <v>500</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>493</v>
+        <v>501</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>494</v>
+        <v>502</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -17982,139 +18349,139 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>495</v>
+        <v>503</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>496</v>
+        <v>504</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="37" t="s">
-        <v>498</v>
+        <v>506</v>
       </c>
       <c r="F25" s="37" t="s">
-        <v>499</v>
+        <v>507</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>500</v>
+        <v>508</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>501</v>
+        <v>509</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>502</v>
+        <v>510</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>503</v>
+        <v>511</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="9" t="s">
-        <v>504</v>
+        <v>512</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>505</v>
+        <v>513</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="37" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>477</v>
+        <v>485</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>508</v>
+        <v>516</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>509</v>
+        <v>517</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>508</v>
+        <v>516</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>510</v>
+        <v>518</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>508</v>
+        <v>516</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>511</v>
+        <v>519</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>512</v>
+        <v>520</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>486</v>
+        <v>494</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>508</v>
+        <v>516</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>513</v>
+        <v>521</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="37" t="s">
-        <v>514</v>
+        <v>522</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>515</v>
+        <v>523</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="38" t="s">
-        <v>516</v>
+        <v>524</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>517</v>
+        <v>525</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="39" t="s">
-        <v>518</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made changes in Industry edit function
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2471" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2478" uniqueCount="539">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1771,6 +1771,9 @@
       </rPr>
       <t xml:space="preserve">);</t>
     </r>
+  </si>
+  <si>
+    <t>null</t>
   </si>
   <si>
     <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.20-09-02-2022-19:04.apk</t>
@@ -2230,7 +2233,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="Z169" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A169" activeCellId="0" sqref="A169"/>
-      <selection pane="topRight" activeCell="AD175" activeCellId="0" sqref="AD175"/>
+      <selection pane="topRight" activeCell="AC175" activeCellId="0" sqref="AC175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16680,7 +16683,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
         <v>403</v>
       </c>
@@ -16754,16 +16757,16 @@
         <v>405</v>
       </c>
       <c r="AD175" s="1" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="AE175" s="1" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="AF175" s="1" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="AG175" s="1" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18115,7 +18118,7 @@
         <v>480</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>482</v>
@@ -18341,7 +18344,7 @@
         <v>497</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>498</v>
+        <v>537</v>
       </c>
       <c r="M8"/>
       <c r="N8"/>

</xml_diff>

<commit_message>
made changes in IOS entityContact details
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2611" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2459" uniqueCount="538">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1774,9 +1774,6 @@
   </si>
   <si>
     <t>null</t>
-  </si>
-  <si>
-    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.20-09-02-2022-19:04.apk</t>
   </si>
 </sst>
 </file>
@@ -2233,7 +2230,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="Z169" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A169" activeCellId="0" sqref="A169"/>
-      <selection pane="topRight" activeCell="AC175" activeCellId="0" sqref="AC175"/>
+      <selection pane="topRight" activeCell="AC172" activeCellId="0" sqref="AC172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18118,7 +18115,7 @@
         <v>480</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>538</v>
+        <v>481</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>482</v>

</xml_diff>

<commit_message>
made changes in dashboard features
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2463" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2503" uniqueCount="539">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1774,6 +1774,9 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.20-09-02-2022-19:04.apk</t>
   </si>
 </sst>
 </file>
@@ -18115,7 +18118,7 @@
         <v>480</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>481</v>
+        <v>538</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>482</v>

</xml_diff>

<commit_message>
made changes in commercial features
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2457" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2462" uniqueCount="541">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1777,6 +1777,12 @@
       </rPr>
       <t xml:space="preserve">);</t>
     </r>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.20-09-02-2022-19:04.apk</t>
   </si>
 </sst>
 </file>
@@ -2236,56 +2242,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="4" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="14.33" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
+    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
+    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
+    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
+    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
+    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
+    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
+    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
+    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
+    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
+    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
+    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
+    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
+    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
+    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="991" max="1025" customWidth="true" hidden="false" style="4" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17912,22 +17918,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="5.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="11" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="11" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="26.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="11" width="9.17"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="11" width="12.57" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="11" width="5.18" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="4" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="11" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="11" width="20.5" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="11" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="11" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="11" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="13" customWidth="true" hidden="false" style="11" width="14.87" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="11" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="11" width="26.35" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="17" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="11" width="29.45" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="1025" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18002,21 +18008,28 @@
       <c r="D2" s="23" t="s">
         <v>465</v>
       </c>
+      <c r="E2"/>
+      <c r="F2"/>
       <c r="G2" s="23" t="s">
         <v>466</v>
       </c>
+      <c r="H2"/>
       <c r="I2" s="23" t="s">
         <v>467</v>
       </c>
       <c r="J2" s="24" t="s">
         <v>468</v>
       </c>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
       <c r="N2" s="25" t="s">
         <v>469</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>470</v>
       </c>
+      <c r="P2"/>
       <c r="Q2" s="24" t="n">
         <v>500</v>
       </c>
@@ -18040,28 +18053,35 @@
       <c r="D3" s="22" t="s">
         <v>465</v>
       </c>
+      <c r="E3"/>
+      <c r="F3"/>
       <c r="G3" s="22" t="s">
         <v>466</v>
       </c>
+      <c r="H3"/>
       <c r="I3" s="27" t="s">
         <v>473</v>
       </c>
       <c r="J3" s="27" t="s">
         <v>468</v>
       </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
       <c r="N3" s="25" t="s">
         <v>469</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>470</v>
       </c>
+      <c r="P3"/>
       <c r="Q3" s="24" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="27" t="s">
         <v>471</v>
       </c>
-      <c r="S3" s="28" t="n">
+      <c r="S3" s="28" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18102,7 +18122,7 @@
         <v>482</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>483</v>
+        <v>540</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>484</v>
@@ -18113,13 +18133,14 @@
       <c r="O4" s="12" t="s">
         <v>470</v>
       </c>
+      <c r="P4"/>
       <c r="Q4" s="24" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="S4" s="33" t="n">
+      <c r="S4" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18170,13 +18191,14 @@
       <c r="O5" s="12" t="s">
         <v>470</v>
       </c>
+      <c r="P5"/>
       <c r="Q5" s="24" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="S5" s="33" t="n">
+      <c r="S5" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18212,6 +18234,7 @@
       <c r="J6" s="9" t="s">
         <v>481</v>
       </c>
+      <c r="K6"/>
       <c r="L6" s="12" t="s">
         <v>492</v>
       </c>
@@ -18224,13 +18247,14 @@
       <c r="O6" s="12" t="s">
         <v>470</v>
       </c>
+      <c r="P6"/>
       <c r="Q6" s="24" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="S6" s="33" t="n">
+      <c r="S6" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18266,6 +18290,8 @@
       <c r="J7" s="9" t="s">
         <v>481</v>
       </c>
+      <c r="K7"/>
+      <c r="L7"/>
       <c r="M7" s="12" t="s">
         <v>484</v>
       </c>
@@ -18275,13 +18301,14 @@
       <c r="O7" s="12" t="s">
         <v>470</v>
       </c>
+      <c r="P7"/>
       <c r="Q7" s="24" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="S7" s="33" t="n">
+      <c r="S7" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18321,15 +18348,19 @@
         <v>499</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>500</v>
-      </c>
+        <v>539</v>
+      </c>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
       <c r="Q8" s="24" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>501</v>
       </c>
-      <c r="S8" s="33" t="n">
+      <c r="S8" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18368,18 +18399,30 @@
       <c r="K9" s="35" t="s">
         <v>499</v>
       </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
       <c r="Q9" s="24" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>501</v>
       </c>
-      <c r="S9" s="33" t="n">
+      <c r="S9" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
       <c r="H10" s="34" t="s">
         <v>505</v>
       </c>
@@ -18389,6 +18432,15 @@
       <c r="J10" s="31" t="s">
         <v>498</v>
       </c>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -18433,9 +18485,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
made changes in object class
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2553" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2561" uniqueCount="552">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1813,6 +1813,9 @@
       </rPr>
       <t xml:space="preserve">);</t>
     </r>
+  </si>
+  <si>
+    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.21-24-02-2022-13:09.apk</t>
   </si>
 </sst>
 </file>
@@ -2266,62 +2269,62 @@
   </sheetPr>
   <dimension ref="A1:AMJ198"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A195" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F197" activeCellId="0" sqref="F197"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AJ192" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AO197" activeCellId="0" sqref="AO197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="4" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="14.33" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
+    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
+    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
+    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
+    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
+    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
+    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
+    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
+    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
+    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
+    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
+    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
+    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
+    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
+    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="991" max="1025" customWidth="true" hidden="false" style="4" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18116,7 +18119,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
         <v>452</v>
       </c>
@@ -18366,22 +18369,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="5.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="11" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="11" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="26.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="11" width="9.17"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="11" width="12.57" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="11" width="5.18" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="4" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="11" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="11" width="20.5" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="11" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="11" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="11" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="13" customWidth="true" hidden="false" style="11" width="14.87" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="11" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="11" width="26.35" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="17" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="11" width="29.45" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="1025" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18456,21 +18459,28 @@
       <c r="D2" s="23" t="s">
         <v>477</v>
       </c>
+      <c r="E2"/>
+      <c r="F2"/>
       <c r="G2" s="23" t="s">
         <v>478</v>
       </c>
+      <c r="H2"/>
       <c r="I2" s="23" t="s">
         <v>479</v>
       </c>
       <c r="J2" s="24" t="s">
         <v>480</v>
       </c>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
       <c r="N2" s="25" t="s">
         <v>481</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>482</v>
       </c>
+      <c r="P2"/>
       <c r="Q2" s="24" t="n">
         <v>500</v>
       </c>
@@ -18494,28 +18504,35 @@
       <c r="D3" s="22" t="s">
         <v>477</v>
       </c>
+      <c r="E3"/>
+      <c r="F3"/>
       <c r="G3" s="22" t="s">
         <v>478</v>
       </c>
+      <c r="H3"/>
       <c r="I3" s="27" t="s">
         <v>485</v>
       </c>
       <c r="J3" s="27" t="s">
         <v>480</v>
       </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
       <c r="N3" s="25" t="s">
         <v>481</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>482</v>
       </c>
+      <c r="P3"/>
       <c r="Q3" s="24" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="27" t="s">
         <v>483</v>
       </c>
-      <c r="S3" s="28" t="n">
+      <c r="S3" s="28" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18556,7 +18573,7 @@
         <v>494</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>495</v>
+        <v>551</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>496</v>
@@ -18567,13 +18584,14 @@
       <c r="O4" s="12" t="s">
         <v>482</v>
       </c>
+      <c r="P4"/>
       <c r="Q4" s="24" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>498</v>
       </c>
-      <c r="S4" s="33" t="n">
+      <c r="S4" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18624,13 +18642,14 @@
       <c r="O5" s="12" t="s">
         <v>482</v>
       </c>
+      <c r="P5"/>
       <c r="Q5" s="24" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>498</v>
       </c>
-      <c r="S5" s="33" t="n">
+      <c r="S5" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18666,6 +18685,7 @@
       <c r="J6" s="9" t="s">
         <v>493</v>
       </c>
+      <c r="K6"/>
       <c r="L6" s="12" t="s">
         <v>504</v>
       </c>
@@ -18678,13 +18698,14 @@
       <c r="O6" s="12" t="s">
         <v>482</v>
       </c>
+      <c r="P6"/>
       <c r="Q6" s="24" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>498</v>
       </c>
-      <c r="S6" s="33" t="n">
+      <c r="S6" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18720,6 +18741,8 @@
       <c r="J7" s="9" t="s">
         <v>493</v>
       </c>
+      <c r="K7"/>
+      <c r="L7"/>
       <c r="M7" s="12" t="s">
         <v>496</v>
       </c>
@@ -18729,13 +18752,14 @@
       <c r="O7" s="12" t="s">
         <v>482</v>
       </c>
+      <c r="P7"/>
       <c r="Q7" s="24" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>498</v>
       </c>
-      <c r="S7" s="33" t="n">
+      <c r="S7" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18777,13 +18801,17 @@
       <c r="L8" s="11" t="s">
         <v>512</v>
       </c>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
       <c r="Q8" s="24" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>513</v>
       </c>
-      <c r="S8" s="33" t="n">
+      <c r="S8" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18822,18 +18850,30 @@
       <c r="K9" s="35" t="s">
         <v>511</v>
       </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
       <c r="Q9" s="24" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>513</v>
       </c>
-      <c r="S9" s="33" t="n">
+      <c r="S9" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
       <c r="H10" s="34" t="s">
         <v>517</v>
       </c>
@@ -18843,6 +18883,15 @@
       <c r="J10" s="31" t="s">
         <v>510</v>
       </c>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -18887,9 +18936,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
made changes in android utility
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2561" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2559" uniqueCount="553">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1510,6 +1510,36 @@
   </si>
   <si>
     <t xml:space="preserve">https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.20-09-02-2022-19:04.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation-1-0-21-24-02-2022.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.19-02-02-2022-21:16.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://di</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_0003</t>
   </si>
   <si>
     <r>
@@ -1532,33 +1562,6 @@
       </rPr>
       <t xml:space="preserve">.apk</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.0.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.19-02-02-2022-21:16.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://di</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_0003</t>
   </si>
   <si>
     <t xml:space="preserve">IOS_001</t>
@@ -2269,7 +2272,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ198"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AJ192" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AJ183" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AO197" activeCellId="0" sqref="AO197"/>
     </sheetView>
   </sheetViews>
@@ -18359,12 +18362,12 @@
   </sheetPr>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18538,7 +18541,7 @@
       </c>
       <c r="U3" s="29"/>
     </row>
-    <row r="4" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
         <v>486</v>
       </c>
@@ -18573,7 +18576,7 @@
         <v>494</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>496</v>
@@ -18596,7 +18599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>499</v>
       </c>
@@ -18654,7 +18657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
         <v>503</v>
       </c>
@@ -18744,7 +18747,7 @@
       <c r="K7"/>
       <c r="L7"/>
       <c r="M7" s="12" t="s">
-        <v>496</v>
+        <v>506</v>
       </c>
       <c r="N7" s="25" t="s">
         <v>481</v>
@@ -18766,7 +18769,7 @@
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>42</v>
@@ -18775,7 +18778,7 @@
         <v>487</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="E8" s="30" t="s">
         <v>489</v>
@@ -18787,19 +18790,19 @@
         <v>478</v>
       </c>
       <c r="H8" s="34" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="J8" s="31" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="K8" s="31" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="M8"/>
       <c r="N8"/>
@@ -18809,7 +18812,7 @@
         <v>506</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="S8" s="33" t="b">
         <f aca="false">FALSE()</f>
@@ -18818,7 +18821,7 @@
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>42</v>
@@ -18827,7 +18830,7 @@
         <v>487</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="E9" s="30" t="s">
         <v>489</v>
@@ -18839,16 +18842,16 @@
         <v>478</v>
       </c>
       <c r="H9" s="34" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="J9" s="31" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="K9" s="35" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="L9"/>
       <c r="M9"/>
@@ -18859,7 +18862,7 @@
         <v>507</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="S9" s="33" t="b">
         <f aca="false">FALSE()</f>
@@ -18875,13 +18878,13 @@
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10" s="34" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="J10" s="31" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="K10"/>
       <c r="L10"/>
@@ -18943,7 +18946,7 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18953,7 +18956,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="36" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18963,12 +18966,12 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="36" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="36" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18978,27 +18981,27 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="36" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="36" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -19007,139 +19010,139 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="37" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="F25" s="37" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="38" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="37" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
+        <v>542</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="F34" s="0" t="s">
         <v>541</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>539</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="37" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="39" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="40" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made changes in source of fund objects'
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2591" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2644" uniqueCount="557">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1828,6 +1828,9 @@
       </rPr>
       <t xml:space="preserve">);</t>
     </r>
+  </si>
+  <si>
+    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.21-24-02-2022-13:09.apk</t>
   </si>
 </sst>
 </file>
@@ -2292,61 +2295,61 @@
   <dimension ref="A1:AMJ200"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A193" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A196" activeCellId="0" sqref="A196"/>
+      <selection pane="topLeft" activeCell="E196" activeCellId="0" sqref="E196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="4" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="14.33" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
+    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
+    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
+    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
+    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
+    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
+    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
+    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
+    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
+    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
+    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
+    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
+    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
+    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
+    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="991" max="1025" customWidth="true" hidden="false" style="4" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18548,22 +18551,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="5.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="11" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="11" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="26.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="11" width="9.17"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="11" width="12.57" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="11" width="5.18" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="4" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="11" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="11" width="20.5" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="11" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="11" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="11" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="13" customWidth="true" hidden="false" style="11" width="14.87" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="11" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="11" width="26.35" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="17" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="11" width="29.45" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="1025" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18638,21 +18641,28 @@
       <c r="D2" s="23" t="s">
         <v>481</v>
       </c>
+      <c r="E2"/>
+      <c r="F2"/>
       <c r="G2" s="23" t="s">
         <v>482</v>
       </c>
+      <c r="H2"/>
       <c r="I2" s="23" t="s">
         <v>483</v>
       </c>
       <c r="J2" s="24" t="s">
         <v>484</v>
       </c>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
       <c r="N2" s="25" t="s">
         <v>485</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>486</v>
       </c>
+      <c r="P2"/>
       <c r="Q2" s="24" t="n">
         <v>500</v>
       </c>
@@ -18676,28 +18686,35 @@
       <c r="D3" s="22" t="s">
         <v>481</v>
       </c>
+      <c r="E3"/>
+      <c r="F3"/>
       <c r="G3" s="22" t="s">
         <v>482</v>
       </c>
+      <c r="H3"/>
       <c r="I3" s="27" t="s">
         <v>489</v>
       </c>
       <c r="J3" s="27" t="s">
         <v>484</v>
       </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
       <c r="N3" s="25" t="s">
         <v>485</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>486</v>
       </c>
+      <c r="P3"/>
       <c r="Q3" s="24" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="27" t="s">
         <v>487</v>
       </c>
-      <c r="S3" s="28" t="n">
+      <c r="S3" s="28" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18738,7 +18755,7 @@
         <v>498</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>499</v>
+        <v>556</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>500</v>
@@ -18749,13 +18766,14 @@
       <c r="O4" s="12" t="s">
         <v>486</v>
       </c>
+      <c r="P4"/>
       <c r="Q4" s="24" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>502</v>
       </c>
-      <c r="S4" s="33" t="n">
+      <c r="S4" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18806,13 +18824,14 @@
       <c r="O5" s="12" t="s">
         <v>486</v>
       </c>
+      <c r="P5"/>
       <c r="Q5" s="24" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>502</v>
       </c>
-      <c r="S5" s="33" t="n">
+      <c r="S5" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18848,6 +18867,7 @@
       <c r="J6" s="9" t="s">
         <v>497</v>
       </c>
+      <c r="K6"/>
       <c r="L6" s="12" t="s">
         <v>509</v>
       </c>
@@ -18860,13 +18880,14 @@
       <c r="O6" s="12" t="s">
         <v>486</v>
       </c>
+      <c r="P6"/>
       <c r="Q6" s="24" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>502</v>
       </c>
-      <c r="S6" s="33" t="n">
+      <c r="S6" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18902,6 +18923,8 @@
       <c r="J7" s="9" t="s">
         <v>497</v>
       </c>
+      <c r="K7"/>
+      <c r="L7"/>
       <c r="M7" s="12" t="s">
         <v>511</v>
       </c>
@@ -18911,13 +18934,14 @@
       <c r="O7" s="12" t="s">
         <v>486</v>
       </c>
+      <c r="P7"/>
       <c r="Q7" s="24" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>502</v>
       </c>
-      <c r="S7" s="33" t="n">
+      <c r="S7" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18959,13 +18983,17 @@
       <c r="L8" s="11" t="s">
         <v>518</v>
       </c>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
       <c r="Q8" s="24" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>519</v>
       </c>
-      <c r="S8" s="33" t="n">
+      <c r="S8" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -19004,18 +19032,30 @@
       <c r="K9" s="36" t="s">
         <v>517</v>
       </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
       <c r="Q9" s="24" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>519</v>
       </c>
-      <c r="S9" s="33" t="n">
+      <c r="S9" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
       <c r="H10" s="35" t="s">
         <v>523</v>
       </c>
@@ -19025,6 +19065,15 @@
       <c r="J10" s="34" t="s">
         <v>516</v>
       </c>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -19069,9 +19118,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updating source wealth object class
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2608" uniqueCount="557">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -2294,8 +2294,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ200"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A193" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E196" activeCellId="0" sqref="E196"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AJ193" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AM197" activeCellId="0" sqref="AM197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
made chnages in IOS entity name objects
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2609" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2641" uniqueCount="564">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1411,6 +1411,24 @@
   </si>
   <si>
     <t xml:space="preserve">TestCase_196</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_197</t>
+  </si>
+  <si>
+    <t xml:space="preserve">golden street unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pink street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">koduvally city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kozhikodu post</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_198</t>
   </si>
   <si>
     <t xml:space="preserve">mode</t>
@@ -1831,9 +1849,6 @@
       </rPr>
       <t xml:space="preserve">);</t>
     </r>
-  </si>
-  <si>
-    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.21-24-02-2022-13:09.apk</t>
   </si>
   <si>
     <t>null</t>
@@ -2288,10 +2303,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ200"/>
+  <dimension ref="A1:AMJ202"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AJ193" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AM197" activeCellId="0" sqref="AM197"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B196" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E199" activeCellId="0" sqref="E199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18432,6 +18447,235 @@
       <c r="AM200" s="1" t="s">
         <v>451</v>
       </c>
+    </row>
+    <row r="201" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B201" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="C201" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E201" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F201" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G201" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="H201" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="I201" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="J201" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="K201" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="M201" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="N201" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="O201" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="P201" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q201" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="R201" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="S201" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="T201" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="U201" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="V201" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="W201" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="X201" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="Y201" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="Z201" s="9" t="n">
+        <v>1234</v>
+      </c>
+      <c r="AA201" s="9"/>
+      <c r="AB201" s="9"/>
+      <c r="AC201" s="9"/>
+      <c r="AD201" s="9"/>
+      <c r="AE201" s="9"/>
+      <c r="AF201" s="9"/>
+      <c r="AG201" s="9"/>
+      <c r="AH201" s="9"/>
+      <c r="AI201" s="9"/>
+      <c r="AJ201" s="9"/>
+      <c r="AK201" s="9"/>
+      <c r="AL201" s="9"/>
+      <c r="AM201" s="9"/>
+      <c r="AN201" s="15"/>
+      <c r="AO201" s="16"/>
+      <c r="AP201" s="9"/>
+      <c r="AQ201" s="9"/>
+      <c r="AR201" s="9"/>
+      <c r="AS201" s="9"/>
+      <c r="AT201" s="9"/>
+      <c r="AU201" s="9"/>
+      <c r="AV201" s="16"/>
+      <c r="AW201" s="16"/>
+      <c r="AX201" s="9"/>
+      <c r="AY201" s="9"/>
+      <c r="AZ201" s="9"/>
+      <c r="BA201" s="9"/>
+      <c r="BB201" s="15"/>
+      <c r="BC201" s="9"/>
+      <c r="BD201" s="9"/>
+      <c r="BE201" s="9"/>
+      <c r="BF201" s="9"/>
+      <c r="BG201" s="9"/>
+      <c r="BH201" s="9"/>
+      <c r="BI201" s="9"/>
+      <c r="BJ201" s="9"/>
+      <c r="BK201" s="9"/>
+      <c r="BL201" s="9"/>
+      <c r="BM201" s="9"/>
+      <c r="BN201" s="9"/>
+      <c r="BO201" s="9"/>
+      <c r="BP201" s="9"/>
+      <c r="BQ201" s="9"/>
+      <c r="BR201" s="9"/>
+      <c r="BS201" s="9"/>
+      <c r="BT201" s="9"/>
+      <c r="BU201" s="9"/>
+      <c r="BV201" s="9"/>
+      <c r="BW201" s="9"/>
+      <c r="BX201" s="9"/>
+      <c r="BY201" s="9"/>
+    </row>
+    <row r="202" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B202" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="C202" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E202" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G202" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="H202" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="I202" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="J202" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="K202" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="M202" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="N202" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="O202" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="P202" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q202" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="R202" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="S202" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="T202" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="U202" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="V202" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="W202" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="X202" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="Y202" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="Z202" s="9" t="n">
+        <v>1234</v>
+      </c>
+      <c r="AA202" s="9"/>
+      <c r="AB202" s="9"/>
+      <c r="AC202" s="9"/>
+      <c r="AD202" s="9"/>
+      <c r="AE202" s="9"/>
+      <c r="AF202" s="9"/>
+      <c r="AG202" s="9"/>
+      <c r="AH202" s="9"/>
+      <c r="AI202" s="9"/>
+      <c r="AJ202" s="9"/>
+      <c r="AK202" s="9"/>
+      <c r="AL202" s="9"/>
+      <c r="AM202" s="9"/>
+      <c r="AN202" s="15"/>
+      <c r="AO202" s="16"/>
+      <c r="AP202" s="9"/>
+      <c r="AQ202" s="9"/>
+      <c r="AR202" s="9"/>
+      <c r="AS202" s="9"/>
+      <c r="AT202" s="9"/>
+      <c r="AU202" s="9"/>
+      <c r="AV202" s="16"/>
+      <c r="AW202" s="16"/>
+      <c r="AX202" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -18519,6 +18763,8 @@
     <hyperlink ref="I198" r:id="rId82" display="parkjimin@gmail.com"/>
     <hyperlink ref="I199" r:id="rId83" display="parkjimin@gmail.com"/>
     <hyperlink ref="I200" r:id="rId84" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I201" r:id="rId85" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I202" r:id="rId86" display="parkjimin@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -18573,97 +18819,97 @@
         <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>464</v>
+        <v>470</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="R1" s="21" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>43</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2" s="23" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="H2"/>
       <c r="I2" s="23" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="K2"/>
       <c r="L2"/>
       <c r="M2"/>
       <c r="N2" s="25" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="P2"/>
       <c r="Q2" s="24" t="n">
         <v>500</v>
       </c>
       <c r="R2" s="26" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="S2" s="24" t="n">
         <v>0</v>
@@ -18671,44 +18917,44 @@
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
       <c r="B3" s="22" t="s">
         <v>43</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" s="22" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="H3"/>
       <c r="I3" s="27" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="K3"/>
       <c r="L3"/>
       <c r="M3"/>
       <c r="N3" s="25" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="P3"/>
       <c r="Q3" s="24" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="27" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="S3" s="28" t="b">
         <f aca="false">FALSE()</f>
@@ -18718,56 +18964,56 @@
     </row>
     <row r="4" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>499</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>500</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>501</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>502</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>503</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="L4" s="32" t="s">
+        <v>506</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>507</v>
+      </c>
+      <c r="N4" s="25" t="s">
+        <v>508</v>
+      </c>
+      <c r="O4" s="12" t="s">
         <v>493</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>494</v>
-      </c>
-      <c r="F4" s="30" t="s">
-        <v>495</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>496</v>
-      </c>
-      <c r="I4" s="31" t="s">
-        <v>497</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>498</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>499</v>
-      </c>
-      <c r="L4" s="32" t="s">
-        <v>557</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>501</v>
-      </c>
-      <c r="N4" s="25" t="s">
-        <v>502</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>487</v>
       </c>
       <c r="P4"/>
       <c r="Q4" s="24" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="S4" s="33" t="b">
         <f aca="false">FALSE()</f>
@@ -18776,56 +19022,56 @@
     </row>
     <row r="5" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>499</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>500</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>501</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>511</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>512</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>504</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="K5" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>513</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>507</v>
+      </c>
+      <c r="N5" s="25" t="s">
+        <v>508</v>
+      </c>
+      <c r="O5" s="12" t="s">
         <v>493</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>494</v>
-      </c>
-      <c r="F5" s="30" t="s">
-        <v>495</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>505</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>506</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>498</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>499</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>507</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>501</v>
-      </c>
-      <c r="N5" s="25" t="s">
-        <v>502</v>
-      </c>
-      <c r="O5" s="12" t="s">
-        <v>487</v>
       </c>
       <c r="P5"/>
       <c r="Q5" s="24" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="S5" s="33" t="b">
         <f aca="false">FALSE()</f>
@@ -18834,54 +19080,54 @@
     </row>
     <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="I6" s="31" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>498</v>
+        <v>504</v>
       </c>
       <c r="K6"/>
       <c r="L6" s="12" t="s">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="N6" s="25" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="P6"/>
       <c r="Q6" s="24" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="S6" s="33" t="b">
         <f aca="false">FALSE()</f>
@@ -18890,52 +19136,52 @@
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>511</v>
+        <v>517</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="I7" s="31" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>498</v>
+        <v>504</v>
       </c>
       <c r="K7"/>
       <c r="L7"/>
       <c r="M7" s="12" t="s">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c r="N7" s="25" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="P7"/>
       <c r="Q7" s="24" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="S7" s="33" t="b">
         <f aca="false">FALSE()</f>
@@ -18944,40 +19190,40 @@
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="H8" s="34" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="J8" s="31" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="K8" s="31" t="s">
-        <v>518</v>
+        <v>524</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>558</v>
+        <v>563</v>
       </c>
       <c r="M8"/>
       <c r="N8"/>
@@ -18987,7 +19233,7 @@
         <v>506</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>520</v>
+        <v>526</v>
       </c>
       <c r="S8" s="33" t="b">
         <f aca="false">FALSE()</f>
@@ -18996,37 +19242,37 @@
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>521</v>
+        <v>527</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="H9" s="34" t="s">
-        <v>522</v>
+        <v>528</v>
       </c>
       <c r="I9" s="9" t="s">
+        <v>529</v>
+      </c>
+      <c r="J9" s="31" t="s">
         <v>523</v>
       </c>
-      <c r="J9" s="31" t="s">
-        <v>517</v>
-      </c>
       <c r="K9" s="35" t="s">
-        <v>518</v>
+        <v>524</v>
       </c>
       <c r="L9"/>
       <c r="M9"/>
@@ -19037,7 +19283,7 @@
         <v>507</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>520</v>
+        <v>526</v>
       </c>
       <c r="S9" s="33" t="b">
         <f aca="false">FALSE()</f>
@@ -19053,13 +19299,13 @@
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10" s="34" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="J10" s="31" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="K10"/>
       <c r="L10"/>
@@ -19121,62 +19367,62 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="36" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="36" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="36" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="36" t="s">
-        <v>528</v>
+        <v>534</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="36" t="s">
-        <v>529</v>
+        <v>535</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="36" t="s">
-        <v>528</v>
+        <v>534</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="36" t="s">
-        <v>497</v>
+        <v>503</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>531</v>
+        <v>537</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>532</v>
+        <v>538</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -19185,139 +19431,139 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>533</v>
+        <v>539</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>534</v>
+        <v>540</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>535</v>
+        <v>541</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="37" t="s">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="F25" s="37" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>539</v>
+        <v>545</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>540</v>
+        <v>546</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>541</v>
+        <v>547</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="38" t="s">
-        <v>542</v>
+        <v>548</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>543</v>
+        <v>549</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="37" t="s">
-        <v>544</v>
+        <v>550</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>545</v>
+        <v>551</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>545</v>
+        <v>551</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>546</v>
+        <v>552</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>547</v>
+        <v>553</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>545</v>
+        <v>551</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>546</v>
+        <v>552</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>548</v>
+        <v>554</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>545</v>
+        <v>551</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>546</v>
+        <v>552</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>549</v>
+        <v>555</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>550</v>
+        <v>556</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>545</v>
+        <v>551</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>545</v>
+        <v>551</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>546</v>
+        <v>552</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>551</v>
+        <v>557</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="37" t="s">
-        <v>552</v>
+        <v>558</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>553</v>
+        <v>559</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="39" t="s">
-        <v>554</v>
+        <v>560</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>555</v>
+        <v>561</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="40" t="s">
-        <v>556</v>
+        <v>562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating End to end features file
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3040" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3034" uniqueCount="594">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1473,6 +1473,9 @@
     <t xml:space="preserve">TestCase_199</t>
   </si>
   <si>
+    <t xml:space="preserve">www.discovery.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Business Transaction</t>
   </si>
   <si>
@@ -1482,6 +1485,9 @@
     <t xml:space="preserve">TestCase_200</t>
   </si>
   <si>
+    <t xml:space="preserve">www.greenearth.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Operating Account</t>
   </si>
   <si>
@@ -1617,100 +1623,100 @@
     <t xml:space="preserve">11.0.0</t>
   </si>
   <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uiautomator2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://readuser:Re@d@1234@20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.5-06-12-2021-19:31.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.21-24-02-2022-13:09.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation-1-0-22-8-3-2022.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.19-02-02-2022-21:16.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://di</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_0003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPadPro3rdGen_iOS_15.3.0_b7060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://us.pcloudy.com/appiumcloud/wd/hub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.7.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPad_iOS_13.7.0_c08f6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.4.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPad8thGen_iOS_14.4.2_d5dd0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uiautomator2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://readuser:Re@d@1234@20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.5-06-12-2021-19:31.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.21-24-02-2022-13:09.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automation-1-0-22-8-3-2022.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.0.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.19-02-02-2022-21:16.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://di</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_0003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15.3.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPadPro3rdGen_iOS_15.3.0_b7060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://us.pcloudy.com/appiumcloud/wd/hub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.7.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPad_iOS_13.7.0_c08f6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14.4.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPad8thGen_iOS_14.4.2_d5dd0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
@@ -1918,9 +1924,6 @@
   <si>
     <t xml:space="preserve">e2e testdata</t>
   </si>
-  <si>
-    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.22-08-03-2022-16:32.apk</t>
-  </si>
 </sst>
 </file>
 
@@ -1935,7 +1938,7 @@
     <numFmt numFmtId="169" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="170" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2017,6 +2020,12 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2128,7 +2137,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2253,19 +2262,23 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2289,11 +2302,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2376,62 +2389,62 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A85" activeCellId="0" sqref="A85"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E156" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H163" activeCellId="0" sqref="H163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="14.33" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
-    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
-    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
-    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
-    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
-    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
-    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
-    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
-    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
-    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
-    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
-    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
-    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
-    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
-    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
-    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="991" max="1025" customWidth="true" hidden="false" style="4" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="4" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18825,7 +18838,7 @@
         <v>189</v>
       </c>
       <c r="T202" s="9" t="s">
-        <v>195</v>
+        <v>483</v>
       </c>
       <c r="U202" s="2" t="s">
         <v>473</v>
@@ -18849,7 +18862,7 @@
         <v>393</v>
       </c>
       <c r="AB202" s="17" t="n">
-        <v>190</v>
+        <v>75</v>
       </c>
       <c r="AC202" s="1" t="s">
         <v>419</v>
@@ -18892,10 +18905,10 @@
         <v>478</v>
       </c>
       <c r="AR202" s="9" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="AS202" s="9" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="AT202" s="9" t="n">
         <v>7898760</v>
@@ -18945,7 +18958,7 @@
         <v>481</v>
       </c>
       <c r="B203" s="9" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C203" s="9" t="s">
         <v>52</v>
@@ -18996,7 +19009,7 @@
         <v>189</v>
       </c>
       <c r="T203" s="9" t="s">
-        <v>195</v>
+        <v>487</v>
       </c>
       <c r="U203" s="2" t="s">
         <v>473</v>
@@ -19020,7 +19033,7 @@
         <v>393</v>
       </c>
       <c r="AB203" s="17" t="n">
-        <v>191</v>
+        <v>76</v>
       </c>
       <c r="AC203" s="1" t="s">
         <v>419</v>
@@ -19063,10 +19076,10 @@
         <v>478</v>
       </c>
       <c r="AR203" s="9" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="AS203" s="9" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="AT203" s="9" t="n">
         <v>8976432</v>
@@ -19089,7 +19102,7 @@
         <v>481</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C204" s="9" t="s">
         <v>52</v>
@@ -19212,7 +19225,7 @@
         <v>481</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C205" s="9" t="s">
         <v>52</v>
@@ -19335,7 +19348,7 @@
         <v>481</v>
       </c>
       <c r="B206" s="9" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="C206" s="9" t="s">
         <v>52</v>
@@ -19458,7 +19471,7 @@
         <v>481</v>
       </c>
       <c r="B207" s="9" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C207" s="9" t="s">
         <v>52</v>
@@ -19578,7 +19591,7 @@
         <v>481</v>
       </c>
       <c r="B208" s="9" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="C208" s="9" t="s">
         <v>52</v>
@@ -19693,7 +19706,7 @@
         <v>480</v>
       </c>
       <c r="AQ208" s="1" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="AR208" s="9"/>
       <c r="AS208" s="9"/>
@@ -19703,7 +19716,7 @@
         <v>481</v>
       </c>
       <c r="B209" s="9" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="C209" s="9" t="s">
         <v>52</v>
@@ -19828,7 +19841,7 @@
         <v>481</v>
       </c>
       <c r="B210" s="9" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C210" s="9" t="s">
         <v>52</v>
@@ -19953,7 +19966,7 @@
         <v>481</v>
       </c>
       <c r="B211" s="9" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="C211" s="9" t="s">
         <v>52</v>
@@ -20187,32 +20200,32 @@
   </sheetPr>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="11" width="12.57" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="11" width="5.18" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="4" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="11" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="11" width="20.5" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="11" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="11" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="11" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="13" customWidth="true" hidden="false" style="11" width="14.87" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="11" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="11" width="26.35" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="17" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="11" width="29.45" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="1025" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="11" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="11" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="26.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="11" width="9.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20223,97 +20236,90 @@
         <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="R1" s="21" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>516</v>
-      </c>
-      <c r="E2"/>
-      <c r="F2"/>
+        <v>518</v>
+      </c>
       <c r="G2" s="23" t="s">
-        <v>517</v>
-      </c>
-      <c r="H2"/>
+        <v>519</v>
+      </c>
       <c r="I2" s="23" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>519</v>
-      </c>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
+        <v>521</v>
+      </c>
       <c r="N2" s="25" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>521</v>
-      </c>
-      <c r="P2"/>
+        <v>523</v>
+      </c>
       <c r="Q2" s="24" t="n">
         <v>500</v>
       </c>
       <c r="R2" s="26" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="S2" s="24" t="n">
         <v>0</v>
@@ -20321,405 +20327,366 @@
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
+        <v>525</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>517</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>518</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>519</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>526</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>521</v>
+      </c>
+      <c r="N3" s="25" t="s">
+        <v>522</v>
+      </c>
+      <c r="O3" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>515</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>516</v>
-      </c>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3" s="22" t="s">
-        <v>517</v>
-      </c>
-      <c r="H3"/>
-      <c r="I3" s="27" t="s">
-        <v>524</v>
-      </c>
-      <c r="J3" s="27" t="s">
-        <v>519</v>
-      </c>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3" s="25" t="s">
-        <v>520</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>521</v>
-      </c>
-      <c r="P3"/>
       <c r="Q3" s="24" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="27" t="s">
-        <v>522</v>
-      </c>
-      <c r="S3" s="28" t="b">
+        <v>524</v>
+      </c>
+      <c r="S3" s="28" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="U3" s="29"/>
     </row>
-    <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="I4" s="31" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>592</v>
+        <v>536</v>
       </c>
       <c r="M4" s="33" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="N4" s="25" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>521</v>
-      </c>
-      <c r="P4"/>
+        <v>523</v>
+      </c>
       <c r="Q4" s="24" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>537</v>
-      </c>
-      <c r="S4" s="34" t="b">
+        <v>539</v>
+      </c>
+      <c r="S4" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
+        <v>540</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>529</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>530</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>531</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>534</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>535</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>543</v>
+      </c>
+      <c r="M5" s="33" t="s">
+        <v>537</v>
+      </c>
+      <c r="N5" s="25" t="s">
         <v>538</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>527</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>528</v>
-      </c>
-      <c r="F5" s="30" t="s">
-        <v>529</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>539</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>540</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>532</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>533</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>541</v>
-      </c>
-      <c r="M5" s="33" t="s">
-        <v>535</v>
-      </c>
-      <c r="N5" s="25" t="s">
-        <v>536</v>
-      </c>
       <c r="O5" s="12" t="s">
-        <v>521</v>
-      </c>
-      <c r="P5"/>
+        <v>523</v>
+      </c>
       <c r="Q5" s="24" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>537</v>
-      </c>
-      <c r="S5" s="34" t="b">
+        <v>539</v>
+      </c>
+      <c r="S5" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>530</v>
-      </c>
-      <c r="I6" s="31" t="s">
-        <v>543</v>
+        <v>532</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>533</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>532</v>
-      </c>
-      <c r="K6"/>
+        <v>534</v>
+      </c>
       <c r="L6" s="12" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M6" s="33" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="N6" s="25" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>521</v>
-      </c>
-      <c r="P6"/>
+        <v>523</v>
+      </c>
       <c r="Q6" s="24" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>537</v>
-      </c>
-      <c r="S6" s="34" t="b">
+        <v>539</v>
+      </c>
+      <c r="S6" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>530</v>
-      </c>
-      <c r="I7" s="31" t="s">
-        <v>543</v>
+        <v>532</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>533</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>532</v>
-      </c>
-      <c r="K7"/>
-      <c r="L7"/>
+        <v>534</v>
+      </c>
       <c r="M7" s="33" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="N7" s="25" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>521</v>
-      </c>
-      <c r="P7"/>
+        <v>523</v>
+      </c>
       <c r="Q7" s="24" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>537</v>
-      </c>
-      <c r="S7" s="34" t="b">
+        <v>539</v>
+      </c>
+      <c r="S7" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="H8" s="35" t="s">
-        <v>548</v>
+        <v>519</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>549</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>549</v>
-      </c>
-      <c r="J8" s="31" t="s">
         <v>550</v>
       </c>
-      <c r="K8" s="31" t="s">
+      <c r="J8" s="35" t="s">
         <v>551</v>
       </c>
+      <c r="K8" s="35" t="s">
+        <v>552</v>
+      </c>
       <c r="L8" s="11" t="s">
-        <v>552</v>
-      </c>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
+        <v>553</v>
+      </c>
       <c r="Q8" s="24" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>553</v>
-      </c>
-      <c r="S8" s="34" t="b">
+        <v>554</v>
+      </c>
+      <c r="S8" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>52</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="H9" s="35" t="s">
-        <v>555</v>
+        <v>519</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>556</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>556</v>
-      </c>
-      <c r="J9" s="31" t="s">
-        <v>550</v>
-      </c>
-      <c r="K9" s="36" t="s">
+        <v>557</v>
+      </c>
+      <c r="J9" s="35" t="s">
         <v>551</v>
       </c>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
+      <c r="K9" s="37" t="s">
+        <v>552</v>
+      </c>
       <c r="Q9" s="24" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>553</v>
-      </c>
-      <c r="S9" s="34" t="b">
+        <v>554</v>
+      </c>
+      <c r="S9" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10" s="35" t="s">
-        <v>557</v>
+      <c r="H10" s="36" t="s">
+        <v>558</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>558</v>
-      </c>
-      <c r="J10" s="31" t="s">
-        <v>550</v>
-      </c>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="N10"/>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
+        <v>559</v>
+      </c>
+      <c r="J10" s="35" t="s">
+        <v>551</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -20764,69 +20731,69 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="37" t="s">
-        <v>543</v>
+      <c r="B5" s="38" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="37" t="s">
-        <v>560</v>
+      <c r="B6" s="38" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="37" t="s">
-        <v>543</v>
+      <c r="B7" s="38" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="37" t="s">
-        <v>561</v>
+      <c r="B8" s="38" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="37" t="s">
-        <v>562</v>
+      <c r="B9" s="38" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="37" t="s">
-        <v>561</v>
+      <c r="B11" s="38" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="37" t="s">
-        <v>531</v>
+      <c r="B13" s="38" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -20835,139 +20802,139 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="38" t="s">
-        <v>569</v>
-      </c>
-      <c r="F25" s="38" t="s">
-        <v>570</v>
+      <c r="B25" s="39" t="s">
+        <v>571</v>
+      </c>
+      <c r="F25" s="39" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="39" t="s">
-        <v>575</v>
+      <c r="B31" s="40" t="s">
+        <v>577</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="38" t="s">
-        <v>577</v>
+      <c r="B32" s="39" t="s">
+        <v>579</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
+        <v>584</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>580</v>
+      </c>
+      <c r="F35" s="0" t="s">
         <v>582</v>
       </c>
-      <c r="E35" s="0" t="s">
-        <v>578</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>580</v>
-      </c>
       <c r="G35" s="0" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="38" t="s">
-        <v>586</v>
+      <c r="B44" s="39" t="s">
+        <v>588</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="40" t="s">
-        <v>588</v>
+      <c r="B45" s="41" t="s">
+        <v>590</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="41" t="s">
-        <v>590</v>
+      <c r="B46" s="42" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20975,7 +20942,7 @@
         <v>197198</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made chages in excel sheet
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3041" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3036" uniqueCount="595">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1926,9 +1926,6 @@
   </si>
   <si>
     <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.22-08-03-2022-16:32.apk</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
 </sst>
 </file>
@@ -2395,8 +2392,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E156" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H163" activeCellId="0" sqref="H163"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R196" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T201" activeCellId="0" sqref="T201:T202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18788,7 +18785,7 @@
       <c r="AW201" s="16"/>
       <c r="AX201" s="9"/>
     </row>
-    <row r="202" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="9" t="s">
         <v>481</v>
       </c>
@@ -20211,7 +20208,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="F5" activeCellId="1" sqref="T201:T202 F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20646,7 +20643,7 @@
         <v>552</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>595</v>
+        <v>553</v>
       </c>
       <c r="M8"/>
       <c r="N8"/>
@@ -20777,8 +20774,8 @@
   </sheetPr>
   <dimension ref="A4:G50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A50" activeCellId="1" sqref="T201:T202 A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
made changes in IOS utility class
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3036" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3034" uniqueCount="594">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1923,9 +1923,6 @@
   </si>
   <si>
     <t xml:space="preserve">e2e testdata</t>
-  </si>
-  <si>
-    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.22-08-03-2022-16:32.apk</t>
   </si>
 </sst>
 </file>
@@ -2392,62 +2389,62 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R196" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T201" activeCellId="0" sqref="T201:T202"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J199" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T201" activeCellId="0" sqref="T201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="14.33" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
-    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
-    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
-    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
-    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
-    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
-    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
-    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
-    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
-    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
-    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
-    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
-    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
-    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
-    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
-    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="991" max="1025" customWidth="true" hidden="false" style="4" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="4" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20203,32 +20200,32 @@
   </sheetPr>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="F5" activeCellId="1" sqref="T201:T202 F5"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="11" width="12.57" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="11" width="5.18" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="4" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="11" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="11" width="20.5" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="11" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="11" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="11" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="13" customWidth="true" hidden="false" style="11" width="14.87" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="11" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="11" width="26.35" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="17" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="11" width="29.45" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="1025" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="11" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="11" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="26.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="11" width="9.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20303,28 +20300,21 @@
       <c r="D2" s="23" t="s">
         <v>518</v>
       </c>
-      <c r="E2"/>
-      <c r="F2"/>
       <c r="G2" s="23" t="s">
         <v>519</v>
       </c>
-      <c r="H2"/>
       <c r="I2" s="23" t="s">
         <v>520</v>
       </c>
       <c r="J2" s="24" t="s">
         <v>521</v>
       </c>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
       <c r="N2" s="25" t="s">
         <v>522</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="P2"/>
       <c r="Q2" s="24" t="n">
         <v>500</v>
       </c>
@@ -20348,35 +20338,28 @@
       <c r="D3" s="22" t="s">
         <v>518</v>
       </c>
-      <c r="E3"/>
-      <c r="F3"/>
       <c r="G3" s="22" t="s">
         <v>519</v>
       </c>
-      <c r="H3"/>
       <c r="I3" s="27" t="s">
         <v>526</v>
       </c>
       <c r="J3" s="27" t="s">
         <v>521</v>
       </c>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
       <c r="N3" s="25" t="s">
         <v>522</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="P3"/>
       <c r="Q3" s="24" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="27" t="s">
         <v>524</v>
       </c>
-      <c r="S3" s="28" t="b">
+      <c r="S3" s="28" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20417,7 +20400,7 @@
         <v>535</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>594</v>
+        <v>536</v>
       </c>
       <c r="M4" s="33" t="s">
         <v>537</v>
@@ -20428,14 +20411,13 @@
       <c r="O4" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="P4"/>
       <c r="Q4" s="24" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S4" s="34" t="b">
+      <c r="S4" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20486,14 +20468,13 @@
       <c r="O5" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="P5"/>
       <c r="Q5" s="24" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S5" s="34" t="b">
+      <c r="S5" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20529,7 +20510,6 @@
       <c r="J6" s="9" t="s">
         <v>534</v>
       </c>
-      <c r="K6"/>
       <c r="L6" s="12" t="s">
         <v>545</v>
       </c>
@@ -20542,14 +20522,13 @@
       <c r="O6" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="P6"/>
       <c r="Q6" s="24" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S6" s="34" t="b">
+      <c r="S6" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20585,8 +20564,6 @@
       <c r="J7" s="9" t="s">
         <v>534</v>
       </c>
-      <c r="K7"/>
-      <c r="L7"/>
       <c r="M7" s="33" t="s">
         <v>537</v>
       </c>
@@ -20596,14 +20573,13 @@
       <c r="O7" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="P7"/>
       <c r="Q7" s="24" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S7" s="34" t="b">
+      <c r="S7" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20645,17 +20621,13 @@
       <c r="L8" s="11" t="s">
         <v>553</v>
       </c>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
       <c r="Q8" s="24" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>554</v>
       </c>
-      <c r="S8" s="34" t="b">
+      <c r="S8" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20694,30 +20666,18 @@
       <c r="K9" s="37" t="s">
         <v>552</v>
       </c>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
       <c r="Q9" s="24" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>554</v>
       </c>
-      <c r="S9" s="34" t="b">
+      <c r="S9" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
       <c r="H10" s="36" t="s">
         <v>558</v>
       </c>
@@ -20727,15 +20687,6 @@
       <c r="J10" s="35" t="s">
         <v>551</v>
       </c>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="N10"/>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -20775,14 +20726,14 @@
   <dimension ref="A4:G50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="1" sqref="T201:T202 A50"/>
+      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updating apk url ver 22
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3034" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3102" uniqueCount="596">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1923,6 +1923,12 @@
   </si>
   <si>
     <t xml:space="preserve">e2e testdata</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.22-08-03-2022-16:32.apk</t>
   </si>
 </sst>
 </file>
@@ -2395,56 +2401,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="4" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="14.33" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
+    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
+    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
+    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
+    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
+    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
+    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
+    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
+    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
+    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
+    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
+    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
+    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
+    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
+    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="991" max="1025" customWidth="true" hidden="false" style="4" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20210,22 +20216,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="5.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="11" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="11" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="26.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="11" width="9.17"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="11" width="12.57" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="11" width="5.18" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="4" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="11" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="11" width="20.5" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="11" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="11" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="11" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="13" customWidth="true" hidden="false" style="11" width="14.87" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="11" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="11" width="26.35" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="17" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="11" width="29.45" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="1025" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20300,21 +20306,28 @@
       <c r="D2" s="23" t="s">
         <v>518</v>
       </c>
+      <c r="E2"/>
+      <c r="F2"/>
       <c r="G2" s="23" t="s">
         <v>519</v>
       </c>
+      <c r="H2"/>
       <c r="I2" s="23" t="s">
         <v>520</v>
       </c>
       <c r="J2" s="24" t="s">
         <v>521</v>
       </c>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
       <c r="N2" s="25" t="s">
         <v>522</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>523</v>
       </c>
+      <c r="P2"/>
       <c r="Q2" s="24" t="n">
         <v>500</v>
       </c>
@@ -20338,28 +20351,35 @@
       <c r="D3" s="22" t="s">
         <v>518</v>
       </c>
+      <c r="E3"/>
+      <c r="F3"/>
       <c r="G3" s="22" t="s">
         <v>519</v>
       </c>
+      <c r="H3"/>
       <c r="I3" s="27" t="s">
         <v>526</v>
       </c>
       <c r="J3" s="27" t="s">
         <v>521</v>
       </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
       <c r="N3" s="25" t="s">
         <v>522</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>523</v>
       </c>
+      <c r="P3"/>
       <c r="Q3" s="24" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="27" t="s">
         <v>524</v>
       </c>
-      <c r="S3" s="28" t="n">
+      <c r="S3" s="28" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20400,7 +20420,7 @@
         <v>535</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>536</v>
+        <v>595</v>
       </c>
       <c r="M4" s="33" t="s">
         <v>537</v>
@@ -20411,13 +20431,14 @@
       <c r="O4" s="12" t="s">
         <v>523</v>
       </c>
+      <c r="P4"/>
       <c r="Q4" s="24" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S4" s="34" t="n">
+      <c r="S4" s="34" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20468,13 +20489,14 @@
       <c r="O5" s="12" t="s">
         <v>523</v>
       </c>
+      <c r="P5"/>
       <c r="Q5" s="24" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S5" s="34" t="n">
+      <c r="S5" s="34" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20510,6 +20532,7 @@
       <c r="J6" s="9" t="s">
         <v>534</v>
       </c>
+      <c r="K6"/>
       <c r="L6" s="12" t="s">
         <v>545</v>
       </c>
@@ -20522,13 +20545,14 @@
       <c r="O6" s="12" t="s">
         <v>523</v>
       </c>
+      <c r="P6"/>
       <c r="Q6" s="24" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S6" s="34" t="n">
+      <c r="S6" s="34" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20564,6 +20588,8 @@
       <c r="J7" s="9" t="s">
         <v>534</v>
       </c>
+      <c r="K7"/>
+      <c r="L7"/>
       <c r="M7" s="33" t="s">
         <v>537</v>
       </c>
@@ -20573,13 +20599,14 @@
       <c r="O7" s="12" t="s">
         <v>523</v>
       </c>
+      <c r="P7"/>
       <c r="Q7" s="24" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S7" s="34" t="n">
+      <c r="S7" s="34" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20619,15 +20646,19 @@
         <v>552</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>553</v>
-      </c>
+        <v>594</v>
+      </c>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
       <c r="Q8" s="24" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>554</v>
       </c>
-      <c r="S8" s="34" t="n">
+      <c r="S8" s="34" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20666,18 +20697,30 @@
       <c r="K9" s="37" t="s">
         <v>552</v>
       </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
       <c r="Q9" s="24" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>554</v>
       </c>
-      <c r="S9" s="34" t="n">
+      <c r="S9" s="34" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
       <c r="H10" s="36" t="s">
         <v>558</v>
       </c>
@@ -20687,6 +20730,15 @@
       <c r="J10" s="35" t="s">
         <v>551</v>
       </c>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -20731,9 +20783,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
made changes in product object class
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3102" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3034" uniqueCount="594">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1635,7 +1635,7 @@
     <t xml:space="preserve">https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.21-24-02-2022-13:09.apk</t>
   </si>
   <si>
-    <t xml:space="preserve">Automation-1-0-22-8-3-2022.apk</t>
+    <t xml:space="preserve">Automation-1-0-22-10-3-2022.apk</t>
   </si>
   <si>
     <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
@@ -1923,12 +1923,6 @@
   </si>
   <si>
     <t xml:space="preserve">e2e testdata</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.22-08-03-2022-16:32.apk</t>
   </si>
 </sst>
 </file>
@@ -2401,56 +2395,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="14.33" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
-    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
-    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
-    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
-    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
-    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
-    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
-    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
-    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
-    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
-    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
-    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
-    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
-    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
-    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
-    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="991" max="1025" customWidth="true" hidden="false" style="4" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="4" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20207,31 +20201,31 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="L8" activeCellId="0" sqref="L8"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="11" width="12.57" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="11" width="5.18" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="4" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="11" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="11" width="20.5" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="11" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="11" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="11" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="13" customWidth="true" hidden="false" style="11" width="14.87" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="11" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="11" width="26.35" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="17" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="11" width="29.45" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="1025" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="11" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="11" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="26.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="11" width="9.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20306,28 +20300,21 @@
       <c r="D2" s="23" t="s">
         <v>518</v>
       </c>
-      <c r="E2"/>
-      <c r="F2"/>
       <c r="G2" s="23" t="s">
         <v>519</v>
       </c>
-      <c r="H2"/>
       <c r="I2" s="23" t="s">
         <v>520</v>
       </c>
       <c r="J2" s="24" t="s">
         <v>521</v>
       </c>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
       <c r="N2" s="25" t="s">
         <v>522</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="P2"/>
       <c r="Q2" s="24" t="n">
         <v>500</v>
       </c>
@@ -20351,41 +20338,34 @@
       <c r="D3" s="22" t="s">
         <v>518</v>
       </c>
-      <c r="E3"/>
-      <c r="F3"/>
       <c r="G3" s="22" t="s">
         <v>519</v>
       </c>
-      <c r="H3"/>
       <c r="I3" s="27" t="s">
         <v>526</v>
       </c>
       <c r="J3" s="27" t="s">
         <v>521</v>
       </c>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
       <c r="N3" s="25" t="s">
         <v>522</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="P3"/>
       <c r="Q3" s="24" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="27" t="s">
         <v>524</v>
       </c>
-      <c r="S3" s="28" t="b">
+      <c r="S3" s="28" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="U3" s="29"/>
     </row>
-    <row r="4" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
         <v>527</v>
       </c>
@@ -20420,7 +20400,7 @@
         <v>535</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>595</v>
+        <v>536</v>
       </c>
       <c r="M4" s="33" t="s">
         <v>537</v>
@@ -20431,14 +20411,13 @@
       <c r="O4" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="P4"/>
       <c r="Q4" s="24" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S4" s="34" t="b">
+      <c r="S4" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20489,14 +20468,13 @@
       <c r="O5" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="P5"/>
       <c r="Q5" s="24" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S5" s="34" t="b">
+      <c r="S5" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20532,7 +20510,6 @@
       <c r="J6" s="9" t="s">
         <v>534</v>
       </c>
-      <c r="K6"/>
       <c r="L6" s="12" t="s">
         <v>545</v>
       </c>
@@ -20545,14 +20522,13 @@
       <c r="O6" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="P6"/>
       <c r="Q6" s="24" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S6" s="34" t="b">
+      <c r="S6" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20588,8 +20564,6 @@
       <c r="J7" s="9" t="s">
         <v>534</v>
       </c>
-      <c r="K7"/>
-      <c r="L7"/>
       <c r="M7" s="33" t="s">
         <v>537</v>
       </c>
@@ -20599,14 +20573,13 @@
       <c r="O7" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="P7"/>
       <c r="Q7" s="24" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S7" s="34" t="b">
+      <c r="S7" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20646,19 +20619,15 @@
         <v>552</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>594</v>
-      </c>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
+        <v>553</v>
+      </c>
       <c r="Q8" s="24" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>554</v>
       </c>
-      <c r="S8" s="34" t="b">
+      <c r="S8" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20697,30 +20666,18 @@
       <c r="K9" s="37" t="s">
         <v>552</v>
       </c>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
       <c r="Q9" s="24" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>554</v>
       </c>
-      <c r="S9" s="34" t="b">
+      <c r="S9" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
       <c r="H10" s="36" t="s">
         <v>558</v>
       </c>
@@ -20730,15 +20687,6 @@
       <c r="J10" s="35" t="s">
         <v>551</v>
       </c>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="N10"/>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -20783,9 +20731,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
made change in Login page objects
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3034" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3037" uniqueCount="596">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1647,75 +1647,75 @@
     <t xml:space="preserve">Android_002</t>
   </si>
   <si>
-    <t xml:space="preserve">9.0.0</t>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabA8_Android_11.0.0_31b61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.19-02-02-2022-21:16.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://di</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_0003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPadPro3rdGen_iOS_15.3.0_b7060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://us.pcloudy.com/appiumcloud/wd/hub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.7.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPad_iOS_13.7.0_c08f6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.4.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPad8thGen_iOS_14.4.2_d5dd0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
   </si>
   <si>
-    <t xml:space="preserve">https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.19-02-02-2022-21:16.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://di</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_0003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15.3.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPadPro3rdGen_iOS_15.3.0_b7060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">null</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://us.pcloudy.com/appiumcloud/wd/hub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.7.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPad_iOS_13.7.0_c08f6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14.4.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPad8thGen_iOS_14.4.2_d5dd0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
-  </si>
-  <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
   </si>
   <si>
@@ -1726,6 +1726,12 @@
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyM12_Android_11.0.0_df6a7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-Westbangal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ind-west.pcloudy.com/appiumcloud/wd/hub</t>
   </si>
   <si>
     <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
@@ -1938,7 +1944,7 @@
     <numFmt numFmtId="169" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="170" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1985,6 +1991,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2022,23 +2034,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF067D17"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF067D17"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2137,7 +2137,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2218,11 +2218,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2242,11 +2246,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2258,11 +2262,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2270,15 +2274,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2286,11 +2282,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2302,11 +2298,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2389,8 +2385,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J199" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T201" activeCellId="0" sqref="T201"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D203" activeCellId="0" sqref="D203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18953,7 +18949,7 @@
       <c r="BX202" s="9"/>
       <c r="BY202" s="9"/>
     </row>
-    <row r="203" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="9" t="s">
         <v>481</v>
       </c>
@@ -18966,7 +18962,7 @@
       <c r="D203" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E203" s="9" t="s">
+      <c r="E203" s="20" t="s">
         <v>62</v>
       </c>
       <c r="F203" s="1" t="s">
@@ -20201,11 +20197,11 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20241,10 +20237,10 @@
       <c r="D1" s="5" t="s">
         <v>500</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="21" t="s">
         <v>501</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="21" t="s">
         <v>502</v>
       </c>
       <c r="G1" s="5" t="s">
@@ -20280,7 +20276,7 @@
       <c r="Q1" s="5" t="s">
         <v>513</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="R1" s="22" t="s">
         <v>514</v>
       </c>
       <c r="S1" s="5" t="s">
@@ -20288,82 +20284,82 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>516</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>517</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="24" t="s">
         <v>518</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="24" t="s">
         <v>519</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="24" t="s">
         <v>520</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="25" t="s">
         <v>521</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="26" t="s">
         <v>522</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="Q2" s="24" t="n">
+      <c r="Q2" s="25" t="n">
         <v>500</v>
       </c>
-      <c r="R2" s="26" t="s">
+      <c r="R2" s="27" t="s">
         <v>524</v>
       </c>
-      <c r="S2" s="24" t="n">
+      <c r="S2" s="25" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>525</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="22" t="s">
+      <c r="B3" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>517</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="23" t="s">
         <v>518</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="23" t="s">
         <v>519</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="28" t="s">
         <v>526</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="28" t="s">
         <v>521</v>
       </c>
-      <c r="N3" s="25" t="s">
+      <c r="N3" s="26" t="s">
         <v>522</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="Q3" s="24" t="n">
+      <c r="Q3" s="25" t="n">
         <v>501</v>
       </c>
-      <c r="R3" s="27" t="s">
+      <c r="R3" s="28" t="s">
         <v>524</v>
       </c>
-      <c r="S3" s="28" t="n">
+      <c r="S3" s="29" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="U3" s="29"/>
+      <c r="U3" s="30"/>
     </row>
     <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
@@ -20378,10 +20374,10 @@
       <c r="D4" s="9" t="s">
         <v>529</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="31" t="s">
         <v>530</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="31" t="s">
         <v>531</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -20390,7 +20386,7 @@
       <c r="H4" s="9" t="s">
         <v>532</v>
       </c>
-      <c r="I4" s="31" t="s">
+      <c r="I4" s="32" t="s">
         <v>533</v>
       </c>
       <c r="J4" s="9" t="s">
@@ -20399,19 +20395,19 @@
       <c r="K4" s="9" t="s">
         <v>535</v>
       </c>
-      <c r="L4" s="32" t="s">
+      <c r="L4" s="33" t="s">
         <v>536</v>
       </c>
-      <c r="M4" s="33" t="s">
+      <c r="M4" s="12" t="s">
         <v>537</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="26" t="s">
         <v>538</v>
       </c>
       <c r="O4" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="Q4" s="24" t="n">
+      <c r="Q4" s="25" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="9" t="s">
@@ -20422,7 +20418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>540</v>
       </c>
@@ -20435,20 +20431,20 @@
       <c r="D5" s="9" t="s">
         <v>529</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="31" t="s">
         <v>530</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="31" t="s">
         <v>531</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>519</v>
       </c>
       <c r="H5" s="9" t="s">
+        <v>532</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>541</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>542</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>534</v>
@@ -20457,18 +20453,18 @@
         <v>535</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>543</v>
-      </c>
-      <c r="M5" s="33" t="s">
+        <v>542</v>
+      </c>
+      <c r="M5" s="12" t="s">
         <v>537</v>
       </c>
-      <c r="N5" s="25" t="s">
+      <c r="N5" s="26" t="s">
         <v>538</v>
       </c>
       <c r="O5" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="Q5" s="24" t="n">
+      <c r="Q5" s="25" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="9" t="s">
@@ -20481,7 +20477,7 @@
     </row>
     <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>52</v>
@@ -20492,10 +20488,10 @@
       <c r="D6" s="9" t="s">
         <v>529</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="31" t="s">
         <v>530</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="31" t="s">
         <v>531</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -20504,25 +20500,25 @@
       <c r="H6" s="9" t="s">
         <v>532</v>
       </c>
-      <c r="I6" s="35" t="s">
+      <c r="I6" s="32" t="s">
         <v>533</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>534</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>545</v>
-      </c>
-      <c r="M6" s="33" t="s">
+        <v>544</v>
+      </c>
+      <c r="M6" s="12" t="s">
         <v>537</v>
       </c>
-      <c r="N6" s="25" t="s">
+      <c r="N6" s="26" t="s">
         <v>538</v>
       </c>
       <c r="O6" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="Q6" s="24" t="n">
+      <c r="Q6" s="25" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="9" t="s">
@@ -20535,7 +20531,7 @@
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>52</v>
@@ -20546,10 +20542,10 @@
       <c r="D7" s="9" t="s">
         <v>529</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="31" t="s">
         <v>530</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="31" t="s">
         <v>531</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -20558,22 +20554,22 @@
       <c r="H7" s="9" t="s">
         <v>532</v>
       </c>
-      <c r="I7" s="35" t="s">
+      <c r="I7" s="32" t="s">
         <v>533</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>534</v>
       </c>
-      <c r="M7" s="33" t="s">
+      <c r="M7" s="12" t="s">
         <v>537</v>
       </c>
-      <c r="N7" s="25" t="s">
+      <c r="N7" s="26" t="s">
         <v>522</v>
       </c>
       <c r="O7" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="Q7" s="24" t="n">
+      <c r="Q7" s="25" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="9" t="s">
@@ -20586,7 +20582,7 @@
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>52</v>
@@ -20595,37 +20591,37 @@
         <v>528</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>548</v>
-      </c>
-      <c r="E8" s="30" t="s">
+        <v>547</v>
+      </c>
+      <c r="E8" s="31" t="s">
         <v>530</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="31" t="s">
         <v>531</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="35" t="s">
+        <v>548</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>549</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="J8" s="32" t="s">
         <v>550</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="K8" s="32" t="s">
         <v>551</v>
       </c>
-      <c r="K8" s="35" t="s">
+      <c r="L8" s="11" t="s">
         <v>552</v>
       </c>
-      <c r="L8" s="11" t="s">
+      <c r="Q8" s="25" t="n">
+        <v>506</v>
+      </c>
+      <c r="R8" s="9" t="s">
         <v>553</v>
-      </c>
-      <c r="Q8" s="24" t="n">
-        <v>506</v>
-      </c>
-      <c r="R8" s="9" t="s">
-        <v>554</v>
       </c>
       <c r="S8" s="34" t="n">
         <f aca="false">FALSE()</f>
@@ -20634,7 +20630,7 @@
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>52</v>
@@ -20643,34 +20639,34 @@
         <v>528</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>548</v>
-      </c>
-      <c r="E9" s="30" t="s">
+        <v>547</v>
+      </c>
+      <c r="E9" s="31" t="s">
         <v>530</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="31" t="s">
         <v>531</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="35" t="s">
+        <v>555</v>
+      </c>
+      <c r="I9" s="9" t="s">
         <v>556</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>557</v>
-      </c>
-      <c r="J9" s="35" t="s">
+      <c r="J9" s="32" t="s">
+        <v>550</v>
+      </c>
+      <c r="K9" s="36" t="s">
         <v>551</v>
       </c>
-      <c r="K9" s="37" t="s">
-        <v>552</v>
-      </c>
-      <c r="Q9" s="24" t="n">
+      <c r="Q9" s="25" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="S9" s="34" t="n">
         <f aca="false">FALSE()</f>
@@ -20678,14 +20674,14 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H10" s="36" t="s">
+      <c r="H10" s="35" t="s">
+        <v>557</v>
+      </c>
+      <c r="I10" s="9" t="s">
         <v>558</v>
       </c>
-      <c r="I10" s="9" t="s">
-        <v>559</v>
-      </c>
-      <c r="J10" s="35" t="s">
-        <v>551</v>
+      <c r="J10" s="32" t="s">
+        <v>550</v>
       </c>
     </row>
   </sheetData>
@@ -20723,10 +20719,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:G50"/>
+  <dimension ref="A4:H50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20738,46 +20734,46 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="37" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="37" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="38" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="37" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="38" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="37" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="38" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="38" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="37" t="s">
         <v>562</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="38" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>542</v>
+        <v>563</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="38" t="s">
-        <v>562</v>
+      <c r="B11" s="37" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="37" t="s">
         <v>564</v>
       </c>
     </row>
@@ -20798,143 +20794,153 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>541</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>568</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>569</v>
+      </c>
+    </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="39" t="s">
-        <v>571</v>
-      </c>
-      <c r="F25" s="39" t="s">
-        <v>572</v>
+      <c r="B25" s="38" t="s">
+        <v>573</v>
+      </c>
+      <c r="F25" s="38" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="40" t="s">
-        <v>577</v>
+      <c r="B31" s="39" t="s">
+        <v>579</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="39" t="s">
-        <v>579</v>
+      <c r="B32" s="38" t="s">
+        <v>581</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
+        <v>586</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>582</v>
+      </c>
+      <c r="F35" s="0" t="s">
         <v>584</v>
       </c>
-      <c r="E35" s="0" t="s">
-        <v>580</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>582</v>
-      </c>
       <c r="G35" s="0" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="39" t="s">
-        <v>588</v>
+      <c r="B44" s="38" t="s">
+        <v>590</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="41" t="s">
-        <v>590</v>
+      <c r="B45" s="40" t="s">
+        <v>592</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="42" t="s">
-        <v>592</v>
+      <c r="B46" s="41" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20942,10 +20948,13 @@
         <v>197198</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H19" r:id="rId1" display="https://ind-west.pcloudy.com/appiumcloud/wd/hub"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
made changes in product feature file
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3037" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3041" uniqueCount="596">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -2385,8 +2385,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D203" activeCellId="0" sqref="D203"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A203" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E205" activeCellId="0" sqref="E205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19093,7 +19093,7 @@
         <v>99910</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="9" t="s">
         <v>481</v>
       </c>
@@ -19215,8 +19215,11 @@
       <c r="AQ204" s="1" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="205" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AR204" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="231" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="9" t="s">
         <v>481</v>
       </c>
@@ -19339,7 +19342,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="9" t="s">
         <v>481</v>
       </c>
@@ -19461,6 +19464,9 @@
       <c r="AQ206" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="AR206" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="207" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="9" t="s">
@@ -19582,7 +19588,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="9" t="s">
         <v>481</v>
       </c>
@@ -19704,7 +19710,9 @@
       <c r="AQ208" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="AR208" s="9"/>
+      <c r="AR208" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="AS208" s="9"/>
     </row>
     <row r="209" customFormat="false" ht="231" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19829,7 +19837,9 @@
       <c r="AQ209" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AR209" s="9"/>
+      <c r="AR209" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="AS209" s="9"/>
     </row>
     <row r="210" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20196,11 +20206,11 @@
   </sheetPr>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
       <selection pane="bottomRight" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated exeption product mangement
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -2385,8 +2385,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A203" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E205" activeCellId="0" sqref="E205"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A152" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E160" activeCellId="0" sqref="E160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
made changes in wait utility classes
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3041" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3114" uniqueCount="604">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1224,6 +1224,9 @@
     <t xml:space="preserve">TestCase_158</t>
   </si>
   <si>
+    <t xml:space="preserve">transfer fund</t>
+  </si>
+  <si>
     <t xml:space="preserve">Home page -invalid username</t>
   </si>
   <si>
@@ -1519,6 +1522,24 @@
   </si>
   <si>
     <t xml:space="preserve">TestCase_208</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS-Country code Validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_212</t>
   </si>
   <si>
     <t xml:space="preserve">mode</t>
@@ -1929,6 +1950,9 @@
   </si>
   <si>
     <t xml:space="preserve">e2e testdata</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -2385,62 +2409,62 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A152" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E160" activeCellId="0" sqref="E160"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A156" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A163" activeCellId="0" sqref="A163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="4" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="14.33" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
+    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
+    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
+    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
+    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
+    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
+    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
+    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
+    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
+    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
+    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
+    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
+    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
+    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
+    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="991" max="1025" customWidth="true" hidden="false" style="4" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16117,7 +16141,7 @@
       <c r="AI160" s="9"/>
       <c r="AJ160" s="9"/>
     </row>
-    <row r="161" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="9" t="s">
         <v>398</v>
       </c>
@@ -16161,7 +16185,7 @@
       <c r="Y161" s="9"/>
       <c r="Z161" s="9"/>
       <c r="AA161" s="9" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="AB161" s="17" t="n">
         <v>34</v>
@@ -16177,10 +16201,10 @@
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B162" s="9" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C162" s="9" t="s">
         <v>52</v>
@@ -16200,10 +16224,10 @@
     </row>
     <row r="163" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C163" s="9" t="s">
         <v>52</v>
@@ -16218,15 +16242,15 @@
         <v>103</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B164" s="9" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C164" s="9" t="s">
         <v>52</v>
@@ -16246,10 +16270,10 @@
     </row>
     <row r="165" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B165" s="9" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C165" s="9" t="s">
         <v>52</v>
@@ -16264,15 +16288,15 @@
         <v>103</v>
       </c>
       <c r="H165" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B166" s="9" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C166" s="9" t="s">
         <v>52</v>
@@ -16287,7 +16311,7 @@
         <v>104</v>
       </c>
       <c r="H166" s="9" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I166" s="9" t="s">
         <v>93</v>
@@ -16340,10 +16364,10 @@
     </row>
     <row r="167" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B167" s="9" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C167" s="9" t="s">
         <v>52</v>
@@ -16358,7 +16382,7 @@
         <v>104</v>
       </c>
       <c r="H167" s="9" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I167" s="9" t="s">
         <v>93</v>
@@ -16411,10 +16435,10 @@
     </row>
     <row r="168" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B168" s="9" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C168" s="9" t="s">
         <v>52</v>
@@ -16429,7 +16453,7 @@
         <v>105</v>
       </c>
       <c r="H168" s="9" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I168" s="9" t="s">
         <v>93</v>
@@ -16482,10 +16506,10 @@
     </row>
     <row r="169" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B169" s="9" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C169" s="9" t="s">
         <v>52</v>
@@ -16500,7 +16524,7 @@
         <v>105</v>
       </c>
       <c r="H169" s="9" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I169" s="9" t="s">
         <v>93</v>
@@ -16556,7 +16580,7 @@
         <v>90</v>
       </c>
       <c r="B170" s="9" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C170" s="9" t="s">
         <v>52</v>
@@ -16598,7 +16622,7 @@
         <v>287</v>
       </c>
       <c r="B171" s="9" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C171" s="9" t="s">
         <v>52</v>
@@ -16635,10 +16659,10 @@
     </row>
     <row r="172" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C172" s="9" t="s">
         <v>52</v>
@@ -16653,7 +16677,7 @@
         <v>105</v>
       </c>
       <c r="H172" s="9" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I172" s="9" t="s">
         <v>93</v>
@@ -16704,27 +16728,27 @@
         <v>12</v>
       </c>
       <c r="AC172" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AD172" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="AE172" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="AF172" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="AG172" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B173" s="9" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C173" s="9" t="s">
         <v>52</v>
@@ -16739,7 +16763,7 @@
         <v>105</v>
       </c>
       <c r="H173" s="9" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I173" s="9" t="s">
         <v>93</v>
@@ -16790,27 +16814,27 @@
         <v>12</v>
       </c>
       <c r="AC173" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AD173" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="AE173" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="AF173" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AG173" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C174" s="9" t="s">
         <v>52</v>
@@ -16825,7 +16849,7 @@
         <v>105</v>
       </c>
       <c r="H174" s="9" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I174" s="9" t="s">
         <v>93</v>
@@ -16876,27 +16900,27 @@
         <v>12</v>
       </c>
       <c r="AC174" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AD174" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="AE174" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="AF174" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AG174" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B175" s="9" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C175" s="9" t="s">
         <v>52</v>
@@ -16911,7 +16935,7 @@
         <v>105</v>
       </c>
       <c r="H175" s="9" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I175" s="9" t="s">
         <v>93</v>
@@ -16962,19 +16986,19 @@
         <v>12</v>
       </c>
       <c r="AC175" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AD175" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="AE175" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="AF175" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AG175" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16982,7 +17006,7 @@
         <v>391</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C176" s="9" t="s">
         <v>52</v>
@@ -17019,7 +17043,7 @@
       <c r="Y176" s="9"/>
       <c r="Z176" s="9"/>
       <c r="AA176" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AB176" s="17" t="n">
         <v>189</v>
@@ -17035,10 +17059,10 @@
     </row>
     <row r="177" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="9" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B177" s="9" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C177" s="9" t="s">
         <v>52</v>
@@ -17075,7 +17099,7 @@
       <c r="Y177" s="9"/>
       <c r="Z177" s="9"/>
       <c r="AA177" s="9" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AB177" s="17" t="n">
         <v>129</v>
@@ -17091,10 +17115,10 @@
     </row>
     <row r="178" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="9" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C178" s="9" t="s">
         <v>52</v>
@@ -17148,7 +17172,7 @@
         <v>396</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C179" s="9" t="s">
         <v>52</v>
@@ -17187,7 +17211,7 @@
       <c r="Y179" s="9"/>
       <c r="Z179" s="9"/>
       <c r="AA179" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AB179" s="17" t="n">
         <v>555</v>
@@ -17206,7 +17230,7 @@
         <v>398</v>
       </c>
       <c r="B180" s="9" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C180" s="9" t="s">
         <v>52</v>
@@ -17245,7 +17269,7 @@
       <c r="Y180" s="9"/>
       <c r="Z180" s="9"/>
       <c r="AA180" s="9" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AB180" s="17" t="n">
         <v>345</v>
@@ -17264,7 +17288,7 @@
         <v>398</v>
       </c>
       <c r="B181" s="9" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C181" s="9" t="s">
         <v>52</v>
@@ -17317,10 +17341,10 @@
     </row>
     <row r="182" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B182" s="9" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C182" s="9" t="s">
         <v>52</v>
@@ -17357,7 +17381,7 @@
       <c r="Y182" s="9"/>
       <c r="Z182" s="9"/>
       <c r="AA182" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AB182" s="17" t="n">
         <v>189</v>
@@ -17374,10 +17398,10 @@
     </row>
     <row r="183" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C183" s="9" t="s">
         <v>52</v>
@@ -17414,7 +17438,7 @@
       <c r="Y183" s="9"/>
       <c r="Z183" s="9"/>
       <c r="AA183" s="9" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AB183" s="17" t="n">
         <v>129</v>
@@ -17425,21 +17449,21 @@
       <c r="AF183" s="9"/>
       <c r="AG183" s="9"/>
       <c r="AH183" s="17" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="AI183" s="17" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="AJ183" s="9" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C184" s="9" t="s">
         <v>52</v>
@@ -17485,21 +17509,21 @@
       <c r="AF184" s="9"/>
       <c r="AG184" s="9"/>
       <c r="AH184" s="17" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AI184" s="17" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AJ184" s="17" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C185" s="9" t="s">
         <v>52</v>
@@ -17550,18 +17574,18 @@
         <v>12345</v>
       </c>
       <c r="AI185" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ185" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C186" s="9" t="s">
         <v>52</v>
@@ -17616,10 +17640,10 @@
     </row>
     <row r="187" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B187" s="9" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C187" s="9" t="s">
         <v>52</v>
@@ -17658,7 +17682,7 @@
       <c r="Y187" s="9"/>
       <c r="Z187" s="9"/>
       <c r="AA187" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AB187" s="17" t="n">
         <v>555</v>
@@ -17669,21 +17693,21 @@
       <c r="AF187" s="9"/>
       <c r="AG187" s="9"/>
       <c r="AH187" s="17" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="AI187" s="17" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="AJ187" s="17" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C188" s="9" t="s">
         <v>52</v>
@@ -17722,7 +17746,7 @@
       <c r="Y188" s="9"/>
       <c r="Z188" s="9"/>
       <c r="AA188" s="9" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AB188" s="17" t="n">
         <v>345</v>
@@ -17733,21 +17757,21 @@
       <c r="AF188" s="9"/>
       <c r="AG188" s="9"/>
       <c r="AH188" s="17" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AI188" s="17" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AJ188" s="17" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B189" s="9" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C189" s="9" t="s">
         <v>52</v>
@@ -17798,18 +17822,18 @@
         <v>12345</v>
       </c>
       <c r="AI189" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ189" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C190" s="9" t="s">
         <v>52</v>
@@ -17846,7 +17870,7 @@
       <c r="Y190" s="9"/>
       <c r="Z190" s="9"/>
       <c r="AA190" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AB190" s="17" t="n">
         <v>189</v>
@@ -17860,19 +17884,19 @@
         <v>12346</v>
       </c>
       <c r="AI190" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ190" s="9" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AK190" s="18"/>
     </row>
     <row r="191" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B191" s="9" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C191" s="9" t="s">
         <v>52</v>
@@ -17909,7 +17933,7 @@
       <c r="Y191" s="9"/>
       <c r="Z191" s="9"/>
       <c r="AA191" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AB191" s="17" t="n">
         <v>189</v>
@@ -17923,19 +17947,19 @@
         <v>12347</v>
       </c>
       <c r="AI191" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ191" s="9" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AK191" s="18"/>
     </row>
     <row r="192" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B192" s="9" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C192" s="9" t="s">
         <v>52</v>
@@ -17972,7 +17996,7 @@
       <c r="Y192" s="9"/>
       <c r="Z192" s="9"/>
       <c r="AA192" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AB192" s="17" t="n">
         <v>189</v>
@@ -17986,25 +18010,25 @@
         <v>12346</v>
       </c>
       <c r="AI192" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ192" s="9" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AK192" s="18"/>
       <c r="AM192" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AO192" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C193" s="9" t="s">
         <v>52</v>
@@ -18041,7 +18065,7 @@
       <c r="Y193" s="9"/>
       <c r="Z193" s="9"/>
       <c r="AA193" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AB193" s="17" t="n">
         <v>189</v>
@@ -18055,25 +18079,25 @@
         <v>12347</v>
       </c>
       <c r="AI193" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ193" s="9" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AK193" s="18"/>
       <c r="AM193" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AO193" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B194" s="9" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C194" s="9" t="s">
         <v>52</v>
@@ -18110,7 +18134,7 @@
       <c r="Y194" s="9"/>
       <c r="Z194" s="9"/>
       <c r="AA194" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AB194" s="17" t="n">
         <v>189</v>
@@ -18124,28 +18148,28 @@
         <v>12347</v>
       </c>
       <c r="AI194" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ194" s="9" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AK194" s="18"/>
       <c r="AM194" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AN194" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AO194" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B195" s="9" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C195" s="9" t="s">
         <v>52</v>
@@ -18182,7 +18206,7 @@
       <c r="Y195" s="9"/>
       <c r="Z195" s="9"/>
       <c r="AA195" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AB195" s="17" t="n">
         <v>189</v>
@@ -18196,28 +18220,28 @@
         <v>12347</v>
       </c>
       <c r="AI195" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ195" s="9" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AK195" s="18"/>
       <c r="AM195" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AN195" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AO195" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B196" s="9" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C196" s="9" t="s">
         <v>52</v>
@@ -18254,7 +18278,7 @@
       <c r="Y196" s="9"/>
       <c r="Z196" s="9"/>
       <c r="AA196" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AB196" s="17" t="n">
         <v>189</v>
@@ -18268,28 +18292,28 @@
         <v>12347</v>
       </c>
       <c r="AI196" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ196" s="9" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AK196" s="18"/>
       <c r="AM196" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AN196" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AO196" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B197" s="9" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C197" s="9" t="s">
         <v>52</v>
@@ -18326,7 +18350,7 @@
       <c r="Y197" s="9"/>
       <c r="Z197" s="9"/>
       <c r="AA197" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AB197" s="17" t="n">
         <v>189</v>
@@ -18340,28 +18364,28 @@
         <v>12347</v>
       </c>
       <c r="AI197" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ197" s="9" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AK197" s="18"/>
       <c r="AM197" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AN197" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AO197" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B198" s="9" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C198" s="9" t="s">
         <v>52</v>
@@ -18398,7 +18422,7 @@
       <c r="Y198" s="9"/>
       <c r="Z198" s="9"/>
       <c r="AA198" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AB198" s="17" t="n">
         <v>189</v>
@@ -18412,25 +18436,25 @@
         <v>12347</v>
       </c>
       <c r="AI198" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ198" s="9" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AK198" s="18"/>
       <c r="AM198" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AO198" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B199" s="9" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C199" s="9" t="s">
         <v>52</v>
@@ -18467,7 +18491,7 @@
       <c r="Y199" s="9"/>
       <c r="Z199" s="9"/>
       <c r="AA199" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AB199" s="17" t="n">
         <v>189</v>
@@ -18481,14 +18505,14 @@
         <v>12347</v>
       </c>
       <c r="AI199" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ199" s="9" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AK199" s="18"/>
       <c r="AM199" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18496,7 +18520,7 @@
         <v>261</v>
       </c>
       <c r="B200" s="9" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C200" s="9" t="s">
         <v>52</v>
@@ -18550,16 +18574,16 @@
         <v>195</v>
       </c>
       <c r="U200" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="V200" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="W200" s="9" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="X200" s="9" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="Y200" s="9" t="s">
         <v>235</v>
@@ -18574,44 +18598,44 @@
         <v>190</v>
       </c>
       <c r="AC200" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AD200" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="AE200" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="AF200" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="AG200" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AH200" s="17" t="n">
         <v>12345</v>
       </c>
       <c r="AI200" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ200" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AL200" s="9"/>
       <c r="AM200" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AN200" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AO200" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AP200" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AQ200" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="AR200" s="9"/>
       <c r="AS200" s="9"/>
@@ -18653,7 +18677,7 @@
         <v>261</v>
       </c>
       <c r="B201" s="9" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C201" s="9" t="s">
         <v>52</v>
@@ -18707,16 +18731,16 @@
         <v>195</v>
       </c>
       <c r="U201" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="V201" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="W201" s="9" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="X201" s="9" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="Y201" s="9" t="s">
         <v>235</v>
@@ -18731,44 +18755,44 @@
         <v>191</v>
       </c>
       <c r="AC201" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AD201" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="AE201" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="AF201" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AG201" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="AH201" s="17" t="n">
         <v>12345</v>
       </c>
       <c r="AI201" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ201" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AL201" s="9"/>
       <c r="AM201" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AN201" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AO201" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AP201" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AQ201" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="AR201" s="9"/>
       <c r="AS201" s="9"/>
@@ -18780,10 +18804,10 @@
     </row>
     <row r="202" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="9" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B202" s="9" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C202" s="9" t="s">
         <v>52</v>
@@ -18834,19 +18858,19 @@
         <v>189</v>
       </c>
       <c r="T202" s="9" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="U202" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="V202" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="W202" s="9" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="X202" s="9" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="Y202" s="9" t="s">
         <v>235</v>
@@ -18861,50 +18885,50 @@
         <v>75</v>
       </c>
       <c r="AC202" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AD202" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="AE202" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="AF202" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="AG202" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AH202" s="17" t="n">
         <v>12345</v>
       </c>
       <c r="AI202" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ202" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AL202" s="9"/>
       <c r="AM202" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AN202" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AO202" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AP202" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AQ202" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="AR202" s="9" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="AS202" s="9" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="AT202" s="9" t="n">
         <v>7898760</v>
@@ -18951,10 +18975,10 @@
     </row>
     <row r="203" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="9" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B203" s="9" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C203" s="9" t="s">
         <v>52</v>
@@ -19005,19 +19029,19 @@
         <v>189</v>
       </c>
       <c r="T203" s="9" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="U203" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="V203" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="W203" s="9" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="X203" s="9" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="Y203" s="9" t="s">
         <v>235</v>
@@ -19032,50 +19056,50 @@
         <v>76</v>
       </c>
       <c r="AC203" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AD203" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="AE203" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="AF203" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AG203" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="AH203" s="17" t="n">
         <v>12345</v>
       </c>
       <c r="AI203" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ203" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AL203" s="9"/>
       <c r="AM203" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AN203" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AO203" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AP203" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AQ203" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="AR203" s="9" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="AS203" s="9" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="AT203" s="9" t="n">
         <v>8976432</v>
@@ -19095,10 +19119,10 @@
     </row>
     <row r="204" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="9" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C204" s="9" t="s">
         <v>52</v>
@@ -19152,16 +19176,16 @@
         <v>195</v>
       </c>
       <c r="U204" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="V204" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="W204" s="9" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="X204" s="9" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="Y204" s="9" t="s">
         <v>235</v>
@@ -19176,44 +19200,44 @@
         <v>190</v>
       </c>
       <c r="AC204" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AD204" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="AE204" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="AF204" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="AG204" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AH204" s="17" t="n">
         <v>12345</v>
       </c>
       <c r="AI204" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ204" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AL204" s="9"/>
       <c r="AM204" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AN204" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AO204" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AP204" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AQ204" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="AR204" s="1" t="s">
         <v>70</v>
@@ -19221,10 +19245,10 @@
     </row>
     <row r="205" customFormat="false" ht="231" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="9" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C205" s="9" t="s">
         <v>52</v>
@@ -19278,16 +19302,16 @@
         <v>195</v>
       </c>
       <c r="U205" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="V205" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="W205" s="9" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="X205" s="9" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="Y205" s="9" t="s">
         <v>235</v>
@@ -19302,41 +19326,41 @@
         <v>190</v>
       </c>
       <c r="AC205" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AD205" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="AE205" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="AF205" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="AG205" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AH205" s="17" t="n">
         <v>12345</v>
       </c>
       <c r="AI205" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ205" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AL205" s="9"/>
       <c r="AM205" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AN205" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AO205" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AP205" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AQ205" s="1" t="s">
         <v>70</v>
@@ -19344,10 +19368,10 @@
     </row>
     <row r="206" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="9" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B206" s="9" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C206" s="9" t="s">
         <v>52</v>
@@ -19401,16 +19425,16 @@
         <v>195</v>
       </c>
       <c r="U206" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="V206" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="W206" s="9" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="X206" s="9" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="Y206" s="9" t="s">
         <v>235</v>
@@ -19425,41 +19449,41 @@
         <v>190</v>
       </c>
       <c r="AC206" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AD206" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="AE206" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="AF206" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="AG206" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AH206" s="17" t="n">
         <v>12345</v>
       </c>
       <c r="AI206" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ206" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AL206" s="9"/>
       <c r="AM206" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AN206" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AO206" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AP206" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AQ206" s="1" t="s">
         <v>73</v>
@@ -19470,10 +19494,10 @@
     </row>
     <row r="207" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="9" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B207" s="9" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C207" s="9" t="s">
         <v>52</v>
@@ -19527,16 +19551,16 @@
         <v>195</v>
       </c>
       <c r="U207" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="V207" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="W207" s="9" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="X207" s="9" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="Y207" s="9" t="s">
         <v>235</v>
@@ -19551,49 +19575,49 @@
         <v>190</v>
       </c>
       <c r="AC207" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AD207" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="AE207" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="AF207" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="AG207" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AH207" s="17" t="n">
         <v>12345</v>
       </c>
       <c r="AI207" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ207" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AL207" s="9"/>
       <c r="AM207" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AN207" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AO207" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AP207" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="9" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B208" s="9" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C208" s="9" t="s">
         <v>52</v>
@@ -19647,16 +19671,16 @@
         <v>195</v>
       </c>
       <c r="U208" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="V208" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="W208" s="9" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="X208" s="9" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="Y208" s="9" t="s">
         <v>235</v>
@@ -19671,44 +19695,44 @@
         <v>191</v>
       </c>
       <c r="AC208" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AD208" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="AE208" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="AF208" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AG208" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="AH208" s="17" t="n">
         <v>12345</v>
       </c>
       <c r="AI208" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ208" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AL208" s="9"/>
       <c r="AM208" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AN208" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AO208" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AP208" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AQ208" s="1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="AR208" s="1" t="s">
         <v>73</v>
@@ -19717,10 +19741,10 @@
     </row>
     <row r="209" customFormat="false" ht="231" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="9" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B209" s="9" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C209" s="9" t="s">
         <v>52</v>
@@ -19774,16 +19798,16 @@
         <v>195</v>
       </c>
       <c r="U209" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="V209" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="W209" s="9" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="X209" s="9" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="Y209" s="9" t="s">
         <v>235</v>
@@ -19798,41 +19822,41 @@
         <v>191</v>
       </c>
       <c r="AC209" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AD209" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="AE209" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="AF209" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AG209" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="AH209" s="17" t="n">
         <v>12345</v>
       </c>
       <c r="AI209" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ209" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AL209" s="9"/>
       <c r="AM209" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AN209" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AO209" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AP209" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AQ209" s="1" t="s">
         <v>70</v>
@@ -19844,10 +19868,10 @@
     </row>
     <row r="210" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="9" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B210" s="9" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C210" s="9" t="s">
         <v>52</v>
@@ -19901,16 +19925,16 @@
         <v>195</v>
       </c>
       <c r="U210" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="V210" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="W210" s="9" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="X210" s="9" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="Y210" s="9" t="s">
         <v>235</v>
@@ -19925,41 +19949,41 @@
         <v>191</v>
       </c>
       <c r="AC210" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AD210" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="AE210" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="AF210" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AG210" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="AH210" s="17" t="n">
         <v>12345</v>
       </c>
       <c r="AI210" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ210" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AL210" s="9"/>
       <c r="AM210" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AN210" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AO210" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AP210" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AQ210" s="1" t="s">
         <v>73</v>
@@ -19967,12 +19991,12 @@
       <c r="AR210" s="9"/>
       <c r="AS210" s="9"/>
     </row>
-    <row r="211" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="9" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B211" s="9" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C211" s="9" t="s">
         <v>52</v>
@@ -20026,16 +20050,16 @@
         <v>195</v>
       </c>
       <c r="U211" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="V211" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="W211" s="9" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="X211" s="9" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="Y211" s="9" t="s">
         <v>235</v>
@@ -20050,44 +20074,272 @@
         <v>191</v>
       </c>
       <c r="AC211" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AD211" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="AE211" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="AF211" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AG211" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="AH211" s="17" t="n">
         <v>12345</v>
       </c>
       <c r="AI211" s="19" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AJ211" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AL211" s="9"/>
       <c r="AM211" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AN211" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AO211" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AP211" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AR211" s="9"/>
       <c r="AS211" s="9"/>
+    </row>
+    <row r="212" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B212" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="C212" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E212" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F212" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G212" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H212" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I212" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="J212" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="K212" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="M212" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="N212" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="W212" s="9"/>
+      <c r="X212" s="9"/>
+      <c r="Y212" s="9"/>
+      <c r="Z212" s="9"/>
+      <c r="AA212" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="AB212" s="17" t="n">
+        <v>12</v>
+      </c>
+      <c r="AC212" s="9"/>
+      <c r="AD212" s="9"/>
+      <c r="AE212" s="9"/>
+      <c r="AF212" s="9"/>
+      <c r="AG212" s="9"/>
+      <c r="AH212" s="17"/>
+      <c r="AI212" s="9"/>
+      <c r="AJ212" s="9"/>
+    </row>
+    <row r="213" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B213" s="9" t="s">
+        <v>502</v>
+      </c>
+      <c r="C213" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E213" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F213" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G213" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="H213" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I213" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="J213" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="K213" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="M213" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="N213" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="W213" s="9"/>
+      <c r="X213" s="9"/>
+      <c r="Y213" s="9"/>
+      <c r="Z213" s="9"/>
+      <c r="AA213" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="AB213" s="17" t="n">
+        <v>12</v>
+      </c>
+      <c r="AC213" s="9"/>
+      <c r="AD213" s="9"/>
+      <c r="AE213" s="9"/>
+      <c r="AF213" s="9"/>
+      <c r="AG213" s="9"/>
+      <c r="AH213" s="17"/>
+      <c r="AI213" s="9"/>
+      <c r="AJ213" s="9"/>
+    </row>
+    <row r="214" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B214" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="C214" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E214" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F214" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G214" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H214" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I214" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="J214" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="K214" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="M214" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="N214" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="R214" s="9"/>
+      <c r="T214" s="9"/>
+      <c r="W214" s="9"/>
+      <c r="X214" s="9"/>
+      <c r="Y214" s="9"/>
+      <c r="Z214" s="9"/>
+      <c r="AA214" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="AB214" s="17" t="n">
+        <v>55</v>
+      </c>
+      <c r="AC214" s="9"/>
+      <c r="AD214" s="9"/>
+      <c r="AE214" s="9"/>
+      <c r="AF214" s="9"/>
+      <c r="AG214" s="9"/>
+      <c r="AH214" s="17"/>
+      <c r="AI214" s="9"/>
+      <c r="AJ214" s="9"/>
+    </row>
+    <row r="215" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B215" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="C215" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E215" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F215" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G215" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="H215" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I215" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="J215" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="K215" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="M215" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="N215" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="R215" s="9"/>
+      <c r="T215" s="9"/>
+      <c r="W215" s="9"/>
+      <c r="X215" s="9"/>
+      <c r="Y215" s="9"/>
+      <c r="Z215" s="9"/>
+      <c r="AA215" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="AB215" s="17" t="n">
+        <v>34</v>
+      </c>
+      <c r="AC215" s="9"/>
+      <c r="AD215" s="9"/>
+      <c r="AE215" s="9"/>
+      <c r="AF215" s="9"/>
+      <c r="AG215" s="9"/>
+      <c r="AH215" s="17"/>
+      <c r="AI215" s="9"/>
+      <c r="AJ215" s="9"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -20188,6 +20440,10 @@
     <hyperlink ref="I209" r:id="rId94" display="parkjimin@gmail.com"/>
     <hyperlink ref="I210" r:id="rId95" display="parkjimin@gmail.com"/>
     <hyperlink ref="I211" r:id="rId96" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I212" r:id="rId97" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I213" r:id="rId98" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I214" r:id="rId99" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I215" r:id="rId100" display="parkjimin@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -20216,22 +20472,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="5.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="11" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="11" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="26.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="11" width="9.17"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="11" width="12.57" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="11" width="5.18" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="4" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="11" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="11" width="20.5" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="11" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="11" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="11" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="13" customWidth="true" hidden="false" style="11" width="14.87" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="11" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="11" width="26.35" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="17" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="11" width="29.45" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="1025" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20242,90 +20498,97 @@
         <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>505</v>
+        <v>512</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>506</v>
+        <v>513</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="R1" s="22" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>516</v>
+        <v>523</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>518</v>
-      </c>
+        <v>525</v>
+      </c>
+      <c r="E2"/>
+      <c r="F2"/>
       <c r="G2" s="24" t="s">
-        <v>519</v>
-      </c>
+        <v>526</v>
+      </c>
+      <c r="H2"/>
       <c r="I2" s="24" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>521</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
       <c r="N2" s="26" t="s">
-        <v>522</v>
+        <v>529</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>523</v>
-      </c>
+        <v>530</v>
+      </c>
+      <c r="P2"/>
       <c r="Q2" s="25" t="n">
         <v>500</v>
       </c>
       <c r="R2" s="27" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
       <c r="S2" s="25" t="n">
         <v>0</v>
@@ -20333,39 +20596,46 @@
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
+        <v>532</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>524</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>525</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>517</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>518</v>
-      </c>
+      <c r="E3"/>
+      <c r="F3"/>
       <c r="G3" s="23" t="s">
-        <v>519</v>
-      </c>
+        <v>526</v>
+      </c>
+      <c r="H3"/>
       <c r="I3" s="28" t="s">
-        <v>526</v>
+        <v>533</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>521</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
       <c r="N3" s="26" t="s">
-        <v>522</v>
+        <v>529</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>523</v>
-      </c>
+        <v>530</v>
+      </c>
+      <c r="P3"/>
       <c r="Q3" s="25" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="28" t="s">
-        <v>524</v>
-      </c>
-      <c r="S3" s="29" t="n">
+        <v>531</v>
+      </c>
+      <c r="S3" s="29" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20373,326 +20643,358 @@
     </row>
     <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>527</v>
+        <v>534</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>529</v>
+        <v>536</v>
       </c>
       <c r="E4" s="31" t="s">
+        <v>537</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>538</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>539</v>
+      </c>
+      <c r="I4" s="32" t="s">
+        <v>540</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="L4" s="33" t="s">
+        <v>543</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>544</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>545</v>
+      </c>
+      <c r="O4" s="12" t="s">
         <v>530</v>
       </c>
-      <c r="F4" s="31" t="s">
-        <v>531</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>532</v>
-      </c>
-      <c r="I4" s="32" t="s">
-        <v>533</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>534</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>535</v>
-      </c>
-      <c r="L4" s="33" t="s">
-        <v>536</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>537</v>
-      </c>
-      <c r="N4" s="26" t="s">
-        <v>538</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>523</v>
-      </c>
+      <c r="P4"/>
       <c r="Q4" s="25" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>539</v>
-      </c>
-      <c r="S4" s="34" t="n">
+        <v>546</v>
+      </c>
+      <c r="S4" s="34" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>540</v>
+        <v>547</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>529</v>
+        <v>536</v>
       </c>
       <c r="E5" s="31" t="s">
+        <v>537</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>538</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>539</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>548</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>549</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>544</v>
+      </c>
+      <c r="N5" s="26" t="s">
+        <v>545</v>
+      </c>
+      <c r="O5" s="12" t="s">
         <v>530</v>
       </c>
-      <c r="F5" s="31" t="s">
-        <v>531</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>532</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>541</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>534</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>535</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>542</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>537</v>
-      </c>
-      <c r="N5" s="26" t="s">
-        <v>538</v>
-      </c>
-      <c r="O5" s="12" t="s">
-        <v>523</v>
-      </c>
+      <c r="P5"/>
       <c r="Q5" s="25" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>539</v>
-      </c>
-      <c r="S5" s="34" t="n">
+        <v>546</v>
+      </c>
+      <c r="S5" s="34" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>543</v>
+        <v>550</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>529</v>
+        <v>536</v>
       </c>
       <c r="E6" s="31" t="s">
+        <v>537</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>538</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>539</v>
+      </c>
+      <c r="I6" s="32" t="s">
+        <v>540</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="K6"/>
+      <c r="L6" s="12" t="s">
+        <v>551</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>544</v>
+      </c>
+      <c r="N6" s="26" t="s">
+        <v>545</v>
+      </c>
+      <c r="O6" s="12" t="s">
         <v>530</v>
       </c>
-      <c r="F6" s="31" t="s">
-        <v>531</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>532</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>533</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>534</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>544</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>537</v>
-      </c>
-      <c r="N6" s="26" t="s">
-        <v>538</v>
-      </c>
-      <c r="O6" s="12" t="s">
-        <v>523</v>
-      </c>
+      <c r="P6"/>
       <c r="Q6" s="25" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>539</v>
-      </c>
-      <c r="S6" s="34" t="n">
+        <v>546</v>
+      </c>
+      <c r="S6" s="34" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>545</v>
+        <v>552</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
       <c r="D7" s="9" t="s">
+        <v>536</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>537</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>538</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>539</v>
+      </c>
+      <c r="I7" s="32" t="s">
+        <v>540</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7" s="12" t="s">
+        <v>544</v>
+      </c>
+      <c r="N7" s="26" t="s">
         <v>529</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="O7" s="12" t="s">
         <v>530</v>
       </c>
-      <c r="F7" s="31" t="s">
-        <v>531</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>532</v>
-      </c>
-      <c r="I7" s="32" t="s">
-        <v>533</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>534</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>537</v>
-      </c>
-      <c r="N7" s="26" t="s">
-        <v>522</v>
-      </c>
-      <c r="O7" s="12" t="s">
-        <v>523</v>
-      </c>
+      <c r="P7"/>
       <c r="Q7" s="25" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>539</v>
-      </c>
-      <c r="S7" s="34" t="n">
+        <v>546</v>
+      </c>
+      <c r="S7" s="34" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>546</v>
+        <v>553</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>547</v>
+        <v>554</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>530</v>
+        <v>537</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>531</v>
+        <v>538</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="H8" s="35" t="s">
-        <v>548</v>
+        <v>555</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>549</v>
+        <v>556</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>550</v>
+        <v>557</v>
       </c>
       <c r="K8" s="32" t="s">
-        <v>551</v>
+        <v>558</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>552</v>
-      </c>
+        <v>603</v>
+      </c>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
       <c r="Q8" s="25" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>553</v>
-      </c>
-      <c r="S8" s="34" t="n">
+        <v>560</v>
+      </c>
+      <c r="S8" s="34" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
+        <v>561</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>554</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>528</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>547</v>
-      </c>
       <c r="E9" s="31" t="s">
-        <v>530</v>
+        <v>537</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>531</v>
+        <v>538</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="H9" s="35" t="s">
-        <v>555</v>
+        <v>562</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>556</v>
+        <v>563</v>
       </c>
       <c r="J9" s="32" t="s">
-        <v>550</v>
+        <v>557</v>
       </c>
       <c r="K9" s="36" t="s">
-        <v>551</v>
-      </c>
+        <v>558</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
       <c r="Q9" s="25" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>553</v>
-      </c>
-      <c r="S9" s="34" t="n">
+        <v>560</v>
+      </c>
+      <c r="S9" s="34" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
       <c r="H10" s="35" t="s">
+        <v>564</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>565</v>
+      </c>
+      <c r="J10" s="32" t="s">
         <v>557</v>
       </c>
-      <c r="I10" s="9" t="s">
-        <v>558</v>
-      </c>
-      <c r="J10" s="32" t="s">
-        <v>550</v>
-      </c>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -20737,220 +21039,220 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>559</v>
+        <v>566</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="37" t="s">
-        <v>533</v>
+        <v>540</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="37" t="s">
-        <v>560</v>
+        <v>567</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="37" t="s">
-        <v>533</v>
+        <v>540</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="37" t="s">
-        <v>561</v>
+        <v>568</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="37" t="s">
-        <v>562</v>
+        <v>569</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>563</v>
+        <v>570</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="37" t="s">
-        <v>561</v>
+        <v>568</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="37" t="s">
-        <v>564</v>
+        <v>571</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>565</v>
+        <v>572</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>566</v>
+        <v>573</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>567</v>
+        <v>574</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>541</v>
+        <v>548</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>568</v>
+        <v>575</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>569</v>
+        <v>576</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>570</v>
+        <v>577</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>571</v>
+        <v>578</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>572</v>
+        <v>579</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="38" t="s">
-        <v>573</v>
+        <v>580</v>
       </c>
       <c r="F25" s="38" t="s">
-        <v>574</v>
+        <v>581</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>575</v>
+        <v>582</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>576</v>
+        <v>583</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>577</v>
+        <v>584</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>578</v>
+        <v>585</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="39" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>580</v>
+        <v>587</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="38" t="s">
-        <v>581</v>
+        <v>588</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>583</v>
+        <v>590</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>584</v>
+        <v>591</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>585</v>
+        <v>592</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>584</v>
+        <v>591</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>586</v>
+        <v>593</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>584</v>
+        <v>591</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>587</v>
+        <v>594</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>588</v>
+        <v>595</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>558</v>
+        <v>565</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>584</v>
+        <v>591</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>589</v>
+        <v>596</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="38" t="s">
-        <v>590</v>
+        <v>597</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>591</v>
+        <v>598</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="40" t="s">
-        <v>592</v>
+        <v>599</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>593</v>
+        <v>600</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="41" t="s">
-        <v>594</v>
+        <v>601</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20958,7 +21260,7 @@
         <v>197198</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>595</v>
+        <v>602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ios business logic pageobjects updae
</commit_message>
<xml_diff>
--- a/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/test-classes/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3114" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3131" uniqueCount="605">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1540,6 +1540,12 @@
   </si>
   <si>
     <t xml:space="preserve">TestCase_212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_214</t>
   </si>
   <si>
     <t xml:space="preserve">mode</t>
@@ -1950,9 +1956,6 @@
   </si>
   <si>
     <t xml:space="preserve">e2e testdata</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
 </sst>
 </file>
@@ -2409,62 +2412,62 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A156" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A163" activeCellId="0" sqref="A163"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A210" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B218" activeCellId="0" sqref="B218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="14.33" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
-    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
-    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
-    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
-    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
-    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
-    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
-    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
-    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
-    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
-    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
-    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
-    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
-    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
-    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
-    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="991" max="1025" customWidth="true" hidden="false" style="4" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="4" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20340,6 +20343,148 @@
       <c r="AH215" s="17"/>
       <c r="AI215" s="9"/>
       <c r="AJ215" s="9"/>
+    </row>
+    <row r="216" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B216" s="9" t="s">
+        <v>506</v>
+      </c>
+      <c r="C216" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E216" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F216" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G216" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="H216" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="I216" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="J216" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="K216" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="M216" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="N216" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="O216" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="P216" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q216" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="R216" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="S216" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="T216" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="U216" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="V216" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="Z216" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="AA216" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="AB216" s="17" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B217" s="9" t="s">
+        <v>507</v>
+      </c>
+      <c r="C217" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E217" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F217" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G217" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="H217" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="I217" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="J217" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="K217" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="M217" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="N217" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="O217" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="P217" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q217" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="R217" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="S217" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="T217" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="U217" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="V217" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="Z217" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="AA217" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="AB217" s="17" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -20444,6 +20589,8 @@
     <hyperlink ref="I213" r:id="rId98" display="parkjimin@gmail.com"/>
     <hyperlink ref="I214" r:id="rId99" display="parkjimin@gmail.com"/>
     <hyperlink ref="I215" r:id="rId100" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I216" r:id="rId101" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I217" r:id="rId102" display="parkjimin@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -20472,22 +20619,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="11" width="12.57" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="11" width="5.18" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="4" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="11" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="11" width="20.5" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="11" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="11" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="11" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="13" customWidth="true" hidden="false" style="11" width="14.87" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="11" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="11" width="26.35" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="17" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="11" width="29.45" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="1025" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="11" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="11" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="26.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="11" width="9.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20498,97 +20645,90 @@
         <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="R1" s="22" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>525</v>
-      </c>
-      <c r="E2"/>
-      <c r="F2"/>
+        <v>527</v>
+      </c>
       <c r="G2" s="24" t="s">
-        <v>526</v>
-      </c>
-      <c r="H2"/>
+        <v>528</v>
+      </c>
       <c r="I2" s="24" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>528</v>
-      </c>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
+        <v>530</v>
+      </c>
       <c r="N2" s="26" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>530</v>
-      </c>
-      <c r="P2"/>
+        <v>532</v>
+      </c>
       <c r="Q2" s="25" t="n">
         <v>500</v>
       </c>
       <c r="R2" s="27" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="S2" s="25" t="n">
         <v>0</v>
@@ -20596,46 +20736,39 @@
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
+        <v>534</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>526</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>527</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>528</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>535</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>530</v>
+      </c>
+      <c r="N3" s="26" t="s">
+        <v>531</v>
+      </c>
+      <c r="O3" s="12" t="s">
         <v>532</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>524</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>525</v>
-      </c>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3" s="23" t="s">
-        <v>526</v>
-      </c>
-      <c r="H3"/>
-      <c r="I3" s="28" t="s">
-        <v>533</v>
-      </c>
-      <c r="J3" s="28" t="s">
-        <v>528</v>
-      </c>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3" s="26" t="s">
-        <v>529</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>530</v>
-      </c>
-      <c r="P3"/>
       <c r="Q3" s="25" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="28" t="s">
-        <v>531</v>
-      </c>
-      <c r="S3" s="29" t="b">
+        <v>533</v>
+      </c>
+      <c r="S3" s="29" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20643,358 +20776,326 @@
     </row>
     <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="F4" s="31" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="I4" s="32" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="L4" s="33" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="N4" s="26" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>530</v>
-      </c>
-      <c r="P4"/>
+        <v>532</v>
+      </c>
       <c r="Q4" s="25" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>546</v>
-      </c>
-      <c r="S4" s="34" t="b">
+        <v>548</v>
+      </c>
+      <c r="S4" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
+        <v>549</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>538</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>539</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>540</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>543</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>544</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>551</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>546</v>
+      </c>
+      <c r="N5" s="26" t="s">
         <v>547</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>536</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>537</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>538</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>539</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>548</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>541</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>542</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>549</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>544</v>
-      </c>
-      <c r="N5" s="26" t="s">
-        <v>545</v>
-      </c>
       <c r="O5" s="12" t="s">
-        <v>530</v>
-      </c>
-      <c r="P5"/>
+        <v>532</v>
+      </c>
       <c r="Q5" s="25" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>546</v>
-      </c>
-      <c r="S5" s="34" t="b">
+        <v>548</v>
+      </c>
+      <c r="S5" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="F6" s="31" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="I6" s="32" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>541</v>
-      </c>
-      <c r="K6"/>
+        <v>543</v>
+      </c>
       <c r="L6" s="12" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="N6" s="26" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>530</v>
-      </c>
-      <c r="P6"/>
+        <v>532</v>
+      </c>
       <c r="Q6" s="25" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>546</v>
-      </c>
-      <c r="S6" s="34" t="b">
+        <v>548</v>
+      </c>
+      <c r="S6" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="F7" s="31" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="I7" s="32" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>541</v>
-      </c>
-      <c r="K7"/>
-      <c r="L7"/>
+        <v>543</v>
+      </c>
       <c r="M7" s="12" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="N7" s="26" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>530</v>
-      </c>
-      <c r="P7"/>
+        <v>532</v>
+      </c>
       <c r="Q7" s="25" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>546</v>
-      </c>
-      <c r="S7" s="34" t="b">
+        <v>548</v>
+      </c>
+      <c r="S7" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H8" s="35" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="K8" s="32" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>603</v>
-      </c>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
+        <v>561</v>
+      </c>
       <c r="Q8" s="25" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>560</v>
-      </c>
-      <c r="S8" s="34" t="b">
+        <v>562</v>
+      </c>
+      <c r="S8" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>52</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H9" s="35" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="J9" s="32" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="K9" s="36" t="s">
-        <v>558</v>
-      </c>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
+        <v>560</v>
+      </c>
       <c r="Q9" s="25" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>560</v>
-      </c>
-      <c r="S9" s="34" t="b">
+        <v>562</v>
+      </c>
+      <c r="S9" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
       <c r="H10" s="35" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="J10" s="32" t="s">
-        <v>557</v>
-      </c>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="N10"/>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
+        <v>559</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -21039,220 +21140,220 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="37" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="37" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="37" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="37" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="37" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="37" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="37" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="38" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="F25" s="38" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="39" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="38" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
+        <v>595</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>591</v>
+      </c>
+      <c r="F35" s="0" t="s">
         <v>593</v>
       </c>
-      <c r="E35" s="0" t="s">
-        <v>589</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>591</v>
-      </c>
       <c r="G35" s="0" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="38" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="40" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="41" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21260,7 +21361,7 @@
         <v>197198</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
     </row>
   </sheetData>

</xml_diff>